<commit_message>
added new tweak for cashier log
address
varchar
and cashier log
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.beta.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$253</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$265</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="262">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -68,9 +68,6 @@
     <t>customer_full_name</t>
   </si>
   <si>
-    <t>customer_address</t>
-  </si>
-  <si>
     <t>customer_phone</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>supplier_full_name</t>
   </si>
   <si>
-    <t>supplier_address</t>
-  </si>
-  <si>
     <t>supplier_phone</t>
   </si>
   <si>
@@ -305,9 +299,6 @@
     <t>branch_name</t>
   </si>
   <si>
-    <t>branch_address</t>
-  </si>
-  <si>
     <t>branch_telephone</t>
   </si>
   <si>
@@ -533,9 +524,6 @@
     <t>change_name</t>
   </si>
   <si>
-    <t>login,logout,insert,update,delete,view,active,open cashier, close cashier</t>
-  </si>
-  <si>
     <t>change_shift</t>
   </si>
   <si>
@@ -761,13 +749,61 @@
     <t>rs_customer_id</t>
   </si>
   <si>
-    <t>1=debet,2=credit</t>
-  </si>
-  <si>
     <t>debt_purchase_id</t>
   </si>
   <si>
     <t>credit_sales_id</t>
+  </si>
+  <si>
+    <t>login,logout,insert,update,delete,view,active, close cashier</t>
+  </si>
+  <si>
+    <t>CASHIER LOG</t>
+  </si>
+  <si>
+    <t>1=debet,-1=credit</t>
+  </si>
+  <si>
+    <t>tinyint_signed</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>account_type*amount</t>
+  </si>
+  <si>
+    <t>penjumlahan semua transasksi</t>
+  </si>
+  <si>
+    <t>branch_address_city</t>
+  </si>
+  <si>
+    <t>branch_address2</t>
+  </si>
+  <si>
+    <t>branch_address1</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>customer_address1</t>
+  </si>
+  <si>
+    <t>customer_address2</t>
+  </si>
+  <si>
+    <t>customer_address_city</t>
+  </si>
+  <si>
+    <t>supplier_address1</t>
+  </si>
+  <si>
+    <t>supplier_address2</t>
+  </si>
+  <si>
+    <t>supplier_address_city</t>
   </si>
 </sst>
 </file>
@@ -1147,10 +1183,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q255"/>
+  <dimension ref="B1:Q267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215:XFD217"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1200,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1191,13 +1227,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1208,7 +1244,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>255</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1216,11 +1252,11 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1228,34 +1264,34 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1268,7 +1304,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1279,16 +1315,16 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1296,13 +1332,13 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>255</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1310,11 +1346,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>254</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>67</v>
+        <v>255</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1322,11 +1358,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>96</v>
+        <v>253</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1334,13 +1370,11 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1348,89 +1382,89 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>225</v>
+        <v>93</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>223</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>220</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D20" s="1" t="s">
-        <v>219</v>
+        <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>218</v>
+        <v>54</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>209</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>216</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1438,11 +1472,13 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="F22" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1450,761 +1486,767 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" t="s">
-        <v>68</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="P23" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G25" s="1"/>
+      <c r="H25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="P25" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="N26" t="s">
-        <v>45</v>
-      </c>
-      <c r="P26">
-        <v>1</v>
-      </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="N27" t="s">
-        <v>46</v>
-      </c>
-      <c r="P27">
-        <v>2</v>
-      </c>
-      <c r="Q27">
-        <v>3</v>
-      </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F28" s="1" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="G28" s="1"/>
       <c r="N28" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P28">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" t="s">
-        <v>68</v>
+      <c r="N29" t="s">
+        <v>44</v>
+      </c>
+      <c r="P29">
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G30" s="1"/>
+      <c r="N30" t="s">
+        <v>45</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="N31" t="s">
-        <v>48</v>
+      <c r="H31" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="N33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>5</v>
+        <v>58</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>236</v>
-      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="D37" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E38" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F38" s="1" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F39" s="1" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>173</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E41" s="2"/>
       <c r="F41" s="1" t="s">
-        <v>213</v>
+        <v>65</v>
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="E42" s="2"/>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>12</v>
-      </c>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
-      <c r="C47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>236</v>
-      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="D48" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F48" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F49" s="1" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="1"/>
+        <v>171</v>
+      </c>
+      <c r="E50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F51" s="1" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="1"/>
+        <v>249</v>
+      </c>
+      <c r="E52" s="2"/>
       <c r="F52" s="1" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>250</v>
+      </c>
+      <c r="K52" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C54" s="1"/>
-      <c r="D54" s="1" t="s">
-        <v>176</v>
-      </c>
+      <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D55" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E55" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F55" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>178</v>
+        <v>15</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H56" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
+      <c r="D57" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
+      <c r="F57" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
-      <c r="C58" s="1" t="s">
-        <v>174</v>
-      </c>
+      <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>231</v>
+        <v>16</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>232</v>
+        <v>17</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>233</v>
+        <v>18</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>235</v>
+        <v>172</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="F65" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="1" t="s">
-        <v>20</v>
-      </c>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F66" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H66" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
-      <c r="C67" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="C68" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="D68" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E68" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F68" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E69" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F69" s="1" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>25</v>
+        <v>227</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>26</v>
+        <v>228</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>66</v>
+        <v>235</v>
       </c>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>74</v>
+        <v>230</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+      <c r="D74" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="F74" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
-        <v>62</v>
-      </c>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="1"/>
-      <c r="C76" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E76" s="1" t="s">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F76" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>179</v>
+        <v>259</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>66</v>
+        <v>255</v>
       </c>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>180</v>
+        <v>260</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>67</v>
+        <v>255</v>
       </c>
       <c r="G80" s="1"/>
     </row>
@@ -2212,117 +2254,109 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>181</v>
+        <v>261</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="G81" s="1"/>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>182</v>
+        <v>23</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>215</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="G82" s="1"/>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>183</v>
+        <v>24</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>217</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="G83" s="1"/>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>184</v>
+        <v>25</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>216</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="G84" s="1"/>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>185</v>
+        <v>72</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1" t="s">
-        <v>66</v>
+        <v>209</v>
       </c>
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
-      <c r="D86" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
+      <c r="B87" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C87" s="1"/>
-      <c r="D87" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E87" s="5"/>
-      <c r="F87" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
+      <c r="C88" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D88" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E88" s="5"/>
-      <c r="F88" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G88" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E89" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F89" s="1" t="s">
-        <v>66</v>
+        <v>255</v>
       </c>
       <c r="G89" s="1"/>
     </row>
@@ -2330,13 +2364,13 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>28</v>
+        <v>210</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="G90" s="1"/>
     </row>
@@ -2344,13 +2378,11 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="G91" s="1"/>
     </row>
@@ -2358,13 +2390,11 @@
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>197</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>237</v>
+        <v>65</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -2372,470 +2402,484 @@
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G93" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G94" s="1"/>
+        <v>234</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>203</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
+      <c r="D98" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
-      <c r="C99" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="E99" s="5"/>
       <c r="F99" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E100" s="5"/>
       <c r="F100" s="1" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E101" s="1"/>
+        <v>185</v>
+      </c>
+      <c r="E101" s="5"/>
       <c r="F101" s="1" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E102" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F102" s="1" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E103" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F103" s="1" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="G103" s="1"/>
-      <c r="H103" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
+      <c r="D104" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
-      <c r="C105" s="1" t="s">
-        <v>198</v>
-      </c>
+      <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>242</v>
+        <v>188</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>175</v>
+        <v>237</v>
       </c>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G107" s="1"/>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>231</v>
+        <v>191</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>5</v>
+        <v>198</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G109" s="1"/>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
-      <c r="D110" s="1" t="s">
-        <v>243</v>
-      </c>
+      <c r="D110" s="1"/>
       <c r="E110" s="1"/>
-      <c r="F110" s="1" t="s">
-        <v>237</v>
-      </c>
+      <c r="F110" s="1"/>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
+      <c r="C111" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="D111" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E111" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F111" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
+      <c r="D112" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
-      <c r="C113" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E113" s="1"/>
       <c r="F113" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1" t="s">
-        <v>66</v>
+        <v>195</v>
       </c>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="G115" s="1"/>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H115" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
-      <c r="D116" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="D116" s="1"/>
       <c r="E116" s="1"/>
-      <c r="F116" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="F116" s="1"/>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
-      <c r="F117" s="1"/>
+      <c r="C117" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
-      <c r="C118" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>36</v>
+        <v>238</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>236</v>
+        <v>171</v>
       </c>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E119" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F119" s="1" t="s">
         <v>236</v>
       </c>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>35</v>
+        <v>227</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
+      <c r="D121" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
-      <c r="C122" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1" t="s">
-        <v>39</v>
+        <v>197</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>66</v>
+        <v>233</v>
       </c>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
-      <c r="D124" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="D124" s="1"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="F124" s="1"/>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
+      <c r="C125" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D125" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E125" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F125" s="1" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
-      <c r="D126" s="1"/>
+      <c r="D126" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
+      <c r="F126" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
-      <c r="C127" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="C127" s="1"/>
       <c r="D127" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>240</v>
+        <v>65</v>
       </c>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>66</v>
+        <v>209</v>
       </c>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
-      <c r="D129" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>236</v>
-      </c>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
+      <c r="C130" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D130" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="G130" s="1"/>
     </row>
@@ -2843,11 +2887,11 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G131" s="1"/>
     </row>
@@ -2855,59 +2899,59 @@
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>204</v>
+        <v>33</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="G132" s="1"/>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
-      <c r="D133" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="F133" s="1"/>
       <c r="G133" s="1"/>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
-      <c r="C134" s="1"/>
+      <c r="C134" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D134" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E134" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F134" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G134" s="1"/>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
-      <c r="D135" s="1"/>
+      <c r="D135" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E135" s="1"/>
-      <c r="F135" s="1"/>
+      <c r="F135" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="G135" s="1"/>
     </row>
     <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
-      <c r="C136" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>240</v>
+        <v>65</v>
       </c>
       <c r="G136" s="1"/>
     </row>
@@ -2915,37 +2959,35 @@
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
-      <c r="D138" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="D138" s="1"/>
       <c r="E138" s="1"/>
-      <c r="F138" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="F138" s="1"/>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
-      <c r="C139" s="1"/>
+      <c r="C139" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D139" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E139" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F139" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G139" s="1"/>
     </row>
@@ -2953,35 +2995,37 @@
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
-        <v>238</v>
+        <v>64</v>
       </c>
       <c r="G140" s="1"/>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
-      <c r="F141" s="1"/>
+      <c r="D141" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="G141" s="1"/>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="1"/>
-      <c r="C142" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E142" s="1"/>
       <c r="F142" s="1" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="G142" s="1"/>
     </row>
@@ -2989,13 +3033,11 @@
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="G143" s="1"/>
     </row>
@@ -3003,11 +3045,11 @@
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>244</v>
+        <v>200</v>
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G144" s="1"/>
     </row>
@@ -3015,11 +3057,11 @@
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
       <c r="G145" s="1"/>
     </row>
@@ -3027,35 +3069,35 @@
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
-      <c r="D147" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="D147" s="1"/>
       <c r="E147" s="1"/>
-      <c r="F147" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="F147" s="1"/>
       <c r="G147" s="1"/>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
-      <c r="C148" s="1"/>
+      <c r="C148" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D148" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E148" s="1"/>
+        <v>105</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F148" s="1" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
       <c r="G148" s="1"/>
     </row>
@@ -3063,35 +3105,37 @@
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E149" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F149" s="1" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="G149" s="1"/>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
+      <c r="D150" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
+      <c r="F150" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="G150" s="1"/>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" s="1"/>
-      <c r="C151" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="C151" s="1"/>
       <c r="D151" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E151" s="1"/>
       <c r="F151" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G151" s="1"/>
     </row>
@@ -3099,37 +3143,35 @@
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E152" s="1"/>
       <c r="F152" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
-      <c r="D153" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="D153" s="1"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="F153" s="1"/>
       <c r="G153" s="1"/>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
+      <c r="C154" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D154" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E154" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F154" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G154" s="1"/>
     </row>
@@ -3137,11 +3179,13 @@
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E155" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F155" s="1" t="s">
-        <v>237</v>
+        <v>64</v>
       </c>
       <c r="G155" s="1"/>
     </row>
@@ -3149,35 +3193,35 @@
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
-        <v>122</v>
+        <v>240</v>
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="G156" s="1"/>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
+      <c r="D157" s="1" t="s">
+        <v>241</v>
+      </c>
       <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
+      <c r="F157" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G157" s="1"/>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
-      <c r="C158" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
-        <v>240</v>
+        <v>171</v>
       </c>
       <c r="G158" s="1"/>
     </row>
@@ -3185,13 +3229,11 @@
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="G159" s="1"/>
     </row>
@@ -3199,13 +3241,11 @@
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E160" s="1"/>
       <c r="F160" s="1" t="s">
-        <v>236</v>
+        <v>171</v>
       </c>
       <c r="G160" s="1"/>
     </row>
@@ -3213,59 +3253,61 @@
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E161" s="1"/>
       <c r="F161" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="G161" s="1"/>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
-      <c r="D162" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="D162" s="1"/>
       <c r="E162" s="1"/>
-      <c r="F162" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="F162" s="1"/>
       <c r="G162" s="1"/>
     </row>
     <row r="163" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B163" s="1"/>
-      <c r="C163" s="1"/>
+      <c r="C163" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D163" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E163" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F163" s="1" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
-      <c r="D164" s="1"/>
-      <c r="E164" s="1"/>
-      <c r="F164" s="1"/>
+      <c r="D164" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="G164" s="1"/>
     </row>
     <row r="165" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B165" s="1"/>
-      <c r="C165" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E165" s="1"/>
       <c r="F165" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G165" s="1"/>
     </row>
@@ -3273,13 +3315,11 @@
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E166" s="1"/>
       <c r="F166" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G166" s="1"/>
     </row>
@@ -3287,11 +3327,11 @@
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G167" s="1"/>
     </row>
@@ -3299,59 +3339,63 @@
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E168" s="1"/>
       <c r="F168" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G168" s="1"/>
     </row>
     <row r="169" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
-      <c r="D169" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="D169" s="1"/>
       <c r="E169" s="1"/>
-      <c r="F169" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="F169" s="1"/>
       <c r="G169" s="1"/>
     </row>
     <row r="170" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B170" s="1"/>
-      <c r="C170" s="1"/>
+      <c r="C170" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="D170" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E170" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F170" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G170" s="1"/>
     </row>
     <row r="171" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
-      <c r="D171" s="1"/>
-      <c r="E171" s="1"/>
-      <c r="F171" s="1"/>
+      <c r="D171" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="G171" s="1"/>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B172" s="1"/>
-      <c r="C172" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="C172" s="1"/>
       <c r="D172" s="1" t="s">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G172" s="1"/>
     </row>
@@ -3359,13 +3403,11 @@
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E173" s="1"/>
       <c r="F173" s="1" t="s">
-        <v>66</v>
+        <v>171</v>
       </c>
       <c r="G173" s="1"/>
     </row>
@@ -3373,13 +3415,11 @@
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E174" s="1"/>
       <c r="F174" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G174" s="1"/>
     </row>
@@ -3387,35 +3427,35 @@
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="G175" s="1"/>
     </row>
     <row r="176" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
-      <c r="D176" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="D176" s="1"/>
       <c r="E176" s="1"/>
-      <c r="F176" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="F176" s="1"/>
       <c r="G176" s="1"/>
     </row>
     <row r="177" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B177" s="1"/>
-      <c r="C177" s="1"/>
+      <c r="C177" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="D177" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E177" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F177" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G177" s="1"/>
     </row>
@@ -3423,11 +3463,13 @@
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E178" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F178" s="1" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="G178" s="1"/>
     </row>
@@ -3435,11 +3477,11 @@
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="E179" s="1"/>
       <c r="F179" s="1" t="s">
-        <v>175</v>
+        <v>234</v>
       </c>
       <c r="G179" s="1"/>
     </row>
@@ -3447,61 +3489,59 @@
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="E180" s="1"/>
       <c r="F180" s="1" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="G180" s="1"/>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
-      <c r="D181" s="1"/>
+      <c r="D181" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="E181" s="1"/>
-      <c r="F181" s="1"/>
+      <c r="F181" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G181" s="1"/>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B182" s="1"/>
-      <c r="C182" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="C182" s="1"/>
       <c r="D182" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="E182" s="1"/>
       <c r="F182" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G182" s="1"/>
     </row>
     <row r="183" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
-      <c r="D183" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>240</v>
-      </c>
+      <c r="D183" s="1"/>
+      <c r="E183" s="1"/>
+      <c r="F183" s="1"/>
       <c r="G183" s="1"/>
     </row>
     <row r="184" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B184" s="1"/>
-      <c r="C184" s="1"/>
+      <c r="C184" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="D184" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E184" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F184" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G184" s="1"/>
     </row>
@@ -3509,11 +3549,13 @@
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E185" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F185" s="1" t="s">
-        <v>237</v>
+        <v>64</v>
       </c>
       <c r="G185" s="1"/>
     </row>
@@ -3521,11 +3563,13 @@
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E186" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F186" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G186" s="1"/>
     </row>
@@ -3533,11 +3577,11 @@
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1" t="s">
-        <v>207</v>
+        <v>138</v>
       </c>
       <c r="E187" s="1"/>
       <c r="F187" s="1" t="s">
-        <v>239</v>
+        <v>171</v>
       </c>
       <c r="G187" s="1"/>
     </row>
@@ -3545,11 +3589,11 @@
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1" t="s">
-        <v>208</v>
+        <v>139</v>
       </c>
       <c r="E188" s="1"/>
       <c r="F188" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G188" s="1"/>
     </row>
@@ -3557,35 +3601,35 @@
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>209</v>
+        <v>140</v>
       </c>
       <c r="E189" s="1"/>
       <c r="F189" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G189" s="1"/>
     </row>
     <row r="190" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
-      <c r="D190" s="1"/>
+      <c r="D190" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="E190" s="1"/>
-      <c r="F190" s="1"/>
+      <c r="F190" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G190" s="1"/>
     </row>
     <row r="191" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B191" s="1"/>
-      <c r="C191" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>240</v>
+        <v>171</v>
       </c>
       <c r="G191" s="1"/>
     </row>
@@ -3593,39 +3637,35 @@
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="E192" s="1"/>
       <c r="F192" s="1" t="s">
-        <v>66</v>
+        <v>209</v>
       </c>
       <c r="G192" s="1"/>
     </row>
     <row r="193" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
-      <c r="D193" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>236</v>
-      </c>
+      <c r="D193" s="1"/>
+      <c r="E193" s="1"/>
+      <c r="F193" s="1"/>
       <c r="G193" s="1"/>
     </row>
     <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194" s="1"/>
-      <c r="C194" s="1"/>
+      <c r="C194" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="D194" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E194" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F194" s="1" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
       <c r="G194" s="1"/>
     </row>
@@ -3633,35 +3673,37 @@
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E195" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F195" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G195" s="1"/>
     </row>
     <row r="196" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
-      <c r="D196" s="1"/>
+      <c r="D196" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="E196" s="1"/>
-      <c r="F196" s="1"/>
+      <c r="F196" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="G196" s="1"/>
     </row>
     <row r="197" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B197" s="1"/>
-      <c r="C197" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E197" s="1"/>
       <c r="F197" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G197" s="1"/>
     </row>
@@ -3669,13 +3711,11 @@
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="E198" s="1"/>
       <c r="F198" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G198" s="1"/>
     </row>
@@ -3683,11 +3723,11 @@
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>82</v>
+        <v>203</v>
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G199" s="1"/>
     </row>
@@ -3695,11 +3735,11 @@
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G200" s="1"/>
     </row>
@@ -3707,35 +3747,35 @@
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E201" s="1"/>
       <c r="F201" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G201" s="1"/>
     </row>
     <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
-      <c r="D202" s="1" t="s">
-        <v>208</v>
-      </c>
+      <c r="D202" s="1"/>
       <c r="E202" s="1"/>
-      <c r="F202" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="F202" s="1"/>
       <c r="G202" s="1"/>
     </row>
     <row r="203" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
-      <c r="C203" s="1"/>
+      <c r="C203" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="D203" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E203" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F203" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G203" s="1"/>
     </row>
@@ -3743,11 +3783,13 @@
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E204" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F204" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G204" s="1"/>
     </row>
@@ -3755,63 +3797,61 @@
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E205" s="1"/>
+        <v>242</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F205" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G205" s="1"/>
     </row>
     <row r="206" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
-      <c r="D206" s="1"/>
+      <c r="D206" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="E206" s="1"/>
-      <c r="F206" s="1"/>
+      <c r="F206" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="G206" s="1"/>
     </row>
     <row r="207" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B207" s="1"/>
-      <c r="C207" s="1" t="s">
-        <v>210</v>
-      </c>
+      <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="E207" s="1"/>
       <c r="F207" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G207" s="1"/>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
-      <c r="D208" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F208" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="D208" s="1"/>
+      <c r="E208" s="1"/>
+      <c r="F208" s="1"/>
       <c r="G208" s="1"/>
     </row>
     <row r="209" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B209" s="1"/>
-      <c r="C209" s="1"/>
+      <c r="C209" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="D209" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
       <c r="G209" s="1"/>
     </row>
@@ -3819,35 +3859,37 @@
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E210" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F210" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G210" s="1"/>
     </row>
     <row r="211" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
-      <c r="D211" s="1"/>
+      <c r="D211" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="E211" s="1"/>
-      <c r="F211" s="1"/>
+      <c r="F211" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="G211" s="1"/>
     </row>
     <row r="212" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
-      <c r="C212" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="C212" s="1"/>
       <c r="D212" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="E212" s="1"/>
       <c r="F212" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G212" s="1"/>
     </row>
@@ -3855,13 +3897,11 @@
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="E213" s="1"/>
       <c r="F213" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G213" s="1"/>
     </row>
@@ -3869,11 +3909,11 @@
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>82</v>
+        <v>204</v>
       </c>
       <c r="E214" s="1"/>
       <c r="F214" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -3881,11 +3921,11 @@
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E215" s="1"/>
       <c r="F215" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G215" s="1"/>
     </row>
@@ -3893,11 +3933,11 @@
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G216" s="1"/>
     </row>
@@ -3905,11 +3945,11 @@
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G217" s="1"/>
     </row>
@@ -3924,16 +3964,16 @@
     <row r="219" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B219" s="1"/>
       <c r="C219" s="1" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G219" s="1"/>
     </row>
@@ -3941,13 +3981,13 @@
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1" t="s">
-        <v>156</v>
+        <v>242</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="G220" s="1"/>
     </row>
@@ -3955,13 +3995,13 @@
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>213</v>
+        <v>171</v>
       </c>
       <c r="G221" s="1"/>
     </row>
@@ -3969,318 +4009,320 @@
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="E222" s="1"/>
       <c r="F222" s="1" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="G222" s="1"/>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
-      <c r="D223" s="1" t="s">
-        <v>150</v>
-      </c>
+      <c r="D223" s="1"/>
       <c r="E223" s="1"/>
-      <c r="F223" s="1" t="s">
-        <v>175</v>
-      </c>
+      <c r="F223" s="1"/>
       <c r="G223" s="1"/>
     </row>
     <row r="224" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B224" s="1"/>
-      <c r="C224" s="1"/>
+      <c r="C224" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="D224" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E224" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F224" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G224" s="1"/>
     </row>
-    <row r="225" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
-      <c r="D225" s="1"/>
-      <c r="E225" s="1"/>
-      <c r="F225" s="1"/>
+      <c r="D225" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="G225" s="1"/>
     </row>
-    <row r="226" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B226" s="1"/>
-      <c r="C226" s="1" t="s">
-        <v>149</v>
-      </c>
+      <c r="C226" s="1"/>
       <c r="D226" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E226" s="1"/>
       <c r="F226" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G226" s="1"/>
     </row>
-    <row r="227" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E227" s="1"/>
       <c r="F227" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G227" s="1"/>
     </row>
-    <row r="228" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="E228" s="1"/>
       <c r="F228" s="1" t="s">
-        <v>238</v>
+        <v>65</v>
       </c>
       <c r="G228" s="1"/>
     </row>
-    <row r="229" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E229" s="1"/>
       <c r="F229" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G229" s="1"/>
     </row>
-    <row r="230" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
-      <c r="D230" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="D230" s="1"/>
       <c r="E230" s="1"/>
-      <c r="F230" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="F230" s="1"/>
       <c r="G230" s="1"/>
     </row>
-    <row r="231" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B231" s="1"/>
-      <c r="C231" s="1"/>
-      <c r="D231" s="1"/>
-      <c r="E231" s="1"/>
-      <c r="F231" s="1"/>
+      <c r="C231" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="G231" s="1"/>
     </row>
-    <row r="232" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B232" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C232" s="1" t="s">
-        <v>98</v>
-      </c>
+    <row r="232" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B232" s="1"/>
+      <c r="C232" s="1"/>
       <c r="D232" s="1" t="s">
-        <v>2</v>
+        <v>153</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>236</v>
+        <v>64</v>
       </c>
       <c r="G232" s="1"/>
     </row>
-    <row r="233" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
       <c r="D233" s="1" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>66</v>
+        <v>209</v>
       </c>
       <c r="G233" s="1"/>
     </row>
-    <row r="234" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
       <c r="D234" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E234" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F234" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G234" s="1"/>
-      <c r="H234" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="235" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
-      <c r="D235" s="1"/>
+      <c r="D235" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="E235" s="1"/>
-      <c r="F235" s="1"/>
+      <c r="F235" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="G235" s="1"/>
     </row>
-    <row r="236" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B236" s="1"/>
-      <c r="C236" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="C236" s="1"/>
       <c r="D236" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="E236" s="1"/>
       <c r="F236" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G236" s="1"/>
     </row>
-    <row r="237" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
-      <c r="D237" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E237" s="1" t="s">
+      <c r="D237" s="1"/>
+      <c r="E237" s="1"/>
+      <c r="F237" s="1"/>
+      <c r="G237" s="1"/>
+    </row>
+    <row r="238" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B238" s="1"/>
+      <c r="C238" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E238" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F237" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="G237" s="1"/>
-    </row>
-    <row r="238" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B238" s="1"/>
-      <c r="C238" s="1"/>
-      <c r="D238" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E238" s="1"/>
       <c r="F238" s="1" t="s">
-        <v>175</v>
+        <v>236</v>
       </c>
       <c r="G238" s="1"/>
     </row>
-    <row r="239" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E239" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F239" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G239" s="1"/>
     </row>
-    <row r="240" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
       <c r="D240" s="1" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
       <c r="G240" s="1"/>
     </row>
-    <row r="241" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
-      <c r="D241" s="1"/>
+      <c r="D241" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="E241" s="1"/>
-      <c r="F241" s="1"/>
+      <c r="F241" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="G241" s="1"/>
     </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B242" s="1"/>
-      <c r="C242" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="C242" s="1"/>
       <c r="D242" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="E242" s="1"/>
       <c r="F242" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G242" s="1"/>
     </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
-      <c r="D243" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F243" s="1" t="s">
-        <v>240</v>
-      </c>
+      <c r="D243" s="1"/>
+      <c r="E243" s="1"/>
+      <c r="F243" s="1"/>
       <c r="G243" s="1"/>
     </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B244" s="1"/>
-      <c r="C244" s="1"/>
+    <row r="244" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B244" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="D244" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E244" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F244" s="1" t="s">
-        <v>175</v>
+        <v>232</v>
       </c>
       <c r="G244" s="1"/>
     </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
       <c r="D245" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E245" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F245" s="1" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
       <c r="G245" s="1"/>
     </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
       <c r="D246" s="1" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="E246" s="1"/>
       <c r="F246" s="1" t="s">
-        <v>67</v>
+        <v>248</v>
       </c>
       <c r="G246" s="1"/>
-    </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H246" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="247" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
@@ -4288,27 +4330,27 @@
       <c r="F247" s="1"/>
       <c r="G247" s="1"/>
     </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B248" s="1"/>
       <c r="C248" s="1" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="D248" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F248" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G248" s="1"/>
     </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
       <c r="D249" s="1" t="s">
-        <v>99</v>
+        <v>243</v>
       </c>
       <c r="E249" s="1" t="s">
         <v>5</v>
@@ -4318,62 +4360,210 @@
       </c>
       <c r="G249" s="1"/>
     </row>
-    <row r="250" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G250" s="1"/>
     </row>
-    <row r="251" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G251" s="1"/>
     </row>
-    <row r="252" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
       <c r="D252" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E252" s="1"/>
       <c r="F252" s="1" t="s">
-        <v>213</v>
+        <v>65</v>
       </c>
       <c r="G252" s="1"/>
     </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
-      <c r="D253" s="1" t="s">
-        <v>167</v>
-      </c>
+      <c r="D253" s="1"/>
       <c r="E253" s="1"/>
-      <c r="F253" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="F253" s="1"/>
       <c r="G253" s="1"/>
     </row>
-    <row r="255" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B255" t="s">
-        <v>168</v>
+    <row r="254" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B254" s="1"/>
+      <c r="C254" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G254" s="1"/>
+    </row>
+    <row r="255" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B255" s="1"/>
+      <c r="C255" s="1"/>
+      <c r="D255" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G255" s="1"/>
+    </row>
+    <row r="256" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B256" s="1"/>
+      <c r="C256" s="1"/>
+      <c r="D256" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E256" s="1"/>
+      <c r="F256" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G256" s="1"/>
+    </row>
+    <row r="257" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B257" s="1"/>
+      <c r="C257" s="1"/>
+      <c r="D257" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E257" s="1"/>
+      <c r="F257" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G257" s="1"/>
+    </row>
+    <row r="258" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B258" s="1"/>
+      <c r="C258" s="1"/>
+      <c r="D258" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E258" s="1"/>
+      <c r="F258" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G258" s="1"/>
+    </row>
+    <row r="259" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B259" s="1"/>
+      <c r="C259" s="1"/>
+      <c r="D259" s="1"/>
+      <c r="E259" s="1"/>
+      <c r="F259" s="1"/>
+      <c r="G259" s="1"/>
+    </row>
+    <row r="260" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B260" s="1"/>
+      <c r="C260" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F260" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G260" s="1"/>
+    </row>
+    <row r="261" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B261" s="1"/>
+      <c r="C261" s="1"/>
+      <c r="D261" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G261" s="1"/>
+    </row>
+    <row r="262" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B262" s="1"/>
+      <c r="C262" s="1"/>
+      <c r="D262" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E262" s="1"/>
+      <c r="F262" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G262" s="1"/>
+    </row>
+    <row r="263" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B263" s="1"/>
+      <c r="C263" s="1"/>
+      <c r="D263" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E263" s="1"/>
+      <c r="F263" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G263" s="1"/>
+    </row>
+    <row r="264" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B264" s="1"/>
+      <c r="C264" s="1"/>
+      <c r="D264" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E264" s="1"/>
+      <c r="F264" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G264" s="1"/>
+    </row>
+    <row r="265" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B265" s="1"/>
+      <c r="C265" s="1"/>
+      <c r="D265" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E265" s="1"/>
+      <c r="F265" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G265" s="1"/>
+    </row>
+    <row r="267" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B267" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E86:E89"/>
+    <mergeCell ref="E98:E101"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4392,21 +4582,21 @@
   <sheetData>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
         <v>49</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>50</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -4420,7 +4610,7 @@
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11">
         <v>0</v>

</xml_diff>

<commit_message>
Added code to save the values of group access
as per summary

codes that actually set the access is still not yet done
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.beta.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="264">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -671,9 +671,6 @@
     <t>varchar(15)</t>
   </si>
   <si>
-    <t>1=view, 2=enable-disable, 3=insert/update/delete</t>
-  </si>
-  <si>
     <t>(1/2/3)</t>
   </si>
   <si>
@@ -804,6 +801,15 @@
   </si>
   <si>
     <t>supplier_address_city</t>
+  </si>
+  <si>
+    <t>(1/2/4)</t>
+  </si>
+  <si>
+    <t>1=ACCESS, 2=INSERT/UPDATE, 4=VIEW LAPORAN</t>
+  </si>
+  <si>
+    <t>1 = ACCESS, 2 = INSERT, 4 = UPDATE, 8 = VIEW LAPORAN</t>
   </si>
 </sst>
 </file>
@@ -1185,8 +1191,8 @@
   </sheetPr>
   <dimension ref="B1:Q269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1236,7 @@
         <v>54</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>56</v>
@@ -1244,7 +1250,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1271,10 +1277,10 @@
         <v>209</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
       <c r="H6" t="s">
-        <v>217</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1288,7 +1294,7 @@
         <v>209</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H7" t="s">
         <v>66</v>
@@ -1335,10 +1341,10 @@
         <v>92</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1346,11 +1352,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1358,11 +1364,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1370,11 +1376,11 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1394,10 +1400,10 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>216</v>
@@ -1408,14 +1414,14 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
         <v>209</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -1490,7 +1496,7 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1585,7 +1591,7 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G29" s="1"/>
       <c r="N29" t="s">
@@ -1651,7 +1657,7 @@
         <v>54</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>56</v>
@@ -1683,7 +1689,7 @@
         <v>5</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -1700,6 +1706,9 @@
         <v>209</v>
       </c>
       <c r="G36" s="1"/>
+      <c r="H36" s="4" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
@@ -1721,7 +1730,7 @@
         <v>54</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>56</v>
@@ -1750,7 +1759,7 @@
         <v>5</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -1772,7 +1781,7 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="1" t="s">
@@ -1796,7 +1805,7 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="1" t="s">
@@ -1850,11 +1859,11 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -1868,7 +1877,7 @@
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>2</v>
@@ -1877,7 +1886,7 @@
         <v>54</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -1917,7 +1926,7 @@
         <v>5</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -1925,18 +1934,18 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" t="s">
+        <v>249</v>
+      </c>
+      <c r="K54" t="s">
         <v>250</v>
-      </c>
-      <c r="K54" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
@@ -1969,7 +1978,7 @@
         <v>54</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G57" s="1"/>
     </row>
@@ -1981,7 +1990,7 @@
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -1989,11 +1998,11 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2001,11 +2010,11 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2013,11 +2022,11 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G61" s="1"/>
     </row>
@@ -2053,7 +2062,7 @@
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G64" s="1"/>
     </row>
@@ -2089,7 +2098,7 @@
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G67" s="1"/>
     </row>
@@ -2104,10 +2113,10 @@
         <v>209</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H68" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
@@ -2130,7 +2139,7 @@
         <v>54</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G70" s="1"/>
     </row>
@@ -2152,11 +2161,11 @@
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G72" s="1"/>
     </row>
@@ -2164,11 +2173,11 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G73" s="1"/>
     </row>
@@ -2176,11 +2185,11 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2188,11 +2197,11 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G75" s="1"/>
     </row>
@@ -2200,7 +2209,7 @@
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
@@ -2238,7 +2247,7 @@
         <v>54</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>56</v>
@@ -2252,7 +2261,7 @@
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G80" s="1"/>
     </row>
@@ -2260,11 +2269,11 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G81" s="1"/>
     </row>
@@ -2272,11 +2281,11 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -2284,11 +2293,11 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G83" s="1"/>
     </row>
@@ -2324,7 +2333,7 @@
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G86" s="1"/>
     </row>
@@ -2370,7 +2379,7 @@
         <v>54</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>56</v>
@@ -2386,7 +2395,7 @@
         <v>63</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G91" s="1"/>
     </row>
@@ -2400,7 +2409,7 @@
         <v>63</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -2412,7 +2421,7 @@
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G93" s="1"/>
     </row>
@@ -2436,7 +2445,7 @@
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>78</v>
@@ -2450,7 +2459,7 @@
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>211</v>
@@ -2464,7 +2473,7 @@
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>213</v>
@@ -2478,7 +2487,7 @@
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>212</v>
@@ -2492,7 +2501,7 @@
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G99" s="1"/>
     </row>
@@ -2506,7 +2515,7 @@
         <v>192</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G100" s="1"/>
     </row>
@@ -2518,7 +2527,7 @@
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G101" s="1"/>
     </row>
@@ -2530,7 +2539,7 @@
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G102" s="1"/>
     </row>
@@ -2542,7 +2551,7 @@
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G103" s="1"/>
     </row>
@@ -2570,7 +2579,7 @@
         <v>5</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G105" s="1"/>
     </row>
@@ -2584,7 +2593,7 @@
         <v>193</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G106" s="1"/>
     </row>
@@ -2596,7 +2605,7 @@
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G107" s="1"/>
     </row>
@@ -2608,7 +2617,7 @@
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G108" s="1"/>
     </row>
@@ -2623,7 +2632,7 @@
         <v>209</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
@@ -2634,7 +2643,7 @@
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G110" s="1"/>
     </row>
@@ -2651,7 +2660,7 @@
         <v>209</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
@@ -2674,7 +2683,7 @@
         <v>54</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G113" s="1"/>
     </row>
@@ -2688,7 +2697,7 @@
         <v>5</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G114" s="1"/>
     </row>
@@ -2700,7 +2709,7 @@
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G115" s="1"/>
     </row>
@@ -2751,7 +2760,7 @@
         <v>54</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G119" s="1"/>
     </row>
@@ -2759,7 +2768,7 @@
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1" t="s">
@@ -2777,7 +2786,7 @@
         <v>5</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G121" s="1"/>
     </row>
@@ -2785,11 +2794,11 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G122" s="1"/>
     </row>
@@ -2803,7 +2812,7 @@
         <v>5</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G123" s="1"/>
     </row>
@@ -2811,11 +2820,11 @@
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G124" s="1"/>
     </row>
@@ -2827,7 +2836,7 @@
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G125" s="1"/>
     </row>
@@ -2851,7 +2860,7 @@
         <v>54</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G127" s="1"/>
     </row>
@@ -2863,7 +2872,7 @@
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G128" s="1"/>
     </row>
@@ -2909,7 +2918,7 @@
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G132" s="1"/>
     </row>
@@ -2921,7 +2930,7 @@
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G133" s="1"/>
     </row>
@@ -2933,7 +2942,7 @@
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G134" s="1"/>
     </row>
@@ -2969,7 +2978,7 @@
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G137" s="1"/>
     </row>
@@ -3017,7 +3026,7 @@
         <v>54</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G141" s="1"/>
     </row>
@@ -3043,7 +3052,7 @@
         <v>5</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G143" s="1"/>
     </row>
@@ -3067,7 +3076,7 @@
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G145" s="1"/>
     </row>
@@ -3127,7 +3136,7 @@
         <v>5</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G150" s="1"/>
     </row>
@@ -3141,7 +3150,7 @@
         <v>5</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G151" s="1"/>
     </row>
@@ -3153,7 +3162,7 @@
       </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G152" s="1"/>
     </row>
@@ -3165,7 +3174,7 @@
       </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G153" s="1"/>
     </row>
@@ -3177,7 +3186,7 @@
       </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G154" s="1"/>
     </row>
@@ -3201,7 +3210,7 @@
         <v>54</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G156" s="1"/>
     </row>
@@ -3223,7 +3232,7 @@
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
@@ -3235,7 +3244,7 @@
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
@@ -3263,7 +3272,7 @@
       </c>
       <c r="E161" s="1"/>
       <c r="F161" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G161" s="1"/>
     </row>
@@ -3311,7 +3320,7 @@
         <v>5</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G165" s="1"/>
     </row>
@@ -3325,7 +3334,7 @@
         <v>5</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G166" s="1"/>
     </row>
@@ -3337,7 +3346,7 @@
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G167" s="1"/>
     </row>
@@ -3349,7 +3358,7 @@
       </c>
       <c r="E168" s="1"/>
       <c r="F168" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G168" s="1"/>
     </row>
@@ -3361,7 +3370,7 @@
       </c>
       <c r="E169" s="1"/>
       <c r="F169" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G169" s="1"/>
     </row>
@@ -3373,7 +3382,7 @@
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G170" s="1"/>
     </row>
@@ -3397,7 +3406,7 @@
         <v>54</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G172" s="1"/>
     </row>
@@ -3425,7 +3434,7 @@
         <v>5</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G174" s="1"/>
     </row>
@@ -3449,7 +3458,7 @@
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G176" s="1"/>
     </row>
@@ -3485,7 +3494,7 @@
         <v>5</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G179" s="1"/>
     </row>
@@ -3499,7 +3508,7 @@
         <v>5</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G180" s="1"/>
     </row>
@@ -3511,7 +3520,7 @@
       </c>
       <c r="E181" s="1"/>
       <c r="F181" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G181" s="1"/>
     </row>
@@ -3523,7 +3532,7 @@
       </c>
       <c r="E182" s="1"/>
       <c r="F182" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G182" s="1"/>
     </row>
@@ -3547,7 +3556,7 @@
       </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G184" s="1"/>
     </row>
@@ -3571,7 +3580,7 @@
         <v>54</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G186" s="1"/>
     </row>
@@ -3599,7 +3608,7 @@
         <v>5</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G188" s="1"/>
     </row>
@@ -3623,7 +3632,7 @@
       </c>
       <c r="E190" s="1"/>
       <c r="F190" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G190" s="1"/>
     </row>
@@ -3635,7 +3644,7 @@
       </c>
       <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G191" s="1"/>
     </row>
@@ -3695,7 +3704,7 @@
         <v>5</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G196" s="1"/>
     </row>
@@ -3709,7 +3718,7 @@
         <v>5</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G197" s="1"/>
     </row>
@@ -3721,7 +3730,7 @@
       </c>
       <c r="E198" s="1"/>
       <c r="F198" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G198" s="1"/>
     </row>
@@ -3733,7 +3742,7 @@
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G199" s="1"/>
     </row>
@@ -3745,7 +3754,7 @@
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G200" s="1"/>
     </row>
@@ -3757,7 +3766,7 @@
       </c>
       <c r="E201" s="1"/>
       <c r="F201" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G201" s="1"/>
     </row>
@@ -3769,7 +3778,7 @@
       </c>
       <c r="E202" s="1"/>
       <c r="F202" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G202" s="1"/>
     </row>
@@ -3781,7 +3790,7 @@
       </c>
       <c r="E203" s="1"/>
       <c r="F203" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G203" s="1"/>
     </row>
@@ -3805,7 +3814,7 @@
         <v>54</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G205" s="1"/>
     </row>
@@ -3827,13 +3836,13 @@
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G207" s="1"/>
     </row>
@@ -3857,7 +3866,7 @@
       </c>
       <c r="E209" s="1"/>
       <c r="F209" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G209" s="1"/>
     </row>
@@ -3881,7 +3890,7 @@
         <v>5</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G211" s="1"/>
     </row>
@@ -3895,7 +3904,7 @@
         <v>5</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G212" s="1"/>
     </row>
@@ -3907,7 +3916,7 @@
       </c>
       <c r="E213" s="1"/>
       <c r="F213" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G213" s="1"/>
     </row>
@@ -3919,7 +3928,7 @@
       </c>
       <c r="E214" s="1"/>
       <c r="F214" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -3931,7 +3940,7 @@
       </c>
       <c r="E215" s="1"/>
       <c r="F215" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G215" s="1"/>
     </row>
@@ -3943,7 +3952,7 @@
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G216" s="1"/>
     </row>
@@ -3955,7 +3964,7 @@
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G217" s="1"/>
     </row>
@@ -3979,7 +3988,7 @@
       </c>
       <c r="E219" s="1"/>
       <c r="F219" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G219" s="1"/>
     </row>
@@ -4003,7 +4012,7 @@
         <v>54</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G221" s="1"/>
     </row>
@@ -4011,13 +4020,13 @@
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>63</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G222" s="1"/>
     </row>
@@ -4043,7 +4052,7 @@
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G224" s="1"/>
     </row>
@@ -4067,7 +4076,7 @@
         <v>5</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G226" s="1"/>
     </row>
@@ -4081,7 +4090,7 @@
         <v>5</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G227" s="1"/>
     </row>
@@ -4093,7 +4102,7 @@
       </c>
       <c r="E228" s="1"/>
       <c r="F228" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G228" s="1"/>
     </row>
@@ -4105,7 +4114,7 @@
       </c>
       <c r="E229" s="1"/>
       <c r="F229" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G229" s="1"/>
     </row>
@@ -4129,7 +4138,7 @@
       </c>
       <c r="E231" s="1"/>
       <c r="F231" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G231" s="1"/>
     </row>
@@ -4153,7 +4162,7 @@
         <v>54</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G233" s="1"/>
     </row>
@@ -4219,7 +4228,7 @@
       </c>
       <c r="E238" s="1"/>
       <c r="F238" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G238" s="1"/>
     </row>
@@ -4243,7 +4252,7 @@
         <v>5</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G240" s="1"/>
     </row>
@@ -4257,7 +4266,7 @@
         <v>5</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G241" s="1"/>
     </row>
@@ -4269,7 +4278,7 @@
       </c>
       <c r="E242" s="1"/>
       <c r="F242" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G242" s="1"/>
     </row>
@@ -4281,7 +4290,7 @@
       </c>
       <c r="E243" s="1"/>
       <c r="F243" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G243" s="1"/>
     </row>
@@ -4293,7 +4302,7 @@
       </c>
       <c r="E244" s="1"/>
       <c r="F244" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G244" s="1"/>
     </row>
@@ -4319,7 +4328,7 @@
         <v>54</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G246" s="1"/>
     </row>
@@ -4333,7 +4342,7 @@
         <v>63</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G247" s="1"/>
     </row>
@@ -4345,11 +4354,11 @@
       </c>
       <c r="E248" s="1"/>
       <c r="F248" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G248" s="1"/>
       <c r="H248" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="249" spans="2:8" x14ac:dyDescent="0.25">
@@ -4372,7 +4381,7 @@
         <v>54</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G250" s="1"/>
     </row>
@@ -4380,13 +4389,13 @@
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G251" s="1"/>
     </row>
@@ -4410,7 +4419,7 @@
       </c>
       <c r="E253" s="1"/>
       <c r="F253" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G253" s="1"/>
     </row>
@@ -4446,7 +4455,7 @@
         <v>54</v>
       </c>
       <c r="F256" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G256" s="1"/>
     </row>
@@ -4454,13 +4463,13 @@
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
       <c r="D257" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E257" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F257" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G257" s="1"/>
     </row>
@@ -4484,7 +4493,7 @@
       </c>
       <c r="E259" s="1"/>
       <c r="F259" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G259" s="1"/>
     </row>
@@ -4520,7 +4529,7 @@
         <v>54</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G262" s="1"/>
     </row>
@@ -4534,7 +4543,7 @@
         <v>5</v>
       </c>
       <c r="F263" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G263" s="1"/>
     </row>
@@ -4558,7 +4567,7 @@
       </c>
       <c r="E265" s="1"/>
       <c r="F265" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G265" s="1"/>
     </row>

</xml_diff>

<commit_message>
update code in datauserform and update design table
pelase review
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.beta.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,14 +11,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$270</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$274</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="274">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -812,7 +812,34 @@
     <t>1 = ACCESS, 2 = INSERT, 4 = UPDATE, 8 = VIEW LAPORAN</t>
   </si>
   <si>
-    <t>PRODUCT_CATEGORY</t>
+    <t>filename, upload to program/products</t>
+  </si>
+  <si>
+    <t>MESSAGE SYSTEM</t>
+  </si>
+  <si>
+    <t>MASTER MESSAGE</t>
+  </si>
+  <si>
+    <t>msg_content</t>
+  </si>
+  <si>
+    <t>msg_datetime_created</t>
+  </si>
+  <si>
+    <t>msg_datetime_read</t>
+  </si>
+  <si>
+    <t>if there is content status is read</t>
+  </si>
+  <si>
+    <t>user who read the message</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t>msg_read_user_id</t>
   </si>
 </sst>
 </file>
@@ -945,7 +972,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -980,7 +1007,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1192,10 +1219,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q272"/>
+  <dimension ref="B1:Q277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1231,7 @@
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -1437,7 +1464,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1448,7 +1475,7 @@
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>1</v>
+        <v>266</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
@@ -1457,23 +1484,21 @@
         <v>54</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1481,13 +1506,11 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>214</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1495,11 +1518,11 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>3</v>
+        <v>267</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1507,54 +1530,42 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>53</v>
+        <v>269</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>195</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>273</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" t="s">
-        <v>66</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="P25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>44</v>
+      <c r="G25" s="1" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1564,10 +1575,10 @@
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>54</v>
@@ -1575,99 +1586,89 @@
       <c r="F28" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="N28" t="s">
-        <v>43</v>
-      </c>
-      <c r="P28">
-        <v>1</v>
-      </c>
-      <c r="Q28">
-        <v>1</v>
+      <c r="G28" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F29" s="1" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="N29" t="s">
-        <v>44</v>
-      </c>
-      <c r="P29">
-        <v>2</v>
-      </c>
-      <c r="Q29">
-        <v>3</v>
-      </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>215</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>216</v>
       </c>
       <c r="G30" s="1"/>
-      <c r="N30" t="s">
-        <v>45</v>
-      </c>
-      <c r="P30">
-        <v>3</v>
-      </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>209</v>
+        <v>254</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="P32" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1678,218 +1679,245 @@
         <v>209</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="N34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>231</v>
-      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>43</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D36" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>59</v>
+        <v>4</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>209</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>44</v>
+      </c>
+      <c r="P36">
+        <v>2</v>
+      </c>
+      <c r="Q36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>45</v>
+      </c>
+      <c r="P37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
         <v>209</v>
       </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="1" t="s">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E42" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F42" s="1" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E43" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F43" s="1" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="H43" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E44" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="F44" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
-      <c r="C47" s="1" t="s">
-        <v>166</v>
-      </c>
+      <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>209</v>
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E48" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F48" s="1" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="G48" s="1"/>
-      <c r="H48" t="s">
-        <v>244</v>
-      </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
-      <c r="C50" s="1" t="s">
-        <v>245</v>
-      </c>
+      <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -1897,13 +1925,11 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E51" s="2"/>
       <c r="F51" s="1" t="s">
-        <v>209</v>
+        <v>65</v>
       </c>
       <c r="G51" s="1"/>
     </row>
@@ -1911,11 +1937,11 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1" t="s">
-        <v>195</v>
+        <v>216</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -1923,77 +1949,76 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
-      <c r="D54" s="1" t="s">
-        <v>248</v>
-      </c>
+      <c r="D54" s="1"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" t="s">
-        <v>249</v>
-      </c>
-      <c r="K54" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="1"/>
+      <c r="C55" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G55" s="1"/>
+      <c r="H55" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B56" s="1"/>
       <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
-      <c r="C57" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>231</v>
-      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="D58" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E58" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="F58" s="1" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -2001,11 +2026,13 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E59" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F59" s="1" t="s">
-        <v>254</v>
+        <v>209</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2013,11 +2040,11 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E60" s="1"/>
+        <v>171</v>
+      </c>
+      <c r="E60" s="2"/>
       <c r="F60" s="1" t="s">
-        <v>254</v>
+        <v>195</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2025,59 +2052,65 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F61" s="1" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="G61" s="1"/>
+      <c r="H61" t="s">
+        <v>249</v>
+      </c>
+      <c r="K61" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="1"/>
+        <v>248</v>
+      </c>
+      <c r="E62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="G62" s="1"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-      <c r="D63" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C64" s="1"/>
-      <c r="D64" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="1" t="s">
-        <v>254</v>
-      </c>
+      <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="C65" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="D65" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F65" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -2085,11 +2118,11 @@
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>172</v>
+        <v>15</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>171</v>
+        <v>254</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -2097,11 +2130,11 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>173</v>
+        <v>255</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="G67" s="1"/>
     </row>
@@ -2109,40 +2142,35 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>174</v>
+        <v>256</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H68" t="s">
-        <v>225</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="G68" s="1"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="D69" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="F69" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
-      <c r="C70" s="1" t="s">
-        <v>170</v>
-      </c>
+      <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="G70" s="1"/>
     </row>
@@ -2150,13 +2178,11 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="G71" s="1"/>
     </row>
@@ -2164,11 +2190,11 @@
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>226</v>
+        <v>18</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="G72" s="1"/>
     </row>
@@ -2176,11 +2202,11 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>227</v>
+        <v>71</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="G73" s="1"/>
     </row>
@@ -2188,11 +2214,11 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>228</v>
+        <v>172</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>234</v>
+        <v>171</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2200,71 +2226,78 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>229</v>
+        <v>173</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="G75" s="1"/>
+      <c r="H75" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>230</v>
+        <v>174</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G76" s="1"/>
+        <v>209</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B78" s="1"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+      <c r="D78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="G78" s="1"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
-      <c r="C79" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="G79" s="1"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>22</v>
+        <v>226</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="G80" s="1"/>
     </row>
@@ -2272,11 +2305,11 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="G81" s="1"/>
     </row>
@@ -2284,11 +2317,11 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -2296,11 +2329,11 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="G83" s="1"/>
     </row>
@@ -2308,95 +2341,93 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>23</v>
+        <v>230</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>216</v>
+        <v>171</v>
       </c>
       <c r="G84" s="1"/>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
-      <c r="D85" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="1"/>
+      <c r="B86" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C86" s="1"/>
-      <c r="D86" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-      <c r="F86" s="1" t="s">
-        <v>254</v>
-      </c>
+      <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
+      <c r="C87" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D87" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E87" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F87" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G87" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
+      <c r="D88" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
+      <c r="F88" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="G88" s="1"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
+      <c r="D89" s="1" t="s">
+        <v>258</v>
+      </c>
       <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
+      <c r="F89" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="G89" s="1"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
-      <c r="C90" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F90" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G90" s="1"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
         <v>254</v>
       </c>
@@ -2406,13 +2437,11 @@
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -2420,11 +2449,11 @@
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>175</v>
+        <v>24</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="G93" s="1"/>
     </row>
@@ -2432,11 +2461,11 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>176</v>
+        <v>25</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>65</v>
+        <v>254</v>
       </c>
       <c r="G94" s="1"/>
     </row>
@@ -2444,65 +2473,59 @@
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>177</v>
+        <v>72</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="G95" s="1"/>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
-      <c r="D96" s="1" t="s">
-        <v>178</v>
-      </c>
+      <c r="D96" s="1"/>
       <c r="E96" s="1"/>
-      <c r="F96" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="1"/>
+      <c r="B97" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C97" s="1"/>
-      <c r="D97" s="1" t="s">
-        <v>179</v>
-      </c>
+      <c r="D97" s="1"/>
       <c r="E97" s="1"/>
-      <c r="F97" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+      <c r="C98" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D98" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1" t="s">
-        <v>233</v>
+        <v>2</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>212</v>
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E99" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F99" s="1" t="s">
         <v>254</v>
       </c>
@@ -2512,13 +2535,13 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>192</v>
+        <v>210</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="G100" s="1"/>
     </row>
@@ -2526,9 +2549,9 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E101" s="5"/>
+        <v>175</v>
+      </c>
+      <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
         <v>254</v>
       </c>
@@ -2538,11 +2561,11 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E102" s="5"/>
+        <v>176</v>
+      </c>
+      <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>254</v>
+        <v>65</v>
       </c>
       <c r="G102" s="1"/>
     </row>
@@ -2550,77 +2573,83 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E103" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G103" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G104" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G105" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>193</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G106" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G107" s="1"/>
+        <v>254</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E108" s="1"/>
+        <v>182</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="F108" s="1" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="G108" s="1"/>
     </row>
@@ -2628,23 +2657,21 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E109" s="1"/>
+        <v>183</v>
+      </c>
+      <c r="E109" s="5"/>
       <c r="F109" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>218</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="G109" s="1"/>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E110" s="1"/>
+        <v>184</v>
+      </c>
+      <c r="E110" s="5"/>
       <c r="F110" s="1" t="s">
         <v>254</v>
       </c>
@@ -2654,39 +2681,39 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>199</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="E111" s="5"/>
       <c r="F111" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>218</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="G111" s="1"/>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="3"/>
-      <c r="F112" s="1"/>
+      <c r="D112" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G112" s="1"/>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
-      <c r="C113" s="1" t="s">
-        <v>264</v>
-      </c>
+      <c r="C113" s="1"/>
       <c r="D113" s="1" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="G113" s="1"/>
     </row>
@@ -2694,37 +2721,37 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
+      <c r="D115" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
+      <c r="F115" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="G115" s="1"/>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
-      <c r="C116" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G116" s="1"/>
     </row>
@@ -2732,25 +2759,25 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G117" s="1"/>
+        <v>209</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>28</v>
+        <v>191</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="G118" s="1"/>
     </row>
@@ -2758,47 +2785,50 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E119" s="1"/>
+        <v>198</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="F119" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G119" s="1"/>
+        <v>209</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
-      <c r="D120" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="D120" s="1"/>
       <c r="E120" s="1"/>
-      <c r="F120" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="F120" s="1"/>
       <c r="G120" s="1"/>
-      <c r="H120" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
+      <c r="C121" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G121" s="1"/>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
-      <c r="C122" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>235</v>
@@ -2809,11 +2839,11 @@
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>171</v>
+        <v>232</v>
       </c>
       <c r="G123" s="1"/>
     </row>
@@ -2821,51 +2851,50 @@
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="G124" s="1"/>
+      <c r="H124" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1" t="s">
-        <v>226</v>
+        <v>30</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="G125" s="1"/>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
-      <c r="D126" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
       <c r="G126" s="1"/>
     </row>
     <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
+      <c r="C127" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="D127" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E127" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F127" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G127" s="1"/>
     </row>
@@ -2873,35 +2902,37 @@
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>232</v>
+        <v>171</v>
       </c>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
-      <c r="F129" s="1"/>
+      <c r="D129" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
-      <c r="C130" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="C130" s="1"/>
       <c r="D130" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G130" s="1"/>
     </row>
@@ -2909,11 +2940,13 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E131" s="1"/>
+        <v>196</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F131" s="1" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
       <c r="G131" s="1"/>
     </row>
@@ -2921,11 +2954,11 @@
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>83</v>
+        <v>238</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="G132" s="1"/>
     </row>
@@ -2933,11 +2966,11 @@
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="G133" s="1"/>
     </row>
@@ -2952,12 +2985,14 @@
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="C135" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E135" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F135" s="1" t="s">
         <v>231</v>
       </c>
@@ -2967,11 +3002,11 @@
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="G136" s="1"/>
     </row>
@@ -2979,47 +3014,45 @@
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>232</v>
+        <v>65</v>
       </c>
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
-      <c r="D138" s="1"/>
+      <c r="D138" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E138" s="1"/>
-      <c r="F138" s="1"/>
+      <c r="F138" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
-      <c r="C139" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
       <c r="G139" s="1"/>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
-      <c r="C140" s="1"/>
+      <c r="C140" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D140" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="G140" s="1"/>
     </row>
@@ -3027,11 +3060,11 @@
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="G141" s="1"/>
     </row>
@@ -3039,11 +3072,11 @@
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="G142" s="1"/>
     </row>
@@ -3058,16 +3091,16 @@
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" s="1"/>
       <c r="C144" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="G144" s="1"/>
     </row>
@@ -3075,11 +3108,11 @@
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>64</v>
+        <v>254</v>
       </c>
       <c r="G145" s="1"/>
     </row>
@@ -3087,13 +3120,11 @@
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E146" s="1"/>
       <c r="F146" s="1" t="s">
-        <v>231</v>
+        <v>65</v>
       </c>
       <c r="G146" s="1"/>
     </row>
@@ -3101,35 +3132,35 @@
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="G147" s="1"/>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
-      <c r="D148" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="D148" s="1"/>
       <c r="E148" s="1"/>
-      <c r="F148" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F148" s="1"/>
       <c r="G148" s="1"/>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" s="1"/>
-      <c r="C149" s="1"/>
+      <c r="C149" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D149" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E149" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F149" s="1" t="s">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="G149" s="1"/>
     </row>
@@ -3137,11 +3168,11 @@
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>201</v>
+        <v>87</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
       <c r="G150" s="1"/>
     </row>
@@ -3149,35 +3180,37 @@
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E151" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F151" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G151" s="1"/>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
-      <c r="D152" s="1"/>
+      <c r="D152" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
+      <c r="F152" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="G152" s="1"/>
     </row>
     <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" s="1"/>
-      <c r="C153" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E153" s="1"/>
       <c r="F153" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G153" s="1"/>
     </row>
@@ -3185,13 +3218,11 @@
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="E154" s="1"/>
       <c r="F154" s="1" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="G154" s="1"/>
     </row>
@@ -3199,11 +3230,11 @@
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>106</v>
+        <v>201</v>
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>233</v>
+        <v>171</v>
       </c>
       <c r="G155" s="1"/>
     </row>
@@ -3211,44 +3242,46 @@
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="G156" s="1"/>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
-      <c r="D157" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="D157" s="1"/>
       <c r="E157" s="1"/>
-      <c r="F157" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F157" s="1"/>
       <c r="G157" s="1"/>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
+      <c r="C158" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G158" s="1"/>
     </row>
     <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159" s="1"/>
-      <c r="C159" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>235</v>
@@ -3259,13 +3292,11 @@
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="E160" s="1"/>
       <c r="F160" s="1" t="s">
-        <v>64</v>
+        <v>233</v>
       </c>
       <c r="G160" s="1"/>
     </row>
@@ -3273,11 +3304,11 @@
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
-        <v>239</v>
+        <v>117</v>
       </c>
       <c r="E161" s="1"/>
       <c r="F161" s="1" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="G161" s="1"/>
     </row>
@@ -3285,35 +3316,35 @@
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
-        <v>240</v>
+        <v>42</v>
       </c>
       <c r="E162" s="1"/>
       <c r="F162" s="1" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="G162" s="1"/>
     </row>
     <row r="163" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
-      <c r="D163" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="D163" s="1"/>
       <c r="E163" s="1"/>
-      <c r="F163" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="F163" s="1"/>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" s="1"/>
-      <c r="C164" s="1"/>
+      <c r="C164" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D164" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E164" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F164" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G164" s="1"/>
     </row>
@@ -3321,11 +3352,13 @@
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E165" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F165" s="1" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
       <c r="G165" s="1"/>
     </row>
@@ -3333,7 +3366,7 @@
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1" t="s">
-        <v>104</v>
+        <v>239</v>
       </c>
       <c r="E166" s="1"/>
       <c r="F166" s="1" t="s">
@@ -3344,24 +3377,24 @@
     <row r="167" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
+      <c r="D167" s="1" t="s">
+        <v>240</v>
+      </c>
       <c r="E167" s="1"/>
-      <c r="F167" s="1"/>
+      <c r="F167" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B168" s="1"/>
-      <c r="C168" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="C168" s="1"/>
       <c r="D168" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="E168" s="1"/>
       <c r="F168" s="1" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
       <c r="G168" s="1"/>
     </row>
@@ -3369,13 +3402,11 @@
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E169" s="1"/>
       <c r="F169" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G169" s="1"/>
     </row>
@@ -3383,11 +3414,11 @@
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1" t="s">
-        <v>233</v>
+        <v>171</v>
       </c>
       <c r="G170" s="1"/>
     </row>
@@ -3395,59 +3426,61 @@
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="E171" s="1"/>
       <c r="F171" s="1" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="G171" s="1"/>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
-      <c r="D172" s="1" t="s">
-        <v>118</v>
-      </c>
+      <c r="D172" s="1"/>
       <c r="E172" s="1"/>
-      <c r="F172" s="1" t="s">
-        <v>232</v>
-      </c>
+      <c r="F172" s="1"/>
       <c r="G172" s="1"/>
     </row>
     <row r="173" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B173" s="1"/>
-      <c r="C173" s="1"/>
+      <c r="C173" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D173" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E173" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F173" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G173" s="1"/>
     </row>
     <row r="174" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
-      <c r="D174" s="1"/>
-      <c r="E174" s="1"/>
-      <c r="F174" s="1"/>
+      <c r="D174" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G174" s="1"/>
     </row>
     <row r="175" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B175" s="1"/>
-      <c r="C175" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="C175" s="1"/>
       <c r="D175" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E175" s="1"/>
       <c r="F175" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G175" s="1"/>
     </row>
@@ -3455,13 +3488,11 @@
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E176" s="1"/>
       <c r="F176" s="1" t="s">
-        <v>64</v>
+        <v>233</v>
       </c>
       <c r="G176" s="1"/>
     </row>
@@ -3469,13 +3500,11 @@
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E177" s="1"/>
       <c r="F177" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G177" s="1"/>
     </row>
@@ -3483,59 +3512,63 @@
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E178" s="1"/>
       <c r="F178" s="1" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="G178" s="1"/>
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
-      <c r="D179" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="D179" s="1"/>
       <c r="E179" s="1"/>
-      <c r="F179" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F179" s="1"/>
       <c r="G179" s="1"/>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B180" s="1"/>
-      <c r="C180" s="1"/>
+      <c r="C180" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="D180" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E180" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F180" s="1" t="s">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="G180" s="1"/>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
-      <c r="D181" s="1"/>
-      <c r="E181" s="1"/>
-      <c r="F181" s="1"/>
+      <c r="D181" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="G181" s="1"/>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B182" s="1"/>
-      <c r="C182" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="C182" s="1"/>
       <c r="D182" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G182" s="1"/>
     </row>
@@ -3543,13 +3576,11 @@
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E183" s="1"/>
       <c r="F183" s="1" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
       <c r="G183" s="1"/>
     </row>
@@ -3557,7 +3588,7 @@
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1" t="s">
@@ -3569,59 +3600,61 @@
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="E185" s="1"/>
       <c r="F185" s="1" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="G185" s="1"/>
     </row>
     <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
-      <c r="D186" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="D186" s="1"/>
       <c r="E186" s="1"/>
-      <c r="F186" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="F186" s="1"/>
       <c r="G186" s="1"/>
     </row>
     <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B187" s="1"/>
-      <c r="C187" s="1"/>
+      <c r="C187" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="D187" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E187" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F187" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G187" s="1"/>
     </row>
     <row r="188" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
-      <c r="D188" s="1"/>
-      <c r="E188" s="1"/>
-      <c r="F188" s="1"/>
+      <c r="D188" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G188" s="1"/>
     </row>
     <row r="189" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B189" s="1"/>
-      <c r="C189" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E189" s="1"/>
       <c r="F189" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G189" s="1"/>
     </row>
@@ -3629,13 +3662,11 @@
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E190" s="1"/>
       <c r="F190" s="1" t="s">
-        <v>64</v>
+        <v>232</v>
       </c>
       <c r="G190" s="1"/>
     </row>
@@ -3643,13 +3674,11 @@
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>231</v>
+        <v>65</v>
       </c>
       <c r="G191" s="1"/>
     </row>
@@ -3657,35 +3686,35 @@
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="E192" s="1"/>
       <c r="F192" s="1" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="G192" s="1"/>
     </row>
     <row r="193" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
-      <c r="D193" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="D193" s="1"/>
       <c r="E193" s="1"/>
-      <c r="F193" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F193" s="1"/>
       <c r="G193" s="1"/>
     </row>
     <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194" s="1"/>
-      <c r="C194" s="1"/>
+      <c r="C194" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="D194" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E194" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F194" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G194" s="1"/>
     </row>
@@ -3693,11 +3722,13 @@
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E195" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F195" s="1" t="s">
-        <v>209</v>
+        <v>64</v>
       </c>
       <c r="G195" s="1"/>
     </row>
@@ -3705,11 +3736,13 @@
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E196" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F196" s="1" t="s">
-        <v>171</v>
+        <v>231</v>
       </c>
       <c r="G196" s="1"/>
     </row>
@@ -3717,35 +3750,35 @@
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E197" s="1"/>
       <c r="F197" s="1" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="G197" s="1"/>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
-      <c r="D198" s="1"/>
+      <c r="D198" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="E198" s="1"/>
-      <c r="F198" s="1"/>
+      <c r="F198" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="G198" s="1"/>
     </row>
     <row r="199" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B199" s="1"/>
-      <c r="C199" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E199" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G199" s="1"/>
     </row>
@@ -3753,13 +3786,11 @@
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="G200" s="1"/>
     </row>
@@ -3767,11 +3798,11 @@
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="E201" s="1"/>
       <c r="F201" s="1" t="s">
-        <v>233</v>
+        <v>171</v>
       </c>
       <c r="G201" s="1"/>
     </row>
@@ -3779,35 +3810,35 @@
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="E202" s="1"/>
       <c r="F202" s="1" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="G202" s="1"/>
     </row>
     <row r="203" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
-      <c r="D203" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="D203" s="1"/>
       <c r="E203" s="1"/>
-      <c r="F203" s="1" t="s">
-        <v>234</v>
-      </c>
+      <c r="F203" s="1"/>
       <c r="G203" s="1"/>
     </row>
     <row r="204" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B204" s="1"/>
-      <c r="C204" s="1"/>
+      <c r="C204" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="D204" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E204" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F204" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G204" s="1"/>
     </row>
@@ -3815,11 +3846,13 @@
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E205" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F205" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G205" s="1"/>
     </row>
@@ -3827,7 +3860,7 @@
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>205</v>
+        <v>80</v>
       </c>
       <c r="E206" s="1"/>
       <c r="F206" s="1" t="s">
@@ -3838,24 +3871,24 @@
     <row r="207" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
-      <c r="D207" s="1"/>
+      <c r="D207" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="E207" s="1"/>
-      <c r="F207" s="1"/>
+      <c r="F207" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="G207" s="1"/>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
-      <c r="C208" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="C208" s="1"/>
       <c r="D208" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="E208" s="1"/>
       <c r="F208" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G208" s="1"/>
     </row>
@@ -3863,13 +3896,11 @@
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E209" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="E209" s="1"/>
       <c r="F209" s="1" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="G209" s="1"/>
     </row>
@@ -3877,13 +3908,11 @@
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="E210" s="1"/>
       <c r="F210" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G210" s="1"/>
     </row>
@@ -3891,47 +3920,49 @@
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
       <c r="E211" s="1"/>
       <c r="F211" s="1" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="G211" s="1"/>
     </row>
     <row r="212" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
-      <c r="D212" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="D212" s="1"/>
       <c r="E212" s="1"/>
-      <c r="F212" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F212" s="1"/>
       <c r="G212" s="1"/>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B213" s="1"/>
-      <c r="C213" s="1"/>
-      <c r="D213" s="1"/>
-      <c r="E213" s="1"/>
-      <c r="F213" s="1"/>
+      <c r="C213" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G213" s="1"/>
     </row>
     <row r="214" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B214" s="1"/>
-      <c r="C214" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>235</v>
+        <v>64</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -3939,13 +3970,13 @@
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G215" s="1"/>
     </row>
@@ -3953,11 +3984,11 @@
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>233</v>
+        <v>171</v>
       </c>
       <c r="G216" s="1"/>
     </row>
@@ -3965,35 +3996,35 @@
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>202</v>
+        <v>129</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G217" s="1"/>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
-      <c r="D218" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="D218" s="1"/>
       <c r="E218" s="1"/>
-      <c r="F218" s="1" t="s">
-        <v>234</v>
-      </c>
+      <c r="F218" s="1"/>
       <c r="G218" s="1"/>
     </row>
     <row r="219" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B219" s="1"/>
-      <c r="C219" s="1"/>
+      <c r="C219" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="D219" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E219" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F219" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G219" s="1"/>
     </row>
@@ -4001,11 +4032,13 @@
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E220" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F220" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G220" s="1"/>
     </row>
@@ -4013,11 +4046,11 @@
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="E221" s="1"/>
       <c r="F221" s="1" t="s">
-        <v>65</v>
+        <v>233</v>
       </c>
       <c r="G221" s="1"/>
     </row>
@@ -4025,35 +4058,35 @@
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="E222" s="1"/>
       <c r="F222" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G222" s="1"/>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
-      <c r="D223" s="1"/>
+      <c r="D223" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="E223" s="1"/>
-      <c r="F223" s="1"/>
+      <c r="F223" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="G223" s="1"/>
     </row>
     <row r="224" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B224" s="1"/>
-      <c r="C224" s="1" t="s">
-        <v>206</v>
-      </c>
+      <c r="C224" s="1"/>
       <c r="D224" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="E224" s="1"/>
       <c r="F224" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G224" s="1"/>
     </row>
@@ -4061,13 +4094,11 @@
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E225" s="1"/>
       <c r="F225" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G225" s="1"/>
     </row>
@@ -4075,13 +4106,11 @@
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E226" s="1"/>
       <c r="F226" s="1" t="s">
-        <v>171</v>
+        <v>65</v>
       </c>
       <c r="G226" s="1"/>
     </row>
@@ -4089,7 +4118,7 @@
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E227" s="1"/>
       <c r="F227" s="1" t="s">
@@ -4108,13 +4137,13 @@
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B229" s="1"/>
       <c r="C229" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>235</v>
@@ -4125,13 +4154,13 @@
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
       <c r="D230" s="1" t="s">
-        <v>77</v>
+        <v>241</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G230" s="1"/>
     </row>
@@ -4139,11 +4168,13 @@
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E231" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F231" s="1" t="s">
-        <v>233</v>
+        <v>171</v>
       </c>
       <c r="G231" s="1"/>
     </row>
@@ -4151,59 +4182,61 @@
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
       <c r="D232" s="1" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="E232" s="1"/>
       <c r="F232" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G232" s="1"/>
     </row>
     <row r="233" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
-      <c r="D233" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="D233" s="1"/>
       <c r="E233" s="1"/>
-      <c r="F233" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="F233" s="1"/>
       <c r="G233" s="1"/>
     </row>
     <row r="234" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B234" s="1"/>
-      <c r="C234" s="1"/>
+      <c r="C234" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="D234" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E234" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F234" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G234" s="1"/>
     </row>
     <row r="235" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
-      <c r="D235" s="1"/>
-      <c r="E235" s="1"/>
-      <c r="F235" s="1"/>
+      <c r="D235" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G235" s="1"/>
     </row>
     <row r="236" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B236" s="1"/>
-      <c r="C236" s="1" t="s">
-        <v>145</v>
-      </c>
+      <c r="C236" s="1"/>
       <c r="D236" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E236" s="1"/>
       <c r="F236" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G236" s="1"/>
     </row>
@@ -4211,13 +4244,11 @@
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
       <c r="D237" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E237" s="1"/>
       <c r="F237" s="1" t="s">
-        <v>64</v>
+        <v>232</v>
       </c>
       <c r="G237" s="1"/>
     </row>
@@ -4225,13 +4256,11 @@
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E238" s="1"/>
       <c r="F238" s="1" t="s">
-        <v>209</v>
+        <v>65</v>
       </c>
       <c r="G238" s="1"/>
     </row>
@@ -4239,61 +4268,63 @@
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="E239" s="1"/>
       <c r="F239" s="1" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="G239" s="1"/>
     </row>
     <row r="240" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
-      <c r="D240" s="1" t="s">
-        <v>147</v>
-      </c>
+      <c r="D240" s="1"/>
       <c r="E240" s="1"/>
-      <c r="F240" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="F240" s="1"/>
       <c r="G240" s="1"/>
     </row>
     <row r="241" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B241" s="1"/>
-      <c r="C241" s="1"/>
+      <c r="C241" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="D241" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E241" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="F241" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="G241" s="1"/>
     </row>
     <row r="242" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
-      <c r="D242" s="1"/>
-      <c r="E242" s="1"/>
-      <c r="F242" s="1"/>
+      <c r="D242" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="G242" s="1"/>
     </row>
     <row r="243" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B243" s="1"/>
-      <c r="C243" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="C243" s="1"/>
       <c r="D243" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E243" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="G243" s="1"/>
     </row>
@@ -4301,13 +4332,13 @@
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
       <c r="D244" s="1" t="s">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="E244" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="G244" s="1"/>
     </row>
@@ -4315,11 +4346,11 @@
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
       <c r="D245" s="1" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
       <c r="E245" s="1"/>
       <c r="F245" s="1" t="s">
-        <v>233</v>
+        <v>171</v>
       </c>
       <c r="G245" s="1"/>
     </row>
@@ -4327,49 +4358,49 @@
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
       <c r="D246" s="1" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="E246" s="1"/>
       <c r="F246" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G246" s="1"/>
     </row>
     <row r="247" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
-      <c r="D247" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="D247" s="1"/>
       <c r="E247" s="1"/>
-      <c r="F247" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F247" s="1"/>
       <c r="G247" s="1"/>
     </row>
     <row r="248" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B248" s="1"/>
-      <c r="C248" s="1"/>
-      <c r="D248" s="1"/>
-      <c r="E248" s="1"/>
-      <c r="F248" s="1"/>
+      <c r="C248" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G248" s="1"/>
     </row>
     <row r="249" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B249" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C249" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
       <c r="D249" s="1" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="G249" s="1"/>
     </row>
@@ -4377,13 +4408,11 @@
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E250" s="1"/>
       <c r="F250" s="1" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="G250" s="1"/>
     </row>
@@ -4391,52 +4420,49 @@
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="G251" s="1"/>
-      <c r="H251" t="s">
-        <v>246</v>
-      </c>
     </row>
     <row r="252" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
-      <c r="D252" s="1"/>
+      <c r="D252" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="E252" s="1"/>
-      <c r="F252" s="1"/>
+      <c r="F252" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="G252" s="1"/>
     </row>
     <row r="253" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B253" s="1"/>
-      <c r="C253" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D253" s="1" t="s">
+      <c r="C253" s="1"/>
+      <c r="D253" s="1"/>
+      <c r="E253" s="1"/>
+      <c r="F253" s="1"/>
+      <c r="G253" s="1"/>
+    </row>
+    <row r="254" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B254" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D254" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E253" s="1" t="s">
+      <c r="E254" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F253" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G253" s="1"/>
-    </row>
-    <row r="254" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B254" s="1"/>
-      <c r="C254" s="1"/>
-      <c r="D254" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F254" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G254" s="1"/>
     </row>
@@ -4444,56 +4470,63 @@
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
       <c r="D255" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E255" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F255" s="1" t="s">
-        <v>171</v>
+        <v>254</v>
       </c>
       <c r="G255" s="1"/>
+      <c r="H255" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="256" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
       <c r="D256" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="E256" s="1"/>
       <c r="F256" s="1" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="G256" s="1"/>
     </row>
     <row r="257" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
-      <c r="D257" s="1" t="s">
-        <v>159</v>
-      </c>
+      <c r="D257" s="1"/>
       <c r="E257" s="1"/>
-      <c r="F257" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="F257" s="1"/>
       <c r="G257" s="1"/>
     </row>
     <row r="258" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B258" s="1"/>
-      <c r="C258" s="1"/>
-      <c r="D258" s="1"/>
-      <c r="E258" s="1"/>
-      <c r="F258" s="1"/>
+      <c r="C258" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G258" s="1"/>
     </row>
     <row r="259" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B259" s="1"/>
-      <c r="C259" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="C259" s="1"/>
       <c r="D259" s="1" t="s">
-        <v>2</v>
+        <v>242</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>235</v>
@@ -4504,13 +4537,11 @@
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
       <c r="D260" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E260" s="1"/>
       <c r="F260" s="1" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
       <c r="G260" s="1"/>
     </row>
@@ -4518,11 +4549,11 @@
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
       <c r="D261" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E261" s="1"/>
       <c r="F261" s="1" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="G261" s="1"/>
     </row>
@@ -4530,44 +4561,46 @@
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
       <c r="D262" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E262" s="1"/>
       <c r="F262" s="1" t="s">
-        <v>233</v>
+        <v>65</v>
       </c>
       <c r="G262" s="1"/>
     </row>
     <row r="263" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
-      <c r="D263" s="1" t="s">
-        <v>160</v>
-      </c>
+      <c r="D263" s="1"/>
       <c r="E263" s="1"/>
-      <c r="F263" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="F263" s="1"/>
       <c r="G263" s="1"/>
     </row>
     <row r="264" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B264" s="1"/>
-      <c r="C264" s="1"/>
-      <c r="D264" s="1"/>
-      <c r="E264" s="1"/>
-      <c r="F264" s="1"/>
+      <c r="C264" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G264" s="1"/>
     </row>
     <row r="265" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B265" s="1"/>
-      <c r="C265" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C265" s="1"/>
       <c r="D265" s="1" t="s">
-        <v>2</v>
+        <v>243</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F265" s="1" t="s">
         <v>235</v>
@@ -4578,13 +4611,11 @@
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
       <c r="D266" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E266" s="1"/>
       <c r="F266" s="1" t="s">
-        <v>231</v>
+        <v>171</v>
       </c>
       <c r="G266" s="1"/>
     </row>
@@ -4592,11 +4623,11 @@
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
       <c r="D267" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E267" s="1"/>
       <c r="F267" s="1" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
       <c r="G267" s="1"/>
     </row>
@@ -4604,46 +4635,108 @@
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
       <c r="D268" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E268" s="1"/>
       <c r="F268" s="1" t="s">
-        <v>233</v>
+        <v>65</v>
       </c>
       <c r="G268" s="1"/>
     </row>
     <row r="269" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
-      <c r="D269" s="1" t="s">
-        <v>163</v>
-      </c>
+      <c r="D269" s="1"/>
       <c r="E269" s="1"/>
-      <c r="F269" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="F269" s="1"/>
       <c r="G269" s="1"/>
     </row>
     <row r="270" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B270" s="1"/>
-      <c r="C270" s="1"/>
+      <c r="C270" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="D270" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F270" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G270" s="1"/>
+    </row>
+    <row r="271" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B271" s="1"/>
+      <c r="C271" s="1"/>
+      <c r="D271" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F271" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G271" s="1"/>
+    </row>
+    <row r="272" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B272" s="1"/>
+      <c r="C272" s="1"/>
+      <c r="D272" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E272" s="1"/>
+      <c r="F272" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G272" s="1"/>
+    </row>
+    <row r="273" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B273" s="1"/>
+      <c r="C273" s="1"/>
+      <c r="D273" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E273" s="1"/>
+      <c r="F273" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G273" s="1"/>
+    </row>
+    <row r="274" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B274" s="1"/>
+      <c r="C274" s="1"/>
+      <c r="D274" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E274" s="1"/>
+      <c r="F274" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G274" s="1"/>
+    </row>
+    <row r="275" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B275" s="1"/>
+      <c r="C275" s="1"/>
+      <c r="D275" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E270" s="1"/>
-      <c r="F270" s="1" t="s">
+      <c r="E275" s="1"/>
+      <c r="F275" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G270" s="1"/>
-    </row>
-    <row r="272" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B272" t="s">
+      <c r="G275" s="1"/>
+    </row>
+    <row r="277" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
         <v>165</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="E108:E111"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
additional table and change of fields
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.beta.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,14 +11,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$274</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$277</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="276">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -128,12 +128,6 @@
     <t>convert_unit_id_2</t>
   </si>
   <si>
-    <t>MASTER TAG</t>
-  </si>
-  <si>
-    <t>tags_name</t>
-  </si>
-  <si>
     <t>purchase_datetime</t>
   </si>
   <si>
@@ -272,15 +266,9 @@
     <t>unit_description</t>
   </si>
   <si>
-    <t>tags_desctiption</t>
-  </si>
-  <si>
     <t>unit_active</t>
   </si>
   <si>
-    <t>tags_active</t>
-  </si>
-  <si>
     <t>purchase_invoice</t>
   </si>
   <si>
@@ -840,6 +828,24 @@
   </si>
   <si>
     <t>msg_read_user_id</t>
+  </si>
+  <si>
+    <t>PRODUCT CATEGORY</t>
+  </si>
+  <si>
+    <t>MASTER CATEGORY</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>category_desctiption</t>
+  </si>
+  <si>
+    <t>category_active</t>
   </si>
 </sst>
 </file>
@@ -972,7 +978,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1007,7 +1013,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1219,10 +1225,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q277"/>
+  <dimension ref="B1:Q280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="F176" sqref="F176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1242,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1263,13 +1269,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1280,7 +1286,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1288,11 +1294,11 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1300,34 +1306,34 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H6" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1340,7 +1346,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1351,16 +1357,16 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1368,13 +1374,13 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1382,11 +1388,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1394,11 +1400,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1406,11 +1412,11 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1418,11 +1424,11 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1430,13 +1436,13 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1444,14 +1450,14 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -1464,7 +1470,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1475,16 +1481,16 @@
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1498,7 +1504,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1506,11 +1512,11 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1518,11 +1524,11 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1530,28 +1536,28 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -1581,26 +1587,26 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1608,13 +1614,13 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1626,7 +1632,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1634,35 +1640,35 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N32">
         <v>1</v>
       </c>
       <c r="P32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1676,7 +1682,7 @@
         <v>5</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -1688,7 +1694,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="N35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="P35">
         <v>1</v>
@@ -1706,14 +1712,14 @@
         <v>4</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G36" s="1"/>
       <c r="N36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P36">
         <v>2</v>
@@ -1726,15 +1732,15 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G37" s="1"/>
       <c r="N37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P37">
         <v>3</v>
@@ -1744,26 +1750,26 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1784,16 +1790,16 @@
         <v>2</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="N41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.25">
@@ -1806,7 +1812,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -1820,24 +1826,24 @@
         <v>5</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -1852,32 +1858,32 @@
     <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -1891,7 +1897,7 @@
         <v>5</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -1899,13 +1905,13 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -1913,11 +1919,11 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -1925,11 +1931,11 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G51" s="1"/>
     </row>
@@ -1937,11 +1943,11 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -1949,13 +1955,13 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -1970,31 +1976,31 @@
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -2009,16 +2015,16 @@
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -2026,13 +2032,13 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2040,11 +2046,11 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2052,31 +2058,31 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K61" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2107,10 +2113,10 @@
         <v>14</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -2122,7 +2128,7 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -2130,11 +2136,11 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G67" s="1"/>
     </row>
@@ -2142,11 +2148,11 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G68" s="1"/>
     </row>
@@ -2154,11 +2160,11 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G69" s="1"/>
     </row>
@@ -2170,7 +2176,7 @@
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G70" s="1"/>
     </row>
@@ -2182,7 +2188,7 @@
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G71" s="1"/>
     </row>
@@ -2194,7 +2200,7 @@
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G72" s="1"/>
     </row>
@@ -2202,11 +2208,11 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G73" s="1"/>
     </row>
@@ -2214,11 +2220,11 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2226,35 +2232,35 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2268,10 +2274,10 @@
         <v>14</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G78" s="1"/>
     </row>
@@ -2279,13 +2285,13 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G79" s="1"/>
     </row>
@@ -2293,11 +2299,11 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G80" s="1"/>
     </row>
@@ -2305,11 +2311,11 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G81" s="1"/>
     </row>
@@ -2317,11 +2323,11 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -2329,11 +2335,11 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G83" s="1"/>
     </row>
@@ -2341,11 +2347,11 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G84" s="1"/>
     </row>
@@ -2376,13 +2382,13 @@
         <v>21</v>
       </c>
       <c r="E87" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G87" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
@@ -2393,7 +2399,7 @@
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G88" s="1"/>
     </row>
@@ -2401,11 +2407,11 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G89" s="1"/>
     </row>
@@ -2413,11 +2419,11 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G90" s="1"/>
     </row>
@@ -2425,11 +2431,11 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G91" s="1"/>
     </row>
@@ -2441,7 +2447,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -2453,7 +2459,7 @@
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G93" s="1"/>
     </row>
@@ -2465,7 +2471,7 @@
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G94" s="1"/>
     </row>
@@ -2473,11 +2479,11 @@
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G95" s="1"/>
     </row>
@@ -2491,7 +2497,7 @@
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -2502,32 +2508,32 @@
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E98" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G98" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G99" s="1"/>
     </row>
@@ -2535,13 +2541,13 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G100" s="1"/>
     </row>
@@ -2549,11 +2555,11 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G101" s="1"/>
     </row>
@@ -2561,11 +2567,11 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G102" s="1"/>
     </row>
@@ -2573,83 +2579,83 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G108" s="1"/>
     </row>
@@ -2657,11 +2663,11 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G109" s="1"/>
     </row>
@@ -2669,11 +2675,11 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G110" s="1"/>
     </row>
@@ -2681,11 +2687,11 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G111" s="1"/>
     </row>
@@ -2699,7 +2705,7 @@
         <v>5</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G112" s="1"/>
     </row>
@@ -2713,7 +2719,7 @@
         <v>5</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G113" s="1"/>
     </row>
@@ -2721,13 +2727,13 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G114" s="1"/>
     </row>
@@ -2735,11 +2741,11 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G115" s="1"/>
     </row>
@@ -2747,11 +2753,11 @@
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G116" s="1"/>
     </row>
@@ -2759,25 +2765,25 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G118" s="1"/>
     </row>
@@ -2785,39 +2791,39 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
+      <c r="E120" s="3"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
-        <v>112</v>
+        <v>270</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="G121" s="1"/>
     </row>
@@ -2825,114 +2831,114 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>77</v>
+        <v>272</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
-      <c r="D123" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="D123" s="1"/>
       <c r="E123" s="1"/>
-      <c r="F123" s="1" t="s">
-        <v>232</v>
-      </c>
+      <c r="F123" s="1"/>
       <c r="G123" s="1"/>
     </row>
     <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
+      <c r="C124" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="D124" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E124" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F124" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="G124" s="1"/>
-      <c r="H124" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E125" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F125" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G125" s="1"/>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
-      <c r="D126" s="1"/>
+      <c r="D126" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
+      <c r="F126" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="G126" s="1"/>
     </row>
     <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
-      <c r="C127" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="C127" s="1"/>
       <c r="D127" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="G127" s="1"/>
+      <c r="H127" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1" t="s">
-        <v>237</v>
+        <v>30</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="G128" s="1"/>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
-      <c r="D129" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
+      <c r="C130" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D130" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E130" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F130" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G130" s="1"/>
     </row>
@@ -2940,13 +2946,11 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>235</v>
+        <v>167</v>
       </c>
       <c r="G131" s="1"/>
     </row>
@@ -2954,11 +2958,13 @@
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E132" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F132" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G132" s="1"/>
     </row>
@@ -2966,35 +2972,37 @@
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G133" s="1"/>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
-      <c r="E134" s="1"/>
-      <c r="F134" s="1"/>
+      <c r="D134" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="G134" s="1"/>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
-      <c r="C135" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G135" s="1"/>
     </row>
@@ -3002,57 +3010,59 @@
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>82</v>
+        <v>193</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="G136" s="1"/>
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
-      <c r="D137" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="D137" s="1"/>
       <c r="E137" s="1"/>
-      <c r="F137" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="F137" s="1"/>
       <c r="G137" s="1"/>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
-      <c r="C138" s="1"/>
+      <c r="C138" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="D138" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E138" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F138" s="1" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="G138" s="1"/>
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
-      <c r="D139" s="1"/>
+      <c r="D139" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="E139" s="1"/>
-      <c r="F139" s="1"/>
+      <c r="F139" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="G139" s="1"/>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
-      <c r="C140" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
-        <v>231</v>
+        <v>63</v>
       </c>
       <c r="G140" s="1"/>
     </row>
@@ -3060,47 +3070,45 @@
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="G141" s="1"/>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
-      <c r="D142" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="D142" s="1"/>
       <c r="E142" s="1"/>
-      <c r="F142" s="1" t="s">
-        <v>232</v>
-      </c>
+      <c r="F142" s="1"/>
       <c r="G142" s="1"/>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" s="1"/>
-      <c r="C143" s="1"/>
-      <c r="D143" s="1"/>
+      <c r="C143" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E143" s="1"/>
-      <c r="F143" s="1"/>
+      <c r="F143" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="G143" s="1"/>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" s="1"/>
-      <c r="C144" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="C144" s="1"/>
       <c r="D144" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="G144" s="1"/>
     </row>
@@ -3108,59 +3116,59 @@
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="G145" s="1"/>
     </row>
     <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
-      <c r="D146" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="D146" s="1"/>
       <c r="E146" s="1"/>
-      <c r="F146" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="F146" s="1"/>
       <c r="G146" s="1"/>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
-      <c r="C147" s="1"/>
+      <c r="C147" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="D147" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E147" s="1"/>
+        <v>272</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F147" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G147" s="1"/>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
+      <c r="D148" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="E148" s="1"/>
-      <c r="F148" s="1"/>
+      <c r="F148" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="G148" s="1"/>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" s="1"/>
-      <c r="C149" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
-        <v>235</v>
+        <v>63</v>
       </c>
       <c r="G149" s="1"/>
     </row>
@@ -3168,37 +3176,35 @@
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>87</v>
+        <v>275</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>64</v>
+        <v>205</v>
       </c>
       <c r="G150" s="1"/>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
-      <c r="D151" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>231</v>
-      </c>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
       <c r="G151" s="1"/>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
+      <c r="C152" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D152" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E152" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F152" s="1" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="G152" s="1"/>
     </row>
@@ -3206,11 +3212,11 @@
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1" t="s">
-        <v>233</v>
+        <v>62</v>
       </c>
       <c r="G153" s="1"/>
     </row>
@@ -3218,11 +3224,13 @@
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E154" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F154" s="1" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="G154" s="1"/>
     </row>
@@ -3230,11 +3238,11 @@
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1" t="s">
-        <v>201</v>
+        <v>36</v>
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="G155" s="1"/>
     </row>
@@ -3242,35 +3250,35 @@
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="G156" s="1"/>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
+      <c r="D157" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
+      <c r="F157" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="G157" s="1"/>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
-      <c r="C158" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
-        <v>235</v>
+        <v>167</v>
       </c>
       <c r="G158" s="1"/>
     </row>
@@ -3278,37 +3286,35 @@
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="G159" s="1"/>
     </row>
     <row r="160" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
-      <c r="D160" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="D160" s="1"/>
       <c r="E160" s="1"/>
-      <c r="F160" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F160" s="1"/>
       <c r="G160" s="1"/>
     </row>
     <row r="161" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B161" s="1"/>
-      <c r="C161" s="1"/>
+      <c r="C161" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D161" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E161" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F161" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G161" s="1"/>
     </row>
@@ -3316,35 +3322,37 @@
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E162" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F162" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G162" s="1"/>
     </row>
     <row r="163" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
-      <c r="D163" s="1"/>
+      <c r="D163" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="E163" s="1"/>
-      <c r="F163" s="1"/>
+      <c r="F163" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="G163" s="1"/>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" s="1"/>
-      <c r="C164" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="C164" s="1"/>
       <c r="D164" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E164" s="1"/>
       <c r="F164" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G164" s="1"/>
     </row>
@@ -3352,37 +3360,35 @@
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E165" s="1"/>
       <c r="F165" s="1" t="s">
-        <v>64</v>
+        <v>229</v>
       </c>
       <c r="G165" s="1"/>
     </row>
     <row r="166" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
-      <c r="D166" s="1" t="s">
-        <v>239</v>
-      </c>
+      <c r="D166" s="1"/>
       <c r="E166" s="1"/>
-      <c r="F166" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="F166" s="1"/>
       <c r="G166" s="1"/>
     </row>
     <row r="167" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B167" s="1"/>
-      <c r="C167" s="1"/>
+      <c r="C167" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="D167" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E167" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F167" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G167" s="1"/>
     </row>
@@ -3390,11 +3396,13 @@
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E168" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F168" s="1" t="s">
-        <v>171</v>
+        <v>62</v>
       </c>
       <c r="G168" s="1"/>
     </row>
@@ -3402,11 +3410,11 @@
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1" t="s">
-        <v>101</v>
+        <v>235</v>
       </c>
       <c r="E169" s="1"/>
       <c r="F169" s="1" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="G169" s="1"/>
     </row>
@@ -3414,11 +3422,11 @@
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1" t="s">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="G170" s="1"/>
     </row>
@@ -3426,35 +3434,35 @@
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E171" s="1"/>
       <c r="F171" s="1" t="s">
-        <v>209</v>
+        <v>167</v>
       </c>
       <c r="G171" s="1"/>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
-      <c r="D172" s="1"/>
+      <c r="D172" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="E172" s="1"/>
-      <c r="F172" s="1"/>
+      <c r="F172" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="G172" s="1"/>
     </row>
     <row r="173" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B173" s="1"/>
-      <c r="C173" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="C173" s="1"/>
       <c r="D173" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E173" s="1"/>
       <c r="F173" s="1" t="s">
-        <v>235</v>
+        <v>167</v>
       </c>
       <c r="G173" s="1"/>
     </row>
@@ -3462,37 +3470,35 @@
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="E174" s="1"/>
       <c r="F174" s="1" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="G174" s="1"/>
     </row>
     <row r="175" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
-      <c r="D175" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="D175" s="1"/>
       <c r="E175" s="1"/>
-      <c r="F175" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F175" s="1"/>
       <c r="G175" s="1"/>
     </row>
     <row r="176" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B176" s="1"/>
-      <c r="C176" s="1"/>
+      <c r="C176" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D176" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E176" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F176" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G176" s="1"/>
     </row>
@@ -3500,11 +3506,13 @@
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E177" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F177" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G177" s="1"/>
     </row>
@@ -3512,60 +3520,56 @@
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E178" s="1"/>
       <c r="F178" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G178" s="1"/>
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
-      <c r="D179" s="1"/>
+      <c r="D179" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="E179" s="1"/>
-      <c r="F179" s="1"/>
+      <c r="F179" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="G179" s="1"/>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B180" s="1"/>
-      <c r="C180" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="C180" s="1"/>
       <c r="D180" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E180" s="1"/>
       <c r="F180" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G180" s="1"/>
     </row>
     <row r="181" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
-      <c r="D181" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
       <c r="G181" s="1"/>
     </row>
     <row r="182" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B182" s="1"/>
-      <c r="C182" s="1"/>
+      <c r="C182" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="D182" s="1" t="s">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>231</v>
@@ -3576,11 +3580,13 @@
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E183" s="1"/>
+        <v>149</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F183" s="1" t="s">
-        <v>171</v>
+        <v>62</v>
       </c>
       <c r="G183" s="1"/>
     </row>
@@ -3588,11 +3594,13 @@
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E184" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F184" s="1" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="G184" s="1"/>
     </row>
@@ -3600,61 +3608,61 @@
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E185" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F185" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G185" s="1"/>
     </row>
     <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
-      <c r="D186" s="1"/>
+      <c r="D186" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="E186" s="1"/>
-      <c r="F186" s="1"/>
+      <c r="F186" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="G186" s="1"/>
     </row>
     <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B187" s="1"/>
-      <c r="C187" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="C187" s="1"/>
       <c r="D187" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E187" s="1"/>
       <c r="F187" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G187" s="1"/>
     </row>
     <row r="188" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
-      <c r="D188" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="D188" s="1"/>
+      <c r="E188" s="1"/>
+      <c r="F188" s="1"/>
       <c r="G188" s="1"/>
     </row>
     <row r="189" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B189" s="1"/>
-      <c r="C189" s="1"/>
+      <c r="C189" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="D189" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E189" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F189" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G189" s="1"/>
     </row>
@@ -3662,11 +3670,13 @@
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E190" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F190" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G190" s="1"/>
     </row>
@@ -3674,11 +3684,11 @@
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="G191" s="1"/>
     </row>
@@ -3686,49 +3696,47 @@
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E192" s="1"/>
       <c r="F192" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G192" s="1"/>
     </row>
     <row r="193" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
-      <c r="D193" s="1"/>
+      <c r="D193" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="E193" s="1"/>
-      <c r="F193" s="1"/>
+      <c r="F193" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="G193" s="1"/>
     </row>
     <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194" s="1"/>
-      <c r="C194" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D194" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F194" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="C194" s="1"/>
+      <c r="D194" s="1"/>
+      <c r="E194" s="1"/>
+      <c r="F194" s="1"/>
       <c r="G194" s="1"/>
     </row>
     <row r="195" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B195" s="1"/>
-      <c r="C195" s="1"/>
+      <c r="C195" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="D195" s="1" t="s">
-        <v>137</v>
+        <v>2</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>64</v>
+        <v>231</v>
       </c>
       <c r="G195" s="1"/>
     </row>
@@ -3736,13 +3744,13 @@
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>231</v>
+        <v>62</v>
       </c>
       <c r="G196" s="1"/>
     </row>
@@ -3750,11 +3758,13 @@
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E197" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F197" s="1" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="G197" s="1"/>
     </row>
@@ -3762,11 +3772,11 @@
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="E198" s="1"/>
       <c r="F198" s="1" t="s">
-        <v>233</v>
+        <v>167</v>
       </c>
       <c r="G198" s="1"/>
     </row>
@@ -3774,11 +3784,11 @@
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G199" s="1"/>
     </row>
@@ -3786,59 +3796,61 @@
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G200" s="1"/>
     </row>
     <row r="201" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
-      <c r="D201" s="1" t="s">
-        <v>142</v>
-      </c>
+      <c r="D201" s="1"/>
       <c r="E201" s="1"/>
-      <c r="F201" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="F201" s="1"/>
       <c r="G201" s="1"/>
     </row>
     <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202" s="1"/>
-      <c r="C202" s="1"/>
+      <c r="C202" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="D202" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E202" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F202" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G202" s="1"/>
     </row>
     <row r="203" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
-      <c r="D203" s="1"/>
-      <c r="E203" s="1"/>
-      <c r="F203" s="1"/>
+      <c r="D203" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="G203" s="1"/>
     </row>
     <row r="204" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B204" s="1"/>
-      <c r="C204" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="E204" s="1"/>
       <c r="F204" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G204" s="1"/>
     </row>
@@ -3846,13 +3858,11 @@
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E205" s="1"/>
       <c r="F205" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G205" s="1"/>
     </row>
@@ -3860,11 +3870,11 @@
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="E206" s="1"/>
       <c r="F206" s="1" t="s">
-        <v>233</v>
+        <v>63</v>
       </c>
       <c r="G206" s="1"/>
     </row>
@@ -3876,31 +3886,31 @@
       </c>
       <c r="E207" s="1"/>
       <c r="F207" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G207" s="1"/>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
-      <c r="D208" s="1" t="s">
-        <v>202</v>
-      </c>
+      <c r="D208" s="1"/>
       <c r="E208" s="1"/>
-      <c r="F208" s="1" t="s">
-        <v>234</v>
-      </c>
+      <c r="F208" s="1"/>
       <c r="G208" s="1"/>
     </row>
     <row r="209" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B209" s="1"/>
-      <c r="C209" s="1"/>
+      <c r="C209" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="D209" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E209" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F209" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G209" s="1"/>
     </row>
@@ -3908,11 +3918,13 @@
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E210" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F210" s="1" t="s">
-        <v>233</v>
+        <v>62</v>
       </c>
       <c r="G210" s="1"/>
     </row>
@@ -3920,35 +3932,37 @@
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E211" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F211" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G211" s="1"/>
     </row>
     <row r="212" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
-      <c r="D212" s="1"/>
+      <c r="D212" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="E212" s="1"/>
-      <c r="F212" s="1"/>
+      <c r="F212" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="G212" s="1"/>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B213" s="1"/>
-      <c r="C213" s="1" t="s">
-        <v>125</v>
-      </c>
+      <c r="C213" s="1"/>
       <c r="D213" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="E213" s="1"/>
       <c r="F213" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G213" s="1"/>
     </row>
@@ -3956,13 +3970,11 @@
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="E214" s="1"/>
       <c r="F214" s="1" t="s">
-        <v>64</v>
+        <v>229</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -3970,13 +3982,11 @@
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E215" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="E215" s="1"/>
       <c r="F215" s="1" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="G215" s="1"/>
     </row>
@@ -3984,11 +3994,11 @@
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G216" s="1"/>
     </row>
@@ -3996,11 +4006,11 @@
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="G217" s="1"/>
     </row>
@@ -4015,16 +4025,16 @@
     <row r="219" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B219" s="1"/>
       <c r="C219" s="1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E219" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G219" s="1"/>
     </row>
@@ -4032,13 +4042,13 @@
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G220" s="1"/>
     </row>
@@ -4046,11 +4056,11 @@
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E221" s="1"/>
       <c r="F221" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G221" s="1"/>
     </row>
@@ -4058,11 +4068,11 @@
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1" t="s">
-        <v>202</v>
+        <v>113</v>
       </c>
       <c r="E222" s="1"/>
       <c r="F222" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G222" s="1"/>
     </row>
@@ -4070,11 +4080,11 @@
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E223" s="1"/>
       <c r="F223" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G223" s="1"/>
     </row>
@@ -4082,11 +4092,11 @@
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G224" s="1"/>
     </row>
@@ -4094,11 +4104,11 @@
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1" t="s">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="E225" s="1"/>
       <c r="F225" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G225" s="1"/>
     </row>
@@ -4106,47 +4116,49 @@
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="E226" s="1"/>
       <c r="F226" s="1" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="G226" s="1"/>
     </row>
     <row r="227" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
-      <c r="D227" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="D227" s="1"/>
       <c r="E227" s="1"/>
-      <c r="F227" s="1" t="s">
-        <v>233</v>
-      </c>
+      <c r="F227" s="1"/>
       <c r="G227" s="1"/>
     </row>
     <row r="228" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B228" s="1"/>
-      <c r="C228" s="1"/>
-      <c r="D228" s="1"/>
-      <c r="E228" s="1"/>
-      <c r="F228" s="1"/>
+      <c r="C228" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F228" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="G228" s="1"/>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B229" s="1"/>
-      <c r="C229" s="1" t="s">
-        <v>206</v>
-      </c>
+      <c r="C229" s="1"/>
       <c r="D229" s="1" t="s">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>235</v>
+        <v>62</v>
       </c>
       <c r="G229" s="1"/>
     </row>
@@ -4154,13 +4166,13 @@
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
       <c r="D230" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G230" s="1"/>
     </row>
@@ -4168,13 +4180,11 @@
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E231" s="1"/>
       <c r="F231" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G231" s="1"/>
     </row>
@@ -4182,11 +4192,11 @@
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
       <c r="D232" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E232" s="1"/>
       <c r="F232" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G232" s="1"/>
     </row>
@@ -4201,16 +4211,16 @@
     <row r="234" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B234" s="1"/>
       <c r="C234" s="1" t="s">
-        <v>207</v>
+        <v>122</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E234" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G234" s="1"/>
     </row>
@@ -4218,13 +4228,13 @@
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
       <c r="D235" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E235" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G235" s="1"/>
     </row>
@@ -4232,11 +4242,11 @@
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
       <c r="D236" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E236" s="1"/>
       <c r="F236" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G236" s="1"/>
     </row>
@@ -4244,11 +4254,11 @@
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
       <c r="D237" s="1" t="s">
-        <v>117</v>
+        <v>198</v>
       </c>
       <c r="E237" s="1"/>
       <c r="F237" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G237" s="1"/>
     </row>
@@ -4256,11 +4266,11 @@
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1" t="s">
-        <v>131</v>
+        <v>199</v>
       </c>
       <c r="E238" s="1"/>
       <c r="F238" s="1" t="s">
-        <v>65</v>
+        <v>230</v>
       </c>
       <c r="G238" s="1"/>
     </row>
@@ -4268,440 +4278,432 @@
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="E239" s="1"/>
       <c r="F239" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G239" s="1"/>
     </row>
     <row r="240" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
-      <c r="D240" s="1"/>
+      <c r="D240" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="E240" s="1"/>
-      <c r="F240" s="1"/>
+      <c r="F240" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="G240" s="1"/>
     </row>
-    <row r="241" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B241" s="1"/>
-      <c r="C241" s="1" t="s">
-        <v>145</v>
-      </c>
+      <c r="C241" s="1"/>
       <c r="D241" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="E241" s="1"/>
       <c r="F241" s="1" t="s">
-        <v>235</v>
+        <v>63</v>
       </c>
       <c r="G241" s="1"/>
     </row>
-    <row r="242" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
       <c r="D242" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E242" s="1"/>
       <c r="F242" s="1" t="s">
-        <v>64</v>
+        <v>229</v>
       </c>
       <c r="G242" s="1"/>
     </row>
-    <row r="243" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
-      <c r="D243" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F243" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="D243" s="1"/>
+      <c r="E243" s="1"/>
+      <c r="F243" s="1"/>
       <c r="G243" s="1"/>
     </row>
-    <row r="244" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B244" s="1"/>
-      <c r="C244" s="1"/>
+      <c r="C244" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="D244" s="1" t="s">
-        <v>150</v>
+        <v>2</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="G244" s="1"/>
     </row>
-    <row r="245" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
       <c r="D245" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E245" s="1"/>
+        <v>237</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F245" s="1" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="G245" s="1"/>
     </row>
-    <row r="246" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
       <c r="D246" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E246" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F246" s="1" t="s">
-        <v>233</v>
+        <v>167</v>
       </c>
       <c r="G246" s="1"/>
     </row>
-    <row r="247" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
-      <c r="D247" s="1"/>
+      <c r="D247" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="E247" s="1"/>
-      <c r="F247" s="1"/>
+      <c r="F247" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="G247" s="1"/>
     </row>
-    <row r="248" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B248" s="1"/>
-      <c r="C248" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F248" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="C248" s="1"/>
+      <c r="D248" s="1"/>
+      <c r="E248" s="1"/>
+      <c r="F248" s="1"/>
       <c r="G248" s="1"/>
     </row>
-    <row r="249" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B249" s="1"/>
-      <c r="C249" s="1"/>
+      <c r="C249" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="D249" s="1" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="E249" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G249" s="1"/>
     </row>
-    <row r="250" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E250" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F250" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G250" s="1"/>
     </row>
-    <row r="251" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G251" s="1"/>
     </row>
-    <row r="252" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
       <c r="D252" s="1" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="E252" s="1"/>
       <c r="F252" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G252" s="1"/>
     </row>
-    <row r="253" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
-      <c r="D253" s="1"/>
+      <c r="D253" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="E253" s="1"/>
-      <c r="F253" s="1"/>
+      <c r="F253" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G253" s="1"/>
     </row>
-    <row r="254" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B254" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>95</v>
-      </c>
+    <row r="254" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
       <c r="D254" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E254" s="1"/>
       <c r="F254" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G254" s="1"/>
     </row>
-    <row r="255" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
-      <c r="D255" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F255" s="1" t="s">
-        <v>254</v>
-      </c>
+      <c r="D255" s="1"/>
+      <c r="E255" s="1"/>
+      <c r="F255" s="1"/>
       <c r="G255" s="1"/>
-      <c r="H255" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="256" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="256" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
-      <c r="D256" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="D256" s="1"/>
       <c r="E256" s="1"/>
-      <c r="F256" s="1" t="s">
-        <v>247</v>
-      </c>
+      <c r="F256" s="1"/>
       <c r="G256" s="1"/>
     </row>
-    <row r="257" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B257" s="1"/>
-      <c r="C257" s="1"/>
-      <c r="D257" s="1"/>
-      <c r="E257" s="1"/>
-      <c r="F257" s="1"/>
+    <row r="257" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B257" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="G257" s="1"/>
     </row>
-    <row r="258" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B258" s="1"/>
-      <c r="C258" s="1" t="s">
-        <v>108</v>
-      </c>
+      <c r="C258" s="1"/>
       <c r="D258" s="1" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F258" s="1" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="G258" s="1"/>
-    </row>
-    <row r="259" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H258" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="259" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B259" s="1"/>
       <c r="C259" s="1"/>
       <c r="D259" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="E259" s="1"/>
       <c r="F259" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="G259" s="1"/>
     </row>
-    <row r="260" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
-      <c r="D260" s="1" t="s">
-        <v>155</v>
-      </c>
+      <c r="D260" s="1"/>
       <c r="E260" s="1"/>
-      <c r="F260" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="F260" s="1"/>
       <c r="G260" s="1"/>
     </row>
-    <row r="261" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
+      <c r="C261" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="D261" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E261" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F261" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G261" s="1"/>
     </row>
-    <row r="262" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
       <c r="D262" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E262" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F262" s="1" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="G262" s="1"/>
     </row>
-    <row r="263" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
-      <c r="D263" s="1"/>
+      <c r="D263" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="E263" s="1"/>
-      <c r="F263" s="1"/>
+      <c r="F263" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="G263" s="1"/>
     </row>
-    <row r="264" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B264" s="1"/>
-      <c r="C264" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="C264" s="1"/>
       <c r="D264" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E264" s="1"/>
       <c r="F264" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G264" s="1"/>
     </row>
-    <row r="265" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
       <c r="D265" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="E265" s="1"/>
       <c r="F265" s="1" t="s">
-        <v>235</v>
+        <v>63</v>
       </c>
       <c r="G265" s="1"/>
     </row>
-    <row r="266" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
-      <c r="D266" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="D266" s="1"/>
       <c r="E266" s="1"/>
-      <c r="F266" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="F266" s="1"/>
       <c r="G266" s="1"/>
     </row>
-    <row r="267" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B267" s="1"/>
-      <c r="C267" s="1"/>
+      <c r="C267" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="D267" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E267" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F267" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G267" s="1"/>
     </row>
-    <row r="268" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
       <c r="D268" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E268" s="1"/>
+        <v>239</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F268" s="1" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="G268" s="1"/>
     </row>
-    <row r="269" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
-      <c r="D269" s="1"/>
+      <c r="D269" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="E269" s="1"/>
-      <c r="F269" s="1"/>
+      <c r="F269" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="G269" s="1"/>
     </row>
-    <row r="270" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B270" s="1"/>
-      <c r="C270" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C270" s="1"/>
       <c r="D270" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>54</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="E270" s="1"/>
       <c r="F270" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="G270" s="1"/>
     </row>
-    <row r="271" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B271" s="1"/>
       <c r="C271" s="1"/>
       <c r="D271" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="E271" s="1"/>
       <c r="F271" s="1" t="s">
-        <v>231</v>
+        <v>63</v>
       </c>
       <c r="G271" s="1"/>
     </row>
-    <row r="272" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B272" s="1"/>
       <c r="C272" s="1"/>
-      <c r="D272" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D272" s="1"/>
       <c r="E272" s="1"/>
-      <c r="F272" s="1" t="s">
-        <v>171</v>
-      </c>
+      <c r="F272" s="1"/>
       <c r="G272" s="1"/>
     </row>
     <row r="273" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B273" s="1"/>
-      <c r="C273" s="1"/>
+      <c r="C273" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="D273" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E273" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F273" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G273" s="1"/>
     </row>
@@ -4709,11 +4711,13 @@
       <c r="B274" s="1"/>
       <c r="C274" s="1"/>
       <c r="D274" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E274" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F274" s="1" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="G274" s="1"/>
     </row>
@@ -4721,17 +4725,53 @@
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
       <c r="D275" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E275" s="1"/>
       <c r="F275" s="1" t="s">
-        <v>65</v>
+        <v>167</v>
       </c>
       <c r="G275" s="1"/>
     </row>
+    <row r="276" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B276" s="1"/>
+      <c r="C276" s="1"/>
+      <c r="D276" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E276" s="1"/>
+      <c r="F276" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G276" s="1"/>
+    </row>
     <row r="277" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B277" t="s">
-        <v>165</v>
+      <c r="B277" s="1"/>
+      <c r="C277" s="1"/>
+      <c r="D277" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E277" s="1"/>
+      <c r="F277" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G277" s="1"/>
+    </row>
+    <row r="278" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B278" s="1"/>
+      <c r="C278" s="1"/>
+      <c r="D278" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E278" s="1"/>
+      <c r="F278" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G278" s="1"/>
+    </row>
+    <row r="280" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B280" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4755,21 +4795,21 @@
   <sheetData>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
         <v>47</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>48</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -4783,7 +4823,7 @@
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11">
         <v>0</v>

</xml_diff>

<commit_message>
Finance Tables Design Changes
5 new tables
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.beta.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,14 +11,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$302</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$306</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="304">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -473,15 +473,9 @@
     <t>rp_processed</t>
   </si>
   <si>
-    <t>debt_datetime</t>
-  </si>
-  <si>
     <t>debt_nominal</t>
   </si>
   <si>
-    <t>credit_datetime</t>
-  </si>
-  <si>
     <t>credit_nominal</t>
   </si>
   <si>
@@ -491,18 +485,6 @@
     <t>credit_description</t>
   </si>
   <si>
-    <t>dj_datetime</t>
-  </si>
-  <si>
-    <t>dj_nominal</t>
-  </si>
-  <si>
-    <t>dj_branch_id</t>
-  </si>
-  <si>
-    <t>dj_description</t>
-  </si>
-  <si>
     <t>TAX</t>
   </si>
   <si>
@@ -894,6 +876,60 @@
   </si>
   <si>
     <t>tinyint unsigned</t>
+  </si>
+  <si>
+    <t>debt_id</t>
+  </si>
+  <si>
+    <t>debt_pay_method</t>
+  </si>
+  <si>
+    <t>credit_id</t>
+  </si>
+  <si>
+    <t>debt_date_begin</t>
+  </si>
+  <si>
+    <t>debt_date_end</t>
+  </si>
+  <si>
+    <t>credit_date_begin</t>
+  </si>
+  <si>
+    <t>credit_date_end</t>
+  </si>
+  <si>
+    <t>pm_name</t>
+  </si>
+  <si>
+    <t>not null</t>
+  </si>
+  <si>
+    <t>credit_pay_id</t>
+  </si>
+  <si>
+    <t>journal_id</t>
+  </si>
+  <si>
+    <t>journal_datetime</t>
+  </si>
+  <si>
+    <t>journal_nominal</t>
+  </si>
+  <si>
+    <t>journal_branch_id</t>
+  </si>
+  <si>
+    <t>journal_description</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>pm_description</t>
+  </si>
+  <si>
+    <t>PAYMENT METHOD</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1062,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1061,7 +1097,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1273,10 +1309,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q305"/>
+  <dimension ref="B1:Q316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="C309" sqref="C309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1326,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1320,7 +1356,7 @@
         <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>54</v>
@@ -1334,7 +1370,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1358,13 +1394,13 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1375,10 +1411,10 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="H7" t="s">
         <v>64</v>
@@ -1414,7 +1450,7 @@
         <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1425,10 +1461,10 @@
         <v>88</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1436,11 +1472,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1448,11 +1484,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1460,11 +1496,11 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1476,7 +1512,7 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1484,13 +1520,13 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1498,14 +1534,14 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -1518,7 +1554,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1529,7 +1565,7 @@
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
@@ -1538,7 +1574,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1552,7 +1588,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1560,11 +1596,11 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1572,11 +1608,11 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1584,28 +1620,28 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -1638,7 +1674,7 @@
         <v>52</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>54</v>
@@ -1654,7 +1690,7 @@
         <v>61</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1662,13 +1698,13 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1680,7 +1716,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1692,7 +1728,7 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
@@ -1716,7 +1752,7 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1730,7 +1766,7 @@
         <v>5</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -1763,7 +1799,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G36" s="1"/>
       <c r="N36" t="s">
@@ -1784,7 +1820,7 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G37" s="1"/>
       <c r="N37" t="s">
@@ -1817,7 +1853,7 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1841,7 +1877,7 @@
         <v>52</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>54</v>
@@ -1860,7 +1896,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -1874,11 +1910,11 @@
         <v>5</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
@@ -1891,7 +1927,7 @@
         <v>57</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -1915,7 +1951,7 @@
         <v>52</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>54</v>
@@ -1931,7 +1967,7 @@
         <v>5</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -1945,7 +1981,7 @@
         <v>5</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -1959,7 +1995,7 @@
         <v>5</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -1967,11 +2003,11 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -1991,11 +2027,11 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -2003,13 +2039,13 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -2024,7 +2060,7 @@
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>2</v>
@@ -2033,22 +2069,22 @@
         <v>52</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -2063,7 +2099,7 @@
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>2</v>
@@ -2072,7 +2108,7 @@
         <v>52</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -2086,7 +2122,7 @@
         <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2094,11 +2130,11 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2112,25 +2148,25 @@
         <v>5</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="K61" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2164,7 +2200,7 @@
         <v>52</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -2176,7 +2212,7 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -2184,11 +2220,11 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G67" s="1"/>
     </row>
@@ -2196,11 +2232,11 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G68" s="1"/>
     </row>
@@ -2208,11 +2244,11 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G69" s="1"/>
     </row>
@@ -2224,7 +2260,7 @@
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G70" s="1"/>
     </row>
@@ -2236,7 +2272,7 @@
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G71" s="1"/>
     </row>
@@ -2248,7 +2284,7 @@
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G72" s="1"/>
     </row>
@@ -2260,7 +2296,7 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G73" s="1"/>
     </row>
@@ -2268,11 +2304,11 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2280,35 +2316,35 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2325,7 +2361,7 @@
         <v>52</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G78" s="1"/>
     </row>
@@ -2339,7 +2375,7 @@
         <v>5</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G79" s="1"/>
     </row>
@@ -2347,11 +2383,11 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G80" s="1"/>
     </row>
@@ -2359,11 +2395,11 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G81" s="1"/>
     </row>
@@ -2371,11 +2407,11 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -2383,11 +2419,11 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G83" s="1"/>
     </row>
@@ -2395,11 +2431,11 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G84" s="1"/>
     </row>
@@ -2433,7 +2469,7 @@
         <v>52</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>54</v>
@@ -2447,7 +2483,7 @@
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G88" s="1"/>
     </row>
@@ -2455,11 +2491,11 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G89" s="1"/>
     </row>
@@ -2467,11 +2503,11 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G90" s="1"/>
     </row>
@@ -2479,11 +2515,11 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G91" s="1"/>
     </row>
@@ -2495,7 +2531,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -2507,7 +2543,7 @@
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G93" s="1"/>
     </row>
@@ -2519,7 +2555,7 @@
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G94" s="1"/>
     </row>
@@ -2531,7 +2567,7 @@
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G95" s="1"/>
     </row>
@@ -2556,7 +2592,7 @@
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>2</v>
@@ -2565,7 +2601,7 @@
         <v>52</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>54</v>
@@ -2581,7 +2617,7 @@
         <v>61</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G99" s="1"/>
     </row>
@@ -2589,13 +2625,13 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G100" s="1"/>
     </row>
@@ -2603,11 +2639,11 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G101" s="1"/>
     </row>
@@ -2615,7 +2651,7 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
@@ -2627,11 +2663,11 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>76</v>
@@ -2641,69 +2677,69 @@
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G108" s="1"/>
     </row>
@@ -2711,11 +2747,11 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G109" s="1"/>
     </row>
@@ -2723,11 +2759,11 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G110" s="1"/>
     </row>
@@ -2735,11 +2771,11 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G111" s="1"/>
     </row>
@@ -2753,7 +2789,7 @@
         <v>5</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G112" s="1"/>
     </row>
@@ -2767,7 +2803,7 @@
         <v>5</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G113" s="1"/>
     </row>
@@ -2775,13 +2811,13 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G114" s="1"/>
     </row>
@@ -2789,11 +2825,11 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G115" s="1"/>
     </row>
@@ -2801,11 +2837,11 @@
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G116" s="1"/>
     </row>
@@ -2813,25 +2849,25 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G118" s="1"/>
     </row>
@@ -2839,16 +2875,16 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
@@ -2862,7 +2898,7 @@
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>79</v>
@@ -2871,7 +2907,7 @@
         <v>52</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G121" s="1"/>
     </row>
@@ -2879,13 +2915,13 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G122" s="1"/>
     </row>
@@ -2909,7 +2945,7 @@
         <v>52</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G124" s="1"/>
     </row>
@@ -2923,7 +2959,7 @@
         <v>5</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G125" s="1"/>
     </row>
@@ -2935,7 +2971,7 @@
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G126" s="1"/>
     </row>
@@ -2947,7 +2983,7 @@
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" t="s">
@@ -2962,7 +2998,7 @@
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G128" s="1"/>
     </row>
@@ -2977,7 +3013,7 @@
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>2</v>
@@ -2986,7 +3022,7 @@
         <v>52</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G130" s="1"/>
     </row>
@@ -2994,11 +3030,11 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G131" s="1"/>
     </row>
@@ -3012,7 +3048,7 @@
         <v>5</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G132" s="1"/>
     </row>
@@ -3020,11 +3056,11 @@
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G133" s="1"/>
     </row>
@@ -3032,13 +3068,13 @@
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G134" s="1"/>
     </row>
@@ -3046,11 +3082,11 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G135" s="1"/>
     </row>
@@ -3058,11 +3094,11 @@
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G136" s="1"/>
     </row>
@@ -3086,7 +3122,7 @@
         <v>52</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G138" s="1"/>
     </row>
@@ -3098,7 +3134,7 @@
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G139" s="1"/>
     </row>
@@ -3122,7 +3158,7 @@
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G141" s="1"/>
     </row>
@@ -3144,7 +3180,7 @@
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G143" s="1"/>
     </row>
@@ -3156,7 +3192,7 @@
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G144" s="1"/>
     </row>
@@ -3168,7 +3204,7 @@
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G145" s="1"/>
     </row>
@@ -3183,16 +3219,16 @@
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
       <c r="C147" s="1" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G147" s="1"/>
     </row>
@@ -3200,11 +3236,11 @@
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G148" s="1"/>
     </row>
@@ -3212,7 +3248,7 @@
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
@@ -3224,11 +3260,11 @@
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G150" s="1"/>
     </row>
@@ -3252,7 +3288,7 @@
         <v>52</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G152" s="1"/>
     </row>
@@ -3280,7 +3316,7 @@
         <v>5</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G154" s="1"/>
     </row>
@@ -3292,7 +3328,7 @@
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G155" s="1"/>
     </row>
@@ -3304,7 +3340,7 @@
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G156" s="1"/>
     </row>
@@ -3312,11 +3348,11 @@
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E157" s="1"/>
       <c r="F157" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G157" s="1"/>
     </row>
@@ -3324,11 +3360,11 @@
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G158" s="1"/>
     </row>
@@ -3340,7 +3376,7 @@
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G159" s="1"/>
     </row>
@@ -3348,11 +3384,11 @@
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E160" s="1"/>
       <c r="F160" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G160" s="1"/>
     </row>
@@ -3386,7 +3422,7 @@
         <v>5</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G163" s="1"/>
     </row>
@@ -3412,7 +3448,7 @@
       </c>
       <c r="E165" s="1"/>
       <c r="F165" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G165" s="1"/>
     </row>
@@ -3424,7 +3460,7 @@
       </c>
       <c r="E166" s="1"/>
       <c r="F166" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G166" s="1"/>
     </row>
@@ -3436,7 +3472,7 @@
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G167" s="1"/>
     </row>
@@ -3460,7 +3496,7 @@
         <v>52</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G169" s="1"/>
     </row>
@@ -3482,11 +3518,11 @@
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E171" s="1"/>
       <c r="F171" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G171" s="1"/>
     </row>
@@ -3494,11 +3530,11 @@
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E172" s="1"/>
       <c r="F172" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G172" s="1"/>
     </row>
@@ -3510,7 +3546,7 @@
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G173" s="1"/>
     </row>
@@ -3522,7 +3558,7 @@
       </c>
       <c r="E174" s="1"/>
       <c r="F174" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G174" s="1"/>
     </row>
@@ -3534,7 +3570,7 @@
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G175" s="1"/>
     </row>
@@ -3546,7 +3582,7 @@
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G176" s="1"/>
     </row>
@@ -3554,11 +3590,11 @@
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G177" s="1"/>
     </row>
@@ -3582,7 +3618,7 @@
         <v>52</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G179" s="1"/>
     </row>
@@ -3596,7 +3632,7 @@
         <v>5</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G180" s="1"/>
     </row>
@@ -3610,7 +3646,7 @@
         <v>5</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G181" s="1"/>
     </row>
@@ -3622,7 +3658,7 @@
       </c>
       <c r="E182" s="1"/>
       <c r="F182" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G182" s="1"/>
     </row>
@@ -3634,7 +3670,7 @@
       </c>
       <c r="E183" s="1"/>
       <c r="F183" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G183" s="1"/>
     </row>
@@ -3646,7 +3682,7 @@
       </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G184" s="1"/>
     </row>
@@ -3670,7 +3706,7 @@
         <v>52</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G186" s="1"/>
     </row>
@@ -3698,7 +3734,7 @@
         <v>5</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G188" s="1"/>
     </row>
@@ -3712,7 +3748,7 @@
         <v>5</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G189" s="1"/>
     </row>
@@ -3724,7 +3760,7 @@
       </c>
       <c r="E190" s="1"/>
       <c r="F190" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G190" s="1"/>
     </row>
@@ -3736,7 +3772,7 @@
       </c>
       <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G191" s="1"/>
     </row>
@@ -3756,11 +3792,11 @@
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E193" s="1"/>
       <c r="F193" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="G193" s="1"/>
     </row>
@@ -3784,7 +3820,7 @@
         <v>52</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G195" s="1"/>
     </row>
@@ -3798,7 +3834,7 @@
         <v>5</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G196" s="1"/>
     </row>
@@ -3812,7 +3848,7 @@
         <v>5</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G197" s="1"/>
     </row>
@@ -3824,7 +3860,7 @@
       </c>
       <c r="E198" s="1"/>
       <c r="F198" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G198" s="1"/>
     </row>
@@ -3836,7 +3872,7 @@
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G199" s="1"/>
     </row>
@@ -3848,7 +3884,7 @@
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G200" s="1"/>
     </row>
@@ -3863,7 +3899,7 @@
     <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202" s="1"/>
       <c r="C202" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>2</v>
@@ -3872,7 +3908,7 @@
         <v>52</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G202" s="1"/>
     </row>
@@ -3880,7 +3916,7 @@
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>61</v>
@@ -3894,13 +3930,13 @@
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G204" s="1"/>
     </row>
@@ -3908,13 +3944,13 @@
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G205" s="1"/>
     </row>
@@ -3922,11 +3958,11 @@
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E206" s="1"/>
       <c r="F206" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G206" s="1"/>
     </row>
@@ -3934,11 +3970,11 @@
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="E207" s="1"/>
       <c r="F207" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G207" s="1"/>
     </row>
@@ -3981,7 +4017,7 @@
     <row r="211" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B211" s="1"/>
       <c r="C211" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>2</v>
@@ -3990,7 +4026,7 @@
         <v>52</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G211" s="1"/>
     </row>
@@ -3998,7 +4034,7 @@
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>61</v>
@@ -4018,7 +4054,7 @@
         <v>5</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G213" s="1"/>
     </row>
@@ -4026,11 +4062,11 @@
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E214" s="1"/>
       <c r="F214" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -4038,11 +4074,11 @@
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E215" s="1"/>
       <c r="F215" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G215" s="1"/>
     </row>
@@ -4050,11 +4086,11 @@
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G216" s="1"/>
     </row>
@@ -4062,11 +4098,11 @@
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G217" s="1"/>
     </row>
@@ -4074,15 +4110,15 @@
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="G218" s="1"/>
       <c r="H218" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.25">
@@ -4105,7 +4141,7 @@
         <v>52</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G220" s="1"/>
     </row>
@@ -4133,7 +4169,7 @@
         <v>5</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G222" s="1"/>
     </row>
@@ -4145,7 +4181,7 @@
       </c>
       <c r="E223" s="1"/>
       <c r="F223" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G223" s="1"/>
     </row>
@@ -4157,7 +4193,7 @@
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G224" s="1"/>
     </row>
@@ -4169,7 +4205,7 @@
       </c>
       <c r="E225" s="1"/>
       <c r="F225" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G225" s="1"/>
     </row>
@@ -4193,7 +4229,7 @@
         <v>5</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G227" s="1"/>
     </row>
@@ -4207,7 +4243,7 @@
         <v>5</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G228" s="1"/>
     </row>
@@ -4219,7 +4255,7 @@
       </c>
       <c r="E229" s="1"/>
       <c r="F229" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G229" s="1"/>
     </row>
@@ -4231,7 +4267,7 @@
       </c>
       <c r="E230" s="1"/>
       <c r="F230" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G230" s="1"/>
     </row>
@@ -4255,7 +4291,7 @@
       </c>
       <c r="E232" s="1"/>
       <c r="F232" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G232" s="1"/>
     </row>
@@ -4279,7 +4315,7 @@
         <v>52</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G234" s="1"/>
     </row>
@@ -4307,7 +4343,7 @@
         <v>5</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G236" s="1"/>
     </row>
@@ -4319,7 +4355,7 @@
       </c>
       <c r="E237" s="1"/>
       <c r="F237" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G237" s="1"/>
     </row>
@@ -4331,7 +4367,7 @@
       </c>
       <c r="E238" s="1"/>
       <c r="F238" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G238" s="1"/>
     </row>
@@ -4343,7 +4379,7 @@
       </c>
       <c r="E239" s="1"/>
       <c r="F239" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G239" s="1"/>
     </row>
@@ -4355,7 +4391,7 @@
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G240" s="1"/>
     </row>
@@ -4367,7 +4403,7 @@
       </c>
       <c r="E241" s="1"/>
       <c r="F241" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G241" s="1"/>
     </row>
@@ -4379,7 +4415,7 @@
       </c>
       <c r="E242" s="1"/>
       <c r="F242" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G242" s="1"/>
     </row>
@@ -4403,7 +4439,7 @@
         <v>5</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G244" s="1"/>
     </row>
@@ -4417,7 +4453,7 @@
         <v>5</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G245" s="1"/>
     </row>
@@ -4429,7 +4465,7 @@
       </c>
       <c r="E246" s="1"/>
       <c r="F246" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G246" s="1"/>
     </row>
@@ -4441,7 +4477,7 @@
       </c>
       <c r="E247" s="1"/>
       <c r="F247" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G247" s="1"/>
     </row>
@@ -4449,11 +4485,11 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E248" s="1"/>
       <c r="F248" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G248" s="1"/>
     </row>
@@ -4461,11 +4497,11 @@
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
       <c r="D249" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E249" s="1"/>
       <c r="F249" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G249" s="1"/>
     </row>
@@ -4473,11 +4509,11 @@
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G250" s="1"/>
     </row>
@@ -4485,11 +4521,11 @@
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G251" s="1"/>
     </row>
@@ -4513,7 +4549,7 @@
         <v>52</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G253" s="1"/>
     </row>
@@ -4535,13 +4571,13 @@
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
       <c r="D255" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E255" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G255" s="1"/>
     </row>
@@ -4553,7 +4589,7 @@
       </c>
       <c r="E256" s="1"/>
       <c r="F256" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G256" s="1"/>
     </row>
@@ -4565,7 +4601,7 @@
       </c>
       <c r="E257" s="1"/>
       <c r="F257" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G257" s="1"/>
     </row>
@@ -4589,7 +4625,7 @@
         <v>5</v>
       </c>
       <c r="F259" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G259" s="1"/>
     </row>
@@ -4603,7 +4639,7 @@
         <v>5</v>
       </c>
       <c r="F260" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G260" s="1"/>
     </row>
@@ -4615,7 +4651,7 @@
       </c>
       <c r="E261" s="1"/>
       <c r="F261" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G261" s="1"/>
     </row>
@@ -4623,11 +4659,11 @@
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
       <c r="D262" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E262" s="1"/>
       <c r="F262" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G262" s="1"/>
     </row>
@@ -4635,11 +4671,11 @@
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
       <c r="D263" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E263" s="1"/>
       <c r="F263" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G263" s="1"/>
     </row>
@@ -4647,11 +4683,11 @@
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
       <c r="D264" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E264" s="1"/>
       <c r="F264" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G264" s="1"/>
     </row>
@@ -4663,7 +4699,7 @@
       </c>
       <c r="E265" s="1"/>
       <c r="F265" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G265" s="1"/>
     </row>
@@ -4687,7 +4723,7 @@
       </c>
       <c r="E267" s="1"/>
       <c r="F267" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G267" s="1"/>
     </row>
@@ -4702,7 +4738,7 @@
     <row r="269" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B269" s="1"/>
       <c r="C269" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D269" s="1" t="s">
         <v>2</v>
@@ -4711,7 +4747,7 @@
         <v>52</v>
       </c>
       <c r="F269" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G269" s="1"/>
     </row>
@@ -4719,13 +4755,13 @@
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
       <c r="D270" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E270" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F270" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G270" s="1"/>
     </row>
@@ -4739,7 +4775,7 @@
         <v>5</v>
       </c>
       <c r="F271" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G271" s="1"/>
     </row>
@@ -4751,7 +4787,7 @@
       </c>
       <c r="E272" s="1"/>
       <c r="F272" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G272" s="1"/>
     </row>
@@ -4766,7 +4802,7 @@
     <row r="274" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B274" s="1"/>
       <c r="C274" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D274" s="1" t="s">
         <v>126</v>
@@ -4775,7 +4811,7 @@
         <v>5</v>
       </c>
       <c r="F274" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G274" s="1"/>
     </row>
@@ -4789,7 +4825,7 @@
         <v>5</v>
       </c>
       <c r="F275" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G275" s="1"/>
     </row>
@@ -4801,7 +4837,7 @@
       </c>
       <c r="E276" s="1"/>
       <c r="F276" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G276" s="1"/>
     </row>
@@ -4813,7 +4849,7 @@
       </c>
       <c r="E277" s="1"/>
       <c r="F277" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G277" s="1"/>
     </row>
@@ -4837,7 +4873,7 @@
       </c>
       <c r="E279" s="1"/>
       <c r="F279" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G279" s="1"/>
     </row>
@@ -4865,13 +4901,13 @@
         <v>91</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="E282" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F282" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G282" s="1"/>
     </row>
@@ -4885,11 +4921,11 @@
         <v>61</v>
       </c>
       <c r="F283" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="G283" s="1"/>
       <c r="H283" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="284" spans="2:8" x14ac:dyDescent="0.25">
@@ -4900,7 +4936,7 @@
       </c>
       <c r="E284" s="1"/>
       <c r="F284" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G284" s="1"/>
     </row>
@@ -4918,13 +4954,13 @@
         <v>104</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>2</v>
+        <v>286</v>
       </c>
       <c r="E286" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F286" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G286" s="1"/>
     </row>
@@ -4932,13 +4968,13 @@
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
       <c r="D287" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E287" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F287" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="G287" s="1"/>
     </row>
@@ -4946,11 +4982,11 @@
       <c r="B288" s="1"/>
       <c r="C288" s="1"/>
       <c r="D288" s="1" t="s">
-        <v>151</v>
+        <v>289</v>
       </c>
       <c r="E288" s="1"/>
       <c r="F288" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G288" s="1"/>
     </row>
@@ -4958,11 +4994,11 @@
       <c r="B289" s="1"/>
       <c r="C289" s="1"/>
       <c r="D289" s="1" t="s">
-        <v>152</v>
+        <v>290</v>
       </c>
       <c r="E289" s="1"/>
       <c r="F289" s="1" t="s">
-        <v>229</v>
+        <v>161</v>
       </c>
       <c r="G289" s="1"/>
     </row>
@@ -4970,61 +5006,57 @@
       <c r="B290" s="1"/>
       <c r="C290" s="1"/>
       <c r="D290" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E290" s="1"/>
       <c r="F290" s="1" t="s">
-        <v>63</v>
+        <v>223</v>
       </c>
       <c r="G290" s="1"/>
     </row>
     <row r="291" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
-      <c r="D291" s="1"/>
+      <c r="D291" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="E291" s="1"/>
-      <c r="F291" s="1"/>
+      <c r="F291" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G291" s="1"/>
     </row>
     <row r="292" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B292" s="1"/>
-      <c r="C292" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="C292" s="1"/>
       <c r="D292" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F292" s="1" t="s">
-        <v>231</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="E292" s="1"/>
+      <c r="F292" s="1"/>
       <c r="G292" s="1"/>
     </row>
     <row r="293" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B293" s="1"/>
       <c r="C293" s="1"/>
-      <c r="D293" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E293" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F293" s="1" t="s">
-        <v>231</v>
-      </c>
+      <c r="D293" s="1"/>
+      <c r="E293" s="1"/>
+      <c r="F293" s="1"/>
       <c r="G293" s="1"/>
     </row>
     <row r="294" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B294" s="1"/>
-      <c r="C294" s="1"/>
+      <c r="C294" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="D294" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E294" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F294" s="1" t="s">
-        <v>167</v>
+        <v>225</v>
       </c>
       <c r="G294" s="1"/>
     </row>
@@ -5032,11 +5064,13 @@
       <c r="B295" s="1"/>
       <c r="C295" s="1"/>
       <c r="D295" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E295" s="1"/>
+        <v>233</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F295" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G295" s="1"/>
     </row>
@@ -5044,35 +5078,35 @@
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
       <c r="D296" s="1" t="s">
-        <v>156</v>
+        <v>291</v>
       </c>
       <c r="E296" s="1"/>
       <c r="F296" s="1" t="s">
-        <v>63</v>
+        <v>161</v>
       </c>
       <c r="G296" s="1"/>
     </row>
     <row r="297" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
-      <c r="D297" s="1"/>
+      <c r="D297" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="E297" s="1"/>
-      <c r="F297" s="1"/>
+      <c r="F297" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="G297" s="1"/>
     </row>
     <row r="298" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B298" s="1"/>
-      <c r="C298" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="C298" s="1"/>
       <c r="D298" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E298" s="1"/>
       <c r="F298" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="G298" s="1"/>
     </row>
@@ -5080,13 +5114,11 @@
       <c r="B299" s="1"/>
       <c r="C299" s="1"/>
       <c r="D299" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E299" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="E299" s="1"/>
       <c r="F299" s="1" t="s">
-        <v>227</v>
+        <v>281</v>
       </c>
       <c r="G299" s="1"/>
     </row>
@@ -5094,35 +5126,35 @@
       <c r="B300" s="1"/>
       <c r="C300" s="1"/>
       <c r="D300" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E300" s="1"/>
       <c r="F300" s="1" t="s">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="G300" s="1"/>
     </row>
     <row r="301" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B301" s="1"/>
       <c r="C301" s="1"/>
-      <c r="D301" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="D301" s="1"/>
       <c r="E301" s="1"/>
-      <c r="F301" s="1" t="s">
-        <v>229</v>
-      </c>
+      <c r="F301" s="1"/>
       <c r="G301" s="1"/>
     </row>
     <row r="302" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B302" s="1"/>
-      <c r="C302" s="1"/>
+      <c r="C302" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="D302" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E302" s="1"/>
+        <v>296</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F302" s="1" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="G302" s="1"/>
     </row>
@@ -5130,17 +5162,141 @@
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
       <c r="D303" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E303" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F303" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G303" s="1"/>
+    </row>
+    <row r="304" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B304" s="1"/>
+      <c r="C304" s="1"/>
+      <c r="D304" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E304" s="1"/>
+      <c r="F304" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G304" s="1"/>
+    </row>
+    <row r="305" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B305" s="1"/>
+      <c r="C305" s="1"/>
+      <c r="D305" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E305" s="1"/>
+      <c r="F305" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G305" s="1"/>
+    </row>
+    <row r="306" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B306" s="1"/>
+      <c r="C306" s="1"/>
+      <c r="D306" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E306" s="1"/>
+      <c r="F306" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G306" s="1"/>
+    </row>
+    <row r="307" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B307" s="1"/>
+      <c r="C307" s="1"/>
+      <c r="D307" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E307" s="1"/>
+      <c r="F307" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G303" s="1"/>
-    </row>
-    <row r="305" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B305" t="s">
-        <v>161</v>
+      <c r="G307" s="1"/>
+    </row>
+    <row r="308" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B308" s="1"/>
+      <c r="C308" s="1"/>
+      <c r="D308" s="1"/>
+      <c r="E308" s="1"/>
+      <c r="F308" s="1"/>
+      <c r="G308" s="1"/>
+    </row>
+    <row r="309" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B309" s="1"/>
+      <c r="C309" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D309" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F309" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G309" s="1"/>
+    </row>
+    <row r="310" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B310" s="1"/>
+      <c r="C310" s="1"/>
+      <c r="D310" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E310" t="s">
+        <v>294</v>
+      </c>
+      <c r="F310" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G310" s="1"/>
+    </row>
+    <row r="311" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B311" s="1"/>
+      <c r="C311" s="1"/>
+      <c r="D311" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E311" s="1"/>
+      <c r="F311" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G311" s="1"/>
+    </row>
+    <row r="312" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B312" s="1"/>
+      <c r="C312" s="1"/>
+      <c r="D312" s="1"/>
+      <c r="E312" s="1"/>
+      <c r="F312" s="1"/>
+      <c r="G312" s="1"/>
+    </row>
+    <row r="313" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B313" s="1"/>
+      <c r="C313" s="1"/>
+      <c r="D313" s="1"/>
+      <c r="E313" s="1"/>
+      <c r="F313" s="1"/>
+      <c r="G313" s="1"/>
+    </row>
+    <row r="314" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B314" s="1"/>
+      <c r="C314" s="1"/>
+      <c r="D314" s="1"/>
+      <c r="E314" s="1"/>
+      <c r="F314" s="1"/>
+      <c r="G314" s="1"/>
+    </row>
+    <row r="316" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B316" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update design database on credit and debt
added payment table to each debt and credit
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.beta.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$306</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$302</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="306">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -479,12 +479,6 @@
     <t>credit_nominal</t>
   </si>
   <si>
-    <t>debt_description</t>
-  </si>
-  <si>
-    <t>credit_description</t>
-  </si>
-  <si>
     <t>TAX</t>
   </si>
   <si>
@@ -881,33 +875,15 @@
     <t>debt_id</t>
   </si>
   <si>
-    <t>debt_pay_method</t>
-  </si>
-  <si>
     <t>credit_id</t>
   </si>
   <si>
-    <t>debt_date_begin</t>
-  </si>
-  <si>
-    <t>debt_date_end</t>
-  </si>
-  <si>
-    <t>credit_date_begin</t>
-  </si>
-  <si>
-    <t>credit_date_end</t>
-  </si>
-  <si>
     <t>pm_name</t>
   </si>
   <si>
     <t>not null</t>
   </si>
   <si>
-    <t>credit_pay_id</t>
-  </si>
-  <si>
     <t>journal_id</t>
   </si>
   <si>
@@ -923,13 +899,43 @@
     <t>journal_description</t>
   </si>
   <si>
-    <t>varchar(10)</t>
-  </si>
-  <si>
     <t>pm_description</t>
   </si>
   <si>
     <t>PAYMENT METHOD</t>
+  </si>
+  <si>
+    <t>credit_duedate</t>
+  </si>
+  <si>
+    <t>credit_paid</t>
+  </si>
+  <si>
+    <t>debt_duedate</t>
+  </si>
+  <si>
+    <t>debt_paid</t>
+  </si>
+  <si>
+    <t>PAYMENT_DEBT</t>
+  </si>
+  <si>
+    <t>payment_id</t>
+  </si>
+  <si>
+    <t>payment_date</t>
+  </si>
+  <si>
+    <t>payment_nominal</t>
+  </si>
+  <si>
+    <t>payment_description</t>
+  </si>
+  <si>
+    <t>payment_confirmed</t>
+  </si>
+  <si>
+    <t>PAYMENT_CREDIT</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1315,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q316"/>
+  <dimension ref="B1:Q325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="C309" sqref="C309"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="D319" sqref="D319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1332,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1356,7 +1362,7 @@
         <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>54</v>
@@ -1370,7 +1376,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1394,13 +1400,13 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1411,10 +1417,10 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H7" t="s">
         <v>64</v>
@@ -1450,7 +1456,7 @@
         <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1461,10 +1467,10 @@
         <v>88</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1472,11 +1478,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1484,11 +1490,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1496,11 +1502,11 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1512,7 +1518,7 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1520,13 +1526,13 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1534,14 +1540,14 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -1554,7 +1560,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1565,7 +1571,7 @@
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
@@ -1574,7 +1580,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1588,7 +1594,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1596,11 +1602,11 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1608,11 +1614,11 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1620,28 +1626,28 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -1674,7 +1680,7 @@
         <v>52</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>54</v>
@@ -1690,7 +1696,7 @@
         <v>61</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1698,13 +1704,13 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1716,7 +1722,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1728,7 +1734,7 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
@@ -1752,7 +1758,7 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1766,7 +1772,7 @@
         <v>5</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -1799,7 +1805,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G36" s="1"/>
       <c r="N36" t="s">
@@ -1820,7 +1826,7 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G37" s="1"/>
       <c r="N37" t="s">
@@ -1853,7 +1859,7 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1877,7 +1883,7 @@
         <v>52</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>54</v>
@@ -1896,7 +1902,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -1910,11 +1916,11 @@
         <v>5</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
@@ -1927,7 +1933,7 @@
         <v>57</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -1951,7 +1957,7 @@
         <v>52</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>54</v>
@@ -1967,7 +1973,7 @@
         <v>5</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -1981,7 +1987,7 @@
         <v>5</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -1995,7 +2001,7 @@
         <v>5</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -2003,11 +2009,11 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -2027,11 +2033,11 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -2039,13 +2045,13 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -2060,7 +2066,7 @@
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>2</v>
@@ -2069,22 +2075,22 @@
         <v>52</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -2099,7 +2105,7 @@
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>2</v>
@@ -2108,7 +2114,7 @@
         <v>52</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -2122,7 +2128,7 @@
         <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2130,11 +2136,11 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2148,25 +2154,25 @@
         <v>5</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="K61" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2200,7 +2206,7 @@
         <v>52</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -2212,7 +2218,7 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -2220,11 +2226,11 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G67" s="1"/>
     </row>
@@ -2232,11 +2238,11 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G68" s="1"/>
     </row>
@@ -2244,11 +2250,11 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G69" s="1"/>
     </row>
@@ -2260,7 +2266,7 @@
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G70" s="1"/>
     </row>
@@ -2272,7 +2278,7 @@
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G71" s="1"/>
     </row>
@@ -2284,7 +2290,7 @@
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G72" s="1"/>
     </row>
@@ -2296,7 +2302,7 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G73" s="1"/>
     </row>
@@ -2304,11 +2310,11 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2316,35 +2322,35 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2361,7 +2367,7 @@
         <v>52</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G78" s="1"/>
     </row>
@@ -2375,7 +2381,7 @@
         <v>5</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G79" s="1"/>
     </row>
@@ -2383,11 +2389,11 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G80" s="1"/>
     </row>
@@ -2395,11 +2401,11 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G81" s="1"/>
     </row>
@@ -2407,11 +2413,11 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -2419,11 +2425,11 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G83" s="1"/>
     </row>
@@ -2431,11 +2437,11 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G84" s="1"/>
     </row>
@@ -2469,7 +2475,7 @@
         <v>52</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>54</v>
@@ -2483,7 +2489,7 @@
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G88" s="1"/>
     </row>
@@ -2491,11 +2497,11 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G89" s="1"/>
     </row>
@@ -2503,11 +2509,11 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G90" s="1"/>
     </row>
@@ -2515,11 +2521,11 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G91" s="1"/>
     </row>
@@ -2531,7 +2537,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -2543,7 +2549,7 @@
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G93" s="1"/>
     </row>
@@ -2555,7 +2561,7 @@
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G94" s="1"/>
     </row>
@@ -2567,7 +2573,7 @@
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G95" s="1"/>
     </row>
@@ -2592,7 +2598,7 @@
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>2</v>
@@ -2601,7 +2607,7 @@
         <v>52</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>54</v>
@@ -2617,7 +2623,7 @@
         <v>61</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G99" s="1"/>
     </row>
@@ -2625,13 +2631,13 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G100" s="1"/>
     </row>
@@ -2639,11 +2645,11 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G101" s="1"/>
     </row>
@@ -2651,7 +2657,7 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
@@ -2663,11 +2669,11 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>76</v>
@@ -2677,69 +2683,69 @@
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G108" s="1"/>
     </row>
@@ -2747,11 +2753,11 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G109" s="1"/>
     </row>
@@ -2759,11 +2765,11 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G110" s="1"/>
     </row>
@@ -2771,11 +2777,11 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G111" s="1"/>
     </row>
@@ -2789,7 +2795,7 @@
         <v>5</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G112" s="1"/>
     </row>
@@ -2803,7 +2809,7 @@
         <v>5</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G113" s="1"/>
     </row>
@@ -2811,13 +2817,13 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G114" s="1"/>
     </row>
@@ -2825,11 +2831,11 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G115" s="1"/>
     </row>
@@ -2837,11 +2843,11 @@
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G116" s="1"/>
     </row>
@@ -2849,25 +2855,25 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G118" s="1"/>
     </row>
@@ -2875,16 +2881,16 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
@@ -2898,7 +2904,7 @@
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>79</v>
@@ -2907,7 +2913,7 @@
         <v>52</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G121" s="1"/>
     </row>
@@ -2915,13 +2921,13 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G122" s="1"/>
     </row>
@@ -2945,7 +2951,7 @@
         <v>52</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G124" s="1"/>
     </row>
@@ -2959,7 +2965,7 @@
         <v>5</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G125" s="1"/>
     </row>
@@ -2971,7 +2977,7 @@
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G126" s="1"/>
     </row>
@@ -2983,7 +2989,7 @@
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" t="s">
@@ -2998,7 +3004,7 @@
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G128" s="1"/>
     </row>
@@ -3013,7 +3019,7 @@
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>2</v>
@@ -3022,7 +3028,7 @@
         <v>52</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G130" s="1"/>
     </row>
@@ -3030,11 +3036,11 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G131" s="1"/>
     </row>
@@ -3048,7 +3054,7 @@
         <v>5</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G132" s="1"/>
     </row>
@@ -3056,11 +3062,11 @@
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G133" s="1"/>
     </row>
@@ -3068,13 +3074,13 @@
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G134" s="1"/>
     </row>
@@ -3082,11 +3088,11 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G135" s="1"/>
     </row>
@@ -3094,11 +3100,11 @@
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G136" s="1"/>
     </row>
@@ -3122,7 +3128,7 @@
         <v>52</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G138" s="1"/>
     </row>
@@ -3134,7 +3140,7 @@
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G139" s="1"/>
     </row>
@@ -3158,7 +3164,7 @@
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G141" s="1"/>
     </row>
@@ -3180,7 +3186,7 @@
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G143" s="1"/>
     </row>
@@ -3192,7 +3198,7 @@
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G144" s="1"/>
     </row>
@@ -3204,7 +3210,7 @@
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G145" s="1"/>
     </row>
@@ -3219,16 +3225,16 @@
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
       <c r="C147" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G147" s="1"/>
     </row>
@@ -3236,11 +3242,11 @@
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G148" s="1"/>
     </row>
@@ -3248,7 +3254,7 @@
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
@@ -3260,11 +3266,11 @@
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G150" s="1"/>
     </row>
@@ -3288,7 +3294,7 @@
         <v>52</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G152" s="1"/>
     </row>
@@ -3316,7 +3322,7 @@
         <v>5</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G154" s="1"/>
     </row>
@@ -3328,7 +3334,7 @@
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G155" s="1"/>
     </row>
@@ -3340,7 +3346,7 @@
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G156" s="1"/>
     </row>
@@ -3348,11 +3354,11 @@
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E157" s="1"/>
       <c r="F157" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G157" s="1"/>
     </row>
@@ -3360,11 +3366,11 @@
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G158" s="1"/>
     </row>
@@ -3376,7 +3382,7 @@
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G159" s="1"/>
     </row>
@@ -3384,11 +3390,11 @@
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E160" s="1"/>
       <c r="F160" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G160" s="1"/>
     </row>
@@ -3422,7 +3428,7 @@
         <v>5</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G163" s="1"/>
     </row>
@@ -3448,7 +3454,7 @@
       </c>
       <c r="E165" s="1"/>
       <c r="F165" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G165" s="1"/>
     </row>
@@ -3460,7 +3466,7 @@
       </c>
       <c r="E166" s="1"/>
       <c r="F166" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G166" s="1"/>
     </row>
@@ -3472,7 +3478,7 @@
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G167" s="1"/>
     </row>
@@ -3496,7 +3502,7 @@
         <v>52</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G169" s="1"/>
     </row>
@@ -3518,11 +3524,11 @@
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E171" s="1"/>
       <c r="F171" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G171" s="1"/>
     </row>
@@ -3530,11 +3536,11 @@
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E172" s="1"/>
       <c r="F172" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G172" s="1"/>
     </row>
@@ -3546,7 +3552,7 @@
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G173" s="1"/>
     </row>
@@ -3558,7 +3564,7 @@
       </c>
       <c r="E174" s="1"/>
       <c r="F174" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G174" s="1"/>
     </row>
@@ -3570,7 +3576,7 @@
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G175" s="1"/>
     </row>
@@ -3582,7 +3588,7 @@
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G176" s="1"/>
     </row>
@@ -3590,11 +3596,11 @@
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G177" s="1"/>
     </row>
@@ -3618,7 +3624,7 @@
         <v>52</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G179" s="1"/>
     </row>
@@ -3632,7 +3638,7 @@
         <v>5</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G180" s="1"/>
     </row>
@@ -3646,7 +3652,7 @@
         <v>5</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G181" s="1"/>
     </row>
@@ -3658,7 +3664,7 @@
       </c>
       <c r="E182" s="1"/>
       <c r="F182" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G182" s="1"/>
     </row>
@@ -3670,7 +3676,7 @@
       </c>
       <c r="E183" s="1"/>
       <c r="F183" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G183" s="1"/>
     </row>
@@ -3682,7 +3688,7 @@
       </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G184" s="1"/>
     </row>
@@ -3706,7 +3712,7 @@
         <v>52</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G186" s="1"/>
     </row>
@@ -3734,7 +3740,7 @@
         <v>5</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G188" s="1"/>
     </row>
@@ -3748,7 +3754,7 @@
         <v>5</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G189" s="1"/>
     </row>
@@ -3760,7 +3766,7 @@
       </c>
       <c r="E190" s="1"/>
       <c r="F190" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G190" s="1"/>
     </row>
@@ -3772,7 +3778,7 @@
       </c>
       <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G191" s="1"/>
     </row>
@@ -3792,11 +3798,11 @@
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E193" s="1"/>
       <c r="F193" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G193" s="1"/>
     </row>
@@ -3820,7 +3826,7 @@
         <v>52</v>
       </c>
       <c r="F195" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G195" s="1"/>
     </row>
@@ -3834,7 +3840,7 @@
         <v>5</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G196" s="1"/>
     </row>
@@ -3848,7 +3854,7 @@
         <v>5</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G197" s="1"/>
     </row>
@@ -3860,7 +3866,7 @@
       </c>
       <c r="E198" s="1"/>
       <c r="F198" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G198" s="1"/>
     </row>
@@ -3872,7 +3878,7 @@
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G199" s="1"/>
     </row>
@@ -3884,7 +3890,7 @@
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G200" s="1"/>
     </row>
@@ -3899,7 +3905,7 @@
     <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202" s="1"/>
       <c r="C202" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>2</v>
@@ -3908,7 +3914,7 @@
         <v>52</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G202" s="1"/>
     </row>
@@ -3916,7 +3922,7 @@
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>61</v>
@@ -3930,13 +3936,13 @@
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G204" s="1"/>
     </row>
@@ -3944,13 +3950,13 @@
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G205" s="1"/>
     </row>
@@ -3958,11 +3964,11 @@
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E206" s="1"/>
       <c r="F206" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G206" s="1"/>
     </row>
@@ -3970,11 +3976,11 @@
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E207" s="1"/>
       <c r="F207" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G207" s="1"/>
     </row>
@@ -4017,7 +4023,7 @@
     <row r="211" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B211" s="1"/>
       <c r="C211" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>2</v>
@@ -4026,7 +4032,7 @@
         <v>52</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G211" s="1"/>
     </row>
@@ -4034,7 +4040,7 @@
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>61</v>
@@ -4054,7 +4060,7 @@
         <v>5</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G213" s="1"/>
     </row>
@@ -4062,11 +4068,11 @@
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E214" s="1"/>
       <c r="F214" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -4074,11 +4080,11 @@
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E215" s="1"/>
       <c r="F215" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G215" s="1"/>
     </row>
@@ -4086,11 +4092,11 @@
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G216" s="1"/>
     </row>
@@ -4098,11 +4104,11 @@
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G217" s="1"/>
     </row>
@@ -4110,15 +4116,15 @@
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G218" s="1"/>
       <c r="H218" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.25">
@@ -4141,7 +4147,7 @@
         <v>52</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G220" s="1"/>
     </row>
@@ -4169,7 +4175,7 @@
         <v>5</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G222" s="1"/>
     </row>
@@ -4181,7 +4187,7 @@
       </c>
       <c r="E223" s="1"/>
       <c r="F223" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G223" s="1"/>
     </row>
@@ -4193,7 +4199,7 @@
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G224" s="1"/>
     </row>
@@ -4205,7 +4211,7 @@
       </c>
       <c r="E225" s="1"/>
       <c r="F225" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G225" s="1"/>
     </row>
@@ -4229,7 +4235,7 @@
         <v>5</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G227" s="1"/>
     </row>
@@ -4243,7 +4249,7 @@
         <v>5</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G228" s="1"/>
     </row>
@@ -4255,7 +4261,7 @@
       </c>
       <c r="E229" s="1"/>
       <c r="F229" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G229" s="1"/>
     </row>
@@ -4267,7 +4273,7 @@
       </c>
       <c r="E230" s="1"/>
       <c r="F230" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G230" s="1"/>
     </row>
@@ -4291,7 +4297,7 @@
       </c>
       <c r="E232" s="1"/>
       <c r="F232" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G232" s="1"/>
     </row>
@@ -4315,7 +4321,7 @@
         <v>52</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G234" s="1"/>
     </row>
@@ -4343,7 +4349,7 @@
         <v>5</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G236" s="1"/>
     </row>
@@ -4355,7 +4361,7 @@
       </c>
       <c r="E237" s="1"/>
       <c r="F237" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G237" s="1"/>
     </row>
@@ -4367,7 +4373,7 @@
       </c>
       <c r="E238" s="1"/>
       <c r="F238" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G238" s="1"/>
     </row>
@@ -4379,7 +4385,7 @@
       </c>
       <c r="E239" s="1"/>
       <c r="F239" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G239" s="1"/>
     </row>
@@ -4391,7 +4397,7 @@
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G240" s="1"/>
     </row>
@@ -4403,7 +4409,7 @@
       </c>
       <c r="E241" s="1"/>
       <c r="F241" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G241" s="1"/>
     </row>
@@ -4415,7 +4421,7 @@
       </c>
       <c r="E242" s="1"/>
       <c r="F242" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G242" s="1"/>
     </row>
@@ -4439,7 +4445,7 @@
         <v>5</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G244" s="1"/>
     </row>
@@ -4453,7 +4459,7 @@
         <v>5</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G245" s="1"/>
     </row>
@@ -4465,7 +4471,7 @@
       </c>
       <c r="E246" s="1"/>
       <c r="F246" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G246" s="1"/>
     </row>
@@ -4477,7 +4483,7 @@
       </c>
       <c r="E247" s="1"/>
       <c r="F247" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G247" s="1"/>
     </row>
@@ -4485,11 +4491,11 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E248" s="1"/>
       <c r="F248" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G248" s="1"/>
     </row>
@@ -4497,11 +4503,11 @@
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
       <c r="D249" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E249" s="1"/>
       <c r="F249" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G249" s="1"/>
     </row>
@@ -4509,11 +4515,11 @@
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G250" s="1"/>
     </row>
@@ -4521,11 +4527,11 @@
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G251" s="1"/>
     </row>
@@ -4549,7 +4555,7 @@
         <v>52</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G253" s="1"/>
     </row>
@@ -4571,13 +4577,13 @@
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
       <c r="D255" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E255" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G255" s="1"/>
     </row>
@@ -4589,7 +4595,7 @@
       </c>
       <c r="E256" s="1"/>
       <c r="F256" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G256" s="1"/>
     </row>
@@ -4601,7 +4607,7 @@
       </c>
       <c r="E257" s="1"/>
       <c r="F257" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G257" s="1"/>
     </row>
@@ -4625,7 +4631,7 @@
         <v>5</v>
       </c>
       <c r="F259" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G259" s="1"/>
     </row>
@@ -4639,7 +4645,7 @@
         <v>5</v>
       </c>
       <c r="F260" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G260" s="1"/>
     </row>
@@ -4651,7 +4657,7 @@
       </c>
       <c r="E261" s="1"/>
       <c r="F261" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G261" s="1"/>
     </row>
@@ -4659,11 +4665,11 @@
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
       <c r="D262" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E262" s="1"/>
       <c r="F262" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G262" s="1"/>
     </row>
@@ -4671,11 +4677,11 @@
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
       <c r="D263" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E263" s="1"/>
       <c r="F263" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G263" s="1"/>
     </row>
@@ -4683,11 +4689,11 @@
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
       <c r="D264" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E264" s="1"/>
       <c r="F264" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G264" s="1"/>
     </row>
@@ -4699,7 +4705,7 @@
       </c>
       <c r="E265" s="1"/>
       <c r="F265" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G265" s="1"/>
     </row>
@@ -4723,7 +4729,7 @@
       </c>
       <c r="E267" s="1"/>
       <c r="F267" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G267" s="1"/>
     </row>
@@ -4738,7 +4744,7 @@
     <row r="269" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B269" s="1"/>
       <c r="C269" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D269" s="1" t="s">
         <v>2</v>
@@ -4747,7 +4753,7 @@
         <v>52</v>
       </c>
       <c r="F269" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G269" s="1"/>
     </row>
@@ -4755,13 +4761,13 @@
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
       <c r="D270" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E270" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F270" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G270" s="1"/>
     </row>
@@ -4775,7 +4781,7 @@
         <v>5</v>
       </c>
       <c r="F271" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G271" s="1"/>
     </row>
@@ -4787,7 +4793,7 @@
       </c>
       <c r="E272" s="1"/>
       <c r="F272" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G272" s="1"/>
     </row>
@@ -4802,7 +4808,7 @@
     <row r="274" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B274" s="1"/>
       <c r="C274" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D274" s="1" t="s">
         <v>126</v>
@@ -4811,7 +4817,7 @@
         <v>5</v>
       </c>
       <c r="F274" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G274" s="1"/>
     </row>
@@ -4825,7 +4831,7 @@
         <v>5</v>
       </c>
       <c r="F275" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G275" s="1"/>
     </row>
@@ -4837,7 +4843,7 @@
       </c>
       <c r="E276" s="1"/>
       <c r="F276" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G276" s="1"/>
     </row>
@@ -4849,7 +4855,7 @@
       </c>
       <c r="E277" s="1"/>
       <c r="F277" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G277" s="1"/>
     </row>
@@ -4873,7 +4879,7 @@
       </c>
       <c r="E279" s="1"/>
       <c r="F279" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G279" s="1"/>
     </row>
@@ -4907,7 +4913,7 @@
         <v>52</v>
       </c>
       <c r="F282" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G282" s="1"/>
     </row>
@@ -4921,11 +4927,11 @@
         <v>61</v>
       </c>
       <c r="F283" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G283" s="1"/>
       <c r="H283" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="284" spans="2:8" x14ac:dyDescent="0.25">
@@ -4936,7 +4942,7 @@
       </c>
       <c r="E284" s="1"/>
       <c r="F284" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G284" s="1"/>
     </row>
@@ -4954,13 +4960,13 @@
         <v>104</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E286" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F286" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G286" s="1"/>
     </row>
@@ -4968,13 +4974,13 @@
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
       <c r="D287" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E287" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F287" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G287" s="1"/>
     </row>
@@ -4982,11 +4988,11 @@
       <c r="B288" s="1"/>
       <c r="C288" s="1"/>
       <c r="D288" s="1" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="E288" s="1"/>
       <c r="F288" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G288" s="1"/>
     </row>
@@ -4994,11 +5000,11 @@
       <c r="B289" s="1"/>
       <c r="C289" s="1"/>
       <c r="D289" s="1" t="s">
-        <v>290</v>
+        <v>151</v>
       </c>
       <c r="E289" s="1"/>
       <c r="F289" s="1" t="s">
-        <v>161</v>
+        <v>221</v>
       </c>
       <c r="G289" s="1"/>
     </row>
@@ -5006,57 +5012,61 @@
       <c r="B290" s="1"/>
       <c r="C290" s="1"/>
       <c r="D290" s="1" t="s">
-        <v>151</v>
+        <v>298</v>
       </c>
       <c r="E290" s="1"/>
       <c r="F290" s="1" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="G290" s="1"/>
     </row>
     <row r="291" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
-      <c r="D291" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="D291" s="1"/>
       <c r="E291" s="1"/>
-      <c r="F291" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="F291" s="1"/>
       <c r="G291" s="1"/>
     </row>
     <row r="292" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B292" s="1"/>
-      <c r="C292" s="1"/>
+      <c r="C292" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="D292" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E292" s="1"/>
-      <c r="F292" s="1"/>
+        <v>285</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="G292" s="1"/>
     </row>
     <row r="293" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B293" s="1"/>
       <c r="C293" s="1"/>
-      <c r="D293" s="1"/>
-      <c r="E293" s="1"/>
-      <c r="F293" s="1"/>
+      <c r="D293" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F293" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="G293" s="1"/>
     </row>
     <row r="294" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B294" s="1"/>
-      <c r="C294" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="C294" s="1"/>
       <c r="D294" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E294" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="E294" s="1"/>
       <c r="F294" s="1" t="s">
-        <v>225</v>
+        <v>159</v>
       </c>
       <c r="G294" s="1"/>
     </row>
@@ -5064,13 +5074,11 @@
       <c r="B295" s="1"/>
       <c r="C295" s="1"/>
       <c r="D295" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E295" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E295" s="1"/>
       <c r="F295" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G295" s="1"/>
     </row>
@@ -5078,33 +5086,33 @@
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
       <c r="D296" s="1" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="E296" s="1"/>
       <c r="F296" s="1" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="G296" s="1"/>
     </row>
     <row r="297" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
-      <c r="D297" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="D297" s="1"/>
       <c r="E297" s="1"/>
-      <c r="F297" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="F297" s="1"/>
       <c r="G297" s="1"/>
     </row>
     <row r="298" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B298" s="1"/>
-      <c r="C298" s="1"/>
+      <c r="C298" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="D298" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E298" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="E298" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F298" s="1" t="s">
         <v>223</v>
       </c>
@@ -5114,11 +5122,13 @@
       <c r="B299" s="1"/>
       <c r="C299" s="1"/>
       <c r="D299" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="E299" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="E299" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F299" s="1" t="s">
-        <v>281</v>
+        <v>219</v>
       </c>
       <c r="G299" s="1"/>
     </row>
@@ -5126,35 +5136,35 @@
       <c r="B300" s="1"/>
       <c r="C300" s="1"/>
       <c r="D300" s="1" t="s">
-        <v>154</v>
+        <v>289</v>
       </c>
       <c r="E300" s="1"/>
       <c r="F300" s="1" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="G300" s="1"/>
     </row>
     <row r="301" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B301" s="1"/>
       <c r="C301" s="1"/>
-      <c r="D301" s="1"/>
+      <c r="D301" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="E301" s="1"/>
-      <c r="F301" s="1"/>
+      <c r="F301" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="G301" s="1"/>
     </row>
     <row r="302" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B302" s="1"/>
-      <c r="C302" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="C302" s="1"/>
       <c r="D302" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E302" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="E302" s="1"/>
       <c r="F302" s="1" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="G302" s="1"/>
     </row>
@@ -5162,37 +5172,35 @@
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
       <c r="D303" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E303" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="E303" s="1"/>
       <c r="F303" s="1" t="s">
-        <v>221</v>
+        <v>63</v>
       </c>
       <c r="G303" s="1"/>
     </row>
     <row r="304" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B304" s="1"/>
       <c r="C304" s="1"/>
-      <c r="D304" s="1" t="s">
-        <v>297</v>
-      </c>
+      <c r="D304" s="1"/>
       <c r="E304" s="1"/>
-      <c r="F304" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="F304" s="1"/>
       <c r="G304" s="1"/>
     </row>
     <row r="305" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B305" s="1"/>
-      <c r="C305" s="1"/>
+      <c r="C305" s="1" t="s">
+        <v>294</v>
+      </c>
       <c r="D305" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E305" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F305" s="1" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="G305" s="1"/>
     </row>
@@ -5200,11 +5208,13 @@
       <c r="B306" s="1"/>
       <c r="C306" s="1"/>
       <c r="D306" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E306" s="1"/>
+        <v>286</v>
+      </c>
+      <c r="E306" t="s">
+        <v>287</v>
+      </c>
       <c r="F306" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="G306" s="1"/>
     </row>
@@ -5212,11 +5222,11 @@
       <c r="B307" s="1"/>
       <c r="C307" s="1"/>
       <c r="D307" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E307" s="1"/>
       <c r="F307" s="1" t="s">
-        <v>63</v>
+        <v>242</v>
       </c>
       <c r="G307" s="1"/>
     </row>
@@ -5231,16 +5241,16 @@
     <row r="309" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B309" s="1"/>
       <c r="C309" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>148</v>
+        <v>300</v>
       </c>
       <c r="E309" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F309" s="1" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="G309" s="1"/>
     </row>
@@ -5248,13 +5258,13 @@
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
       <c r="D310" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E310" t="s">
-        <v>294</v>
+        <v>284</v>
+      </c>
+      <c r="E310" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="F310" s="1" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
       <c r="G310" s="1"/>
     </row>
@@ -5262,41 +5272,163 @@
       <c r="B311" s="1"/>
       <c r="C311" s="1"/>
       <c r="D311" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E311" s="1"/>
       <c r="F311" s="1" t="s">
-        <v>244</v>
+        <v>159</v>
       </c>
       <c r="G311" s="1"/>
     </row>
     <row r="312" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B312" s="1"/>
       <c r="C312" s="1"/>
-      <c r="D312" s="1"/>
+      <c r="D312" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="E312" s="1"/>
-      <c r="F312" s="1"/>
+      <c r="F312" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="G312" s="1"/>
     </row>
     <row r="313" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B313" s="1"/>
       <c r="C313" s="1"/>
-      <c r="D313" s="1"/>
+      <c r="D313" s="1" t="s">
+        <v>302</v>
+      </c>
       <c r="E313" s="1"/>
-      <c r="F313" s="1"/>
+      <c r="F313" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="G313" s="1"/>
     </row>
     <row r="314" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
-      <c r="D314" s="1"/>
+      <c r="D314" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="E314" s="1"/>
-      <c r="F314" s="1"/>
+      <c r="F314" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G314" s="1"/>
     </row>
+    <row r="315" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B315" s="1"/>
+      <c r="C315" s="1"/>
+      <c r="D315" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E315" s="1"/>
+      <c r="F315" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G315" s="1"/>
+    </row>
     <row r="316" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B316" t="s">
-        <v>155</v>
+      <c r="B316" s="1"/>
+      <c r="C316" s="1"/>
+      <c r="D316" s="1"/>
+      <c r="E316" s="1"/>
+      <c r="F316" s="1"/>
+      <c r="G316" s="1"/>
+    </row>
+    <row r="317" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B317" s="1"/>
+      <c r="C317" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F317" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G317" s="1"/>
+    </row>
+    <row r="318" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B318" s="1"/>
+      <c r="C318" s="1"/>
+      <c r="D318" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F318" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G318" s="1"/>
+    </row>
+    <row r="319" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B319" s="1"/>
+      <c r="C319" s="1"/>
+      <c r="D319" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E319" s="1"/>
+      <c r="F319" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G319" s="1"/>
+    </row>
+    <row r="320" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B320" s="1"/>
+      <c r="C320" s="1"/>
+      <c r="D320" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E320" s="1"/>
+      <c r="F320" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G320" s="1"/>
+    </row>
+    <row r="321" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B321" s="1"/>
+      <c r="C321" s="1"/>
+      <c r="D321" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E321" s="1"/>
+      <c r="F321" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G321" s="1"/>
+    </row>
+    <row r="322" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B322" s="1"/>
+      <c r="C322" s="1"/>
+      <c r="D322" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E322" s="1"/>
+      <c r="F322" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G322" s="1"/>
+    </row>
+    <row r="323" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B323" s="1"/>
+      <c r="C323" s="1"/>
+      <c r="D323" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E323" s="1"/>
+      <c r="F323" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G323" s="1"/>
+    </row>
+    <row r="325" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B325" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new fields and tables
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.beta.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,14 +11,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$302</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$304</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="302">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -251,9 +251,6 @@
     <t>harga beli</t>
   </si>
   <si>
-    <t>products_base_price</t>
-  </si>
-  <si>
     <t>products_sales_price</t>
   </si>
   <si>
@@ -326,9 +323,6 @@
     <t>purchase_id</t>
   </si>
   <si>
-    <t>products_price</t>
-  </si>
-  <si>
     <t>purchase_paid</t>
   </si>
   <si>
@@ -338,24 +332,9 @@
     <t>CREDIT</t>
   </si>
   <si>
-    <t>ro_id</t>
-  </si>
-  <si>
-    <t>products_baseprice</t>
-  </si>
-  <si>
     <t>PRODUCTS MOVEMENT</t>
   </si>
   <si>
-    <t>rp_invoice</t>
-  </si>
-  <si>
-    <t>rp_supplier_id</t>
-  </si>
-  <si>
-    <t>rp_datetime</t>
-  </si>
-  <si>
     <t>rp_total</t>
   </si>
   <si>
@@ -936,6 +915,15 @@
   </si>
   <si>
     <t>PAYMENT_CREDIT</t>
+  </si>
+  <si>
+    <t>product_price</t>
+  </si>
+  <si>
+    <t>product_baseprice</t>
+  </si>
+  <si>
+    <t>rp_date</t>
   </si>
 </sst>
 </file>
@@ -1068,7 +1056,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1103,7 +1091,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1315,10 +1303,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q325"/>
+  <dimension ref="B1:Q327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
-      <selection activeCell="D319" sqref="D319"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="F228" sqref="F228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1362,7 +1350,7 @@
         <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>54</v>
@@ -1376,7 +1364,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1400,13 +1388,13 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="H6" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1417,10 +1405,10 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H7" t="s">
         <v>64</v>
@@ -1436,7 +1424,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1447,16 +1435,16 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1464,13 +1452,13 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1478,11 +1466,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1490,11 +1478,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1502,11 +1490,11 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1514,11 +1502,11 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1526,13 +1514,13 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1540,14 +1528,14 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -1560,7 +1548,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1571,7 +1559,7 @@
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
@@ -1580,7 +1568,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1594,7 +1582,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1602,11 +1590,11 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1614,11 +1602,11 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1626,28 +1614,28 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -1680,7 +1668,7 @@
         <v>52</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>54</v>
@@ -1696,7 +1684,7 @@
         <v>61</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1704,13 +1692,13 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1722,7 +1710,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1734,7 +1722,7 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
@@ -1758,7 +1746,7 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1772,7 +1760,7 @@
         <v>5</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -1805,7 +1793,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G36" s="1"/>
       <c r="N36" t="s">
@@ -1826,7 +1814,7 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G37" s="1"/>
       <c r="N37" t="s">
@@ -1859,7 +1847,7 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1883,7 +1871,7 @@
         <v>52</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>54</v>
@@ -1902,7 +1890,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -1916,11 +1904,11 @@
         <v>5</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
@@ -1933,7 +1921,7 @@
         <v>57</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -1957,7 +1945,7 @@
         <v>52</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>54</v>
@@ -1973,7 +1961,7 @@
         <v>5</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -1987,7 +1975,7 @@
         <v>5</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -2001,7 +1989,7 @@
         <v>5</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -2009,11 +1997,11 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -2033,11 +2021,11 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -2045,13 +2033,13 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -2066,7 +2054,7 @@
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>2</v>
@@ -2075,22 +2063,22 @@
         <v>52</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -2105,7 +2093,7 @@
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>2</v>
@@ -2114,7 +2102,7 @@
         <v>52</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -2128,7 +2116,7 @@
         <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2136,11 +2124,11 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2148,31 +2136,31 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="K61" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2206,7 +2194,7 @@
         <v>52</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -2218,7 +2206,7 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -2226,11 +2214,11 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G67" s="1"/>
     </row>
@@ -2238,11 +2226,11 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G68" s="1"/>
     </row>
@@ -2250,11 +2238,11 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G69" s="1"/>
     </row>
@@ -2266,7 +2254,7 @@
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G70" s="1"/>
     </row>
@@ -2278,7 +2266,7 @@
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G71" s="1"/>
     </row>
@@ -2290,7 +2278,7 @@
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G72" s="1"/>
     </row>
@@ -2302,7 +2290,7 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G73" s="1"/>
     </row>
@@ -2310,11 +2298,11 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2322,35 +2310,35 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2367,7 +2355,7 @@
         <v>52</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G78" s="1"/>
     </row>
@@ -2375,13 +2363,13 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G79" s="1"/>
     </row>
@@ -2389,11 +2377,11 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G80" s="1"/>
     </row>
@@ -2401,11 +2389,11 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G81" s="1"/>
     </row>
@@ -2413,11 +2401,11 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -2425,11 +2413,11 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G83" s="1"/>
     </row>
@@ -2437,11 +2425,11 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G84" s="1"/>
     </row>
@@ -2475,7 +2463,7 @@
         <v>52</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>54</v>
@@ -2489,7 +2477,7 @@
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G88" s="1"/>
     </row>
@@ -2497,11 +2485,11 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G89" s="1"/>
     </row>
@@ -2509,11 +2497,11 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G90" s="1"/>
     </row>
@@ -2521,11 +2509,11 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G91" s="1"/>
     </row>
@@ -2537,7 +2525,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -2549,7 +2537,7 @@
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G93" s="1"/>
     </row>
@@ -2561,7 +2549,7 @@
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G94" s="1"/>
     </row>
@@ -2573,7 +2561,7 @@
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G95" s="1"/>
     </row>
@@ -2598,7 +2586,7 @@
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>2</v>
@@ -2607,7 +2595,7 @@
         <v>52</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>54</v>
@@ -2617,13 +2605,13 @@
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G99" s="1"/>
     </row>
@@ -2631,13 +2619,13 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G100" s="1"/>
     </row>
@@ -2645,11 +2633,11 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G101" s="1"/>
     </row>
@@ -2657,7 +2645,7 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
@@ -2669,11 +2657,11 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>76</v>
@@ -2683,69 +2671,69 @@
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G108" s="1"/>
     </row>
@@ -2753,11 +2741,11 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G109" s="1"/>
     </row>
@@ -2765,11 +2753,11 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G110" s="1"/>
     </row>
@@ -2777,11 +2765,11 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G111" s="1"/>
     </row>
@@ -2795,7 +2783,7 @@
         <v>5</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G112" s="1"/>
     </row>
@@ -2809,7 +2797,7 @@
         <v>5</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G113" s="1"/>
     </row>
@@ -2817,13 +2805,13 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E114" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E114" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="F114" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G114" s="1"/>
     </row>
@@ -2831,11 +2819,11 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G115" s="1"/>
     </row>
@@ -2843,11 +2831,11 @@
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G116" s="1"/>
     </row>
@@ -2855,25 +2843,25 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G118" s="1"/>
     </row>
@@ -2881,16 +2869,16 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
@@ -2904,16 +2892,16 @@
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G121" s="1"/>
     </row>
@@ -2921,13 +2909,13 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G122" s="1"/>
     </row>
@@ -2942,7 +2930,7 @@
     <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
       <c r="C124" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>2</v>
@@ -2951,7 +2939,7 @@
         <v>52</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G124" s="1"/>
     </row>
@@ -2965,7 +2953,7 @@
         <v>5</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G125" s="1"/>
     </row>
@@ -2977,7 +2965,7 @@
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G126" s="1"/>
     </row>
@@ -2989,11 +2977,11 @@
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="2:8" x14ac:dyDescent="0.25">
@@ -3004,7 +2992,7 @@
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G128" s="1"/>
     </row>
@@ -3019,7 +3007,7 @@
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>2</v>
@@ -3028,7 +3016,7 @@
         <v>52</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G130" s="1"/>
     </row>
@@ -3036,11 +3024,11 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G131" s="1"/>
     </row>
@@ -3048,13 +3036,13 @@
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G132" s="1"/>
     </row>
@@ -3062,11 +3050,11 @@
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G133" s="1"/>
     </row>
@@ -3074,13 +3062,13 @@
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G134" s="1"/>
     </row>
@@ -3088,11 +3076,11 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G135" s="1"/>
     </row>
@@ -3100,11 +3088,11 @@
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G136" s="1"/>
     </row>
@@ -3128,7 +3116,7 @@
         <v>52</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G138" s="1"/>
     </row>
@@ -3136,11 +3124,11 @@
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G139" s="1"/>
     </row>
@@ -3148,7 +3136,7 @@
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1" t="s">
@@ -3160,11 +3148,11 @@
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G141" s="1"/>
     </row>
@@ -3186,7 +3174,7 @@
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G143" s="1"/>
     </row>
@@ -3198,7 +3186,7 @@
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G144" s="1"/>
     </row>
@@ -3210,7 +3198,7 @@
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G145" s="1"/>
     </row>
@@ -3225,16 +3213,16 @@
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
       <c r="C147" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G147" s="1"/>
     </row>
@@ -3242,11 +3230,11 @@
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G148" s="1"/>
     </row>
@@ -3254,7 +3242,7 @@
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
@@ -3266,11 +3254,11 @@
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G150" s="1"/>
     </row>
@@ -3294,7 +3282,7 @@
         <v>52</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G152" s="1"/>
     </row>
@@ -3302,7 +3290,7 @@
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>61</v>
@@ -3322,7 +3310,7 @@
         <v>5</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G154" s="1"/>
     </row>
@@ -3334,7 +3322,7 @@
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G155" s="1"/>
     </row>
@@ -3346,7 +3334,7 @@
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G156" s="1"/>
     </row>
@@ -3354,11 +3342,11 @@
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E157" s="1"/>
       <c r="F157" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G157" s="1"/>
     </row>
@@ -3366,11 +3354,11 @@
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G158" s="1"/>
     </row>
@@ -3378,11 +3366,11 @@
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G159" s="1"/>
     </row>
@@ -3390,11 +3378,11 @@
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E160" s="1"/>
       <c r="F160" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G160" s="1"/>
     </row>
@@ -3402,7 +3390,7 @@
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
@@ -3422,13 +3410,13 @@
         <v>37</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G163" s="1"/>
     </row>
@@ -3436,7 +3424,7 @@
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>5</v>
@@ -3450,11 +3438,11 @@
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E165" s="1"/>
       <c r="F165" s="1" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="G165" s="1"/>
     </row>
@@ -3462,11 +3450,11 @@
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1" t="s">
-        <v>113</v>
+        <v>299</v>
       </c>
       <c r="E166" s="1"/>
       <c r="F166" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G166" s="1"/>
     </row>
@@ -3474,49 +3462,47 @@
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1" t="s">
-        <v>40</v>
+        <v>207</v>
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="G167" s="1"/>
     </row>
     <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
-      <c r="D168" s="1"/>
+      <c r="D168" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="E168" s="1"/>
-      <c r="F168" s="1"/>
+      <c r="F168" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="G168" s="1"/>
     </row>
     <row r="169" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B169" s="1"/>
-      <c r="C169" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
       <c r="G169" s="1"/>
     </row>
     <row r="170" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B170" s="1"/>
-      <c r="C170" s="1"/>
+      <c r="C170" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="D170" s="1" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="G170" s="1"/>
     </row>
@@ -3524,11 +3510,13 @@
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E171" s="1"/>
+        <v>94</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F171" s="1" t="s">
-        <v>197</v>
+        <v>62</v>
       </c>
       <c r="G171" s="1"/>
     </row>
@@ -3536,11 +3524,11 @@
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="E172" s="1"/>
       <c r="F172" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G172" s="1"/>
     </row>
@@ -3548,11 +3536,11 @@
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1" t="s">
-        <v>96</v>
+        <v>221</v>
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="G173" s="1"/>
     </row>
@@ -3560,11 +3548,11 @@
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E174" s="1"/>
       <c r="F174" s="1" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="G174" s="1"/>
     </row>
@@ -3572,11 +3560,11 @@
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1" t="s">
-        <v>159</v>
+        <v>214</v>
       </c>
       <c r="G175" s="1"/>
     </row>
@@ -3584,11 +3572,11 @@
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="G176" s="1"/>
     </row>
@@ -3596,49 +3584,47 @@
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1" t="s">
-        <v>268</v>
+        <v>99</v>
       </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G177" s="1"/>
     </row>
     <row r="178" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
-      <c r="D178" s="1"/>
+      <c r="D178" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="E178" s="1"/>
-      <c r="F178" s="1"/>
+      <c r="F178" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="G178" s="1"/>
     </row>
     <row r="179" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B179" s="1"/>
-      <c r="C179" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
       <c r="G179" s="1"/>
     </row>
     <row r="180" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B180" s="1"/>
-      <c r="C180" s="1"/>
+      <c r="C180" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="D180" s="1" t="s">
-        <v>106</v>
+        <v>2</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G180" s="1"/>
     </row>
@@ -3646,13 +3632,13 @@
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>223</v>
+        <v>62</v>
       </c>
       <c r="G181" s="1"/>
     </row>
@@ -3660,11 +3646,13 @@
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E182" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F182" s="1" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="G182" s="1"/>
     </row>
@@ -3672,11 +3660,11 @@
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
       <c r="E183" s="1"/>
       <c r="F183" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G183" s="1"/>
     </row>
@@ -3684,49 +3672,47 @@
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="G184" s="1"/>
     </row>
     <row r="185" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
-      <c r="D185" s="1"/>
+      <c r="D185" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="E185" s="1"/>
-      <c r="F185" s="1"/>
+      <c r="F185" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="G185" s="1"/>
     </row>
     <row r="186" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B186" s="1"/>
-      <c r="C186" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D186" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F186" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
+      <c r="E186" s="1"/>
+      <c r="F186" s="1"/>
       <c r="G186" s="1"/>
     </row>
     <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B187" s="1"/>
-      <c r="C187" s="1"/>
+      <c r="C187" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="D187" s="1" t="s">
-        <v>149</v>
+        <v>2</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="G187" s="1"/>
     </row>
@@ -3734,13 +3720,13 @@
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>197</v>
+        <v>62</v>
       </c>
       <c r="G188" s="1"/>
     </row>
@@ -3748,13 +3734,13 @@
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G189" s="1"/>
     </row>
@@ -3762,11 +3748,13 @@
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E190" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F190" s="1" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="G190" s="1"/>
     </row>
@@ -3774,11 +3762,11 @@
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="G191" s="1"/>
     </row>
@@ -3786,11 +3774,11 @@
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="E192" s="1"/>
       <c r="F192" s="1" t="s">
-        <v>62</v>
+        <v>214</v>
       </c>
       <c r="G192" s="1"/>
     </row>
@@ -3798,49 +3786,47 @@
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1" t="s">
-        <v>281</v>
+        <v>94</v>
       </c>
       <c r="E193" s="1"/>
       <c r="F193" s="1" t="s">
-        <v>283</v>
+        <v>62</v>
       </c>
       <c r="G193" s="1"/>
     </row>
     <row r="194" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
-      <c r="D194" s="1"/>
+      <c r="D194" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="E194" s="1"/>
-      <c r="F194" s="1"/>
+      <c r="F194" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="G194" s="1"/>
     </row>
     <row r="195" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B195" s="1"/>
-      <c r="C195" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D195" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F195" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="C195" s="1"/>
+      <c r="D195" s="1"/>
+      <c r="E195" s="1"/>
+      <c r="F195" s="1"/>
       <c r="G195" s="1"/>
     </row>
     <row r="196" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B196" s="1"/>
-      <c r="C196" s="1"/>
-      <c r="D196" s="1" t="s">
-        <v>148</v>
+      <c r="C196" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G196" s="1"/>
     </row>
@@ -3848,13 +3834,13 @@
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>223</v>
+        <v>62</v>
       </c>
       <c r="G197" s="1"/>
     </row>
@@ -3862,11 +3848,13 @@
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E198" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F198" s="1" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="G198" s="1"/>
     </row>
@@ -3874,11 +3862,11 @@
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G199" s="1"/>
     </row>
@@ -3886,49 +3874,47 @@
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="G200" s="1"/>
     </row>
     <row r="201" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
-      <c r="D201" s="1"/>
+      <c r="D201" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="E201" s="1"/>
-      <c r="F201" s="1"/>
+      <c r="F201" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="G201" s="1"/>
     </row>
     <row r="202" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B202" s="1"/>
-      <c r="C202" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D202" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E202" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F202" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="C202" s="1"/>
+      <c r="D202" s="1"/>
+      <c r="E202" s="1"/>
+      <c r="F202" s="1"/>
       <c r="G202" s="1"/>
     </row>
     <row r="203" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
-      <c r="C203" s="1"/>
+      <c r="C203" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="D203" s="1" t="s">
-        <v>270</v>
+        <v>2</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="G203" s="1"/>
     </row>
@@ -3936,13 +3922,13 @@
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>197</v>
+        <v>62</v>
       </c>
       <c r="G204" s="1"/>
     </row>
@@ -3950,13 +3936,13 @@
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G205" s="1"/>
     </row>
@@ -3964,11 +3950,13 @@
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E206" s="1"/>
+        <v>265</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F206" s="1" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="G206" s="1"/>
     </row>
@@ -3976,11 +3964,11 @@
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="E207" s="1"/>
       <c r="F207" s="1" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="G207" s="1"/>
     </row>
@@ -3988,13 +3976,11 @@
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="E208" s="1"/>
       <c r="F208" s="1" t="s">
-        <v>62</v>
+        <v>214</v>
       </c>
       <c r="G208" s="1"/>
     </row>
@@ -4002,7 +3988,7 @@
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>61</v>
@@ -4015,38 +4001,38 @@
     <row r="210" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
-      <c r="D210" s="1"/>
-      <c r="E210" s="1"/>
-      <c r="F210" s="1"/>
+      <c r="D210" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="G210" s="1"/>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B211" s="1"/>
-      <c r="C211" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F211" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="C211" s="1"/>
+      <c r="D211" s="1"/>
+      <c r="E211" s="1"/>
+      <c r="F211" s="1"/>
       <c r="G211" s="1"/>
     </row>
     <row r="212" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
-      <c r="C212" s="1"/>
+      <c r="C212" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="D212" s="1" t="s">
-        <v>270</v>
+        <v>2</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="G212" s="1"/>
     </row>
@@ -4054,13 +4040,11 @@
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="E213" s="1"/>
       <c r="F213" s="1" t="s">
-        <v>223</v>
+        <v>62</v>
       </c>
       <c r="G213" s="1"/>
     </row>
@@ -4068,11 +4052,13 @@
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E214" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F214" s="1" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -4080,11 +4066,11 @@
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>214</v>
+        <v>158</v>
       </c>
       <c r="E215" s="1"/>
       <c r="F215" s="1" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G215" s="1"/>
     </row>
@@ -4092,11 +4078,11 @@
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>276</v>
+        <v>207</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G216" s="1"/>
     </row>
@@ -4104,11 +4090,11 @@
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="G217" s="1"/>
     </row>
@@ -4116,52 +4102,50 @@
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="1" t="s">
-        <v>279</v>
+        <v>214</v>
       </c>
       <c r="G218" s="1"/>
-      <c r="H218" t="s">
-        <v>280</v>
-      </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
-      <c r="D219" s="1"/>
+      <c r="D219" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="E219" s="1"/>
-      <c r="F219" s="1"/>
+      <c r="F219" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="G219" s="1"/>
+      <c r="H219" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="220" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B220" s="1"/>
-      <c r="C220" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="E220" s="1"/>
+      <c r="F220" s="1"/>
       <c r="G220" s="1"/>
     </row>
     <row r="221" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B221" s="1"/>
-      <c r="C221" s="1"/>
+      <c r="C221" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="D221" s="1" t="s">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="G221" s="1"/>
     </row>
@@ -4169,13 +4153,13 @@
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>219</v>
+        <v>62</v>
       </c>
       <c r="G222" s="1"/>
     </row>
@@ -4183,11 +4167,13 @@
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E223" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F223" s="1" t="s">
-        <v>159</v>
+        <v>212</v>
       </c>
       <c r="G223" s="1"/>
     </row>
@@ -4195,11 +4181,11 @@
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1" t="s">
-        <v>112</v>
+        <v>301</v>
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="G224" s="1"/>
     </row>
@@ -4207,49 +4193,47 @@
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="E225" s="1"/>
       <c r="F225" s="1" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="G225" s="1"/>
     </row>
     <row r="226" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
-      <c r="D226" s="1"/>
+      <c r="D226" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="E226" s="1"/>
-      <c r="F226" s="1"/>
+      <c r="F226" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="G226" s="1"/>
     </row>
     <row r="227" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B227" s="1"/>
-      <c r="C227" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="C227" s="1"/>
+      <c r="D227" s="1"/>
+      <c r="E227" s="1"/>
+      <c r="F227" s="1"/>
       <c r="G227" s="1"/>
     </row>
     <row r="228" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B228" s="1"/>
-      <c r="C228" s="1"/>
+      <c r="C228" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="D228" s="1" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G228" s="1"/>
     </row>
@@ -4257,11 +4241,11 @@
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E229" s="1"/>
       <c r="F229" s="1" t="s">
-        <v>221</v>
+        <v>62</v>
       </c>
       <c r="G229" s="1"/>
     </row>
@@ -4269,11 +4253,13 @@
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
       <c r="D230" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E230" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F230" s="1" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="G230" s="1"/>
     </row>
@@ -4281,11 +4267,11 @@
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1" t="s">
-        <v>118</v>
+        <v>300</v>
       </c>
       <c r="E231" s="1"/>
       <c r="F231" s="1" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="G231" s="1"/>
     </row>
@@ -4293,63 +4279,59 @@
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
       <c r="D232" s="1" t="s">
-        <v>117</v>
+        <v>207</v>
       </c>
       <c r="E232" s="1"/>
       <c r="F232" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="G232" s="1"/>
     </row>
     <row r="233" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
-      <c r="D233" s="1"/>
+      <c r="D233" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="E233" s="1"/>
-      <c r="F233" s="1"/>
+      <c r="F233" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G233" s="1"/>
     </row>
     <row r="234" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B234" s="1"/>
-      <c r="C234" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="C234" s="1"/>
       <c r="D234" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E234" s="1"/>
       <c r="F234" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="G234" s="1"/>
     </row>
     <row r="235" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
-      <c r="D235" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E235" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F235" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="D235" s="1"/>
+      <c r="E235" s="1"/>
+      <c r="F235" s="1"/>
       <c r="G235" s="1"/>
     </row>
     <row r="236" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B236" s="1"/>
-      <c r="C236" s="1"/>
+      <c r="C236" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="D236" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G236" s="1"/>
     </row>
@@ -4357,11 +4339,13 @@
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
       <c r="D237" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E237" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F237" s="1" t="s">
-        <v>159</v>
+        <v>62</v>
       </c>
       <c r="G237" s="1"/>
     </row>
@@ -4369,11 +4353,13 @@
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E238" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F238" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="G238" s="1"/>
     </row>
@@ -4381,11 +4367,11 @@
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E239" s="1"/>
       <c r="F239" s="1" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="G239" s="1"/>
     </row>
@@ -4393,11 +4379,11 @@
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
       <c r="D240" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="G240" s="1"/>
     </row>
@@ -4405,11 +4391,11 @@
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
       <c r="D241" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E241" s="1"/>
       <c r="F241" s="1" t="s">
-        <v>159</v>
+        <v>214</v>
       </c>
       <c r="G241" s="1"/>
     </row>
@@ -4417,61 +4403,59 @@
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
       <c r="D242" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E242" s="1"/>
       <c r="F242" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G242" s="1"/>
     </row>
     <row r="243" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
-      <c r="D243" s="1"/>
+      <c r="D243" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="E243" s="1"/>
-      <c r="F243" s="1"/>
+      <c r="F243" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="G243" s="1"/>
     </row>
     <row r="244" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B244" s="1"/>
-      <c r="C244" s="1" t="s">
+      <c r="C244" s="1"/>
+      <c r="D244" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D244" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E244" s="1"/>
       <c r="F244" s="1" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="G244" s="1"/>
     </row>
     <row r="245" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
-      <c r="D245" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E245" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F245" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="D245" s="1"/>
+      <c r="E245" s="1"/>
+      <c r="F245" s="1"/>
       <c r="G245" s="1"/>
     </row>
     <row r="246" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B246" s="1"/>
-      <c r="C246" s="1"/>
+      <c r="C246" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="D246" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E246" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F246" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G246" s="1"/>
     </row>
@@ -4479,11 +4463,13 @@
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E247" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F247" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G247" s="1"/>
     </row>
@@ -4491,11 +4477,11 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1" t="s">
-        <v>190</v>
+        <v>77</v>
       </c>
       <c r="E248" s="1"/>
       <c r="F248" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="G248" s="1"/>
     </row>
@@ -4503,11 +4489,11 @@
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
       <c r="D249" s="1" t="s">
-        <v>191</v>
+        <v>106</v>
       </c>
       <c r="E249" s="1"/>
       <c r="F249" s="1" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="G249" s="1"/>
     </row>
@@ -4515,11 +4501,11 @@
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G250" s="1"/>
     </row>
@@ -4527,63 +4513,59 @@
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G251" s="1"/>
     </row>
     <row r="252" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
-      <c r="D252" s="1"/>
+      <c r="D252" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="E252" s="1"/>
-      <c r="F252" s="1"/>
+      <c r="F252" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="G252" s="1"/>
     </row>
     <row r="253" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B253" s="1"/>
-      <c r="C253" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="C253" s="1"/>
       <c r="D253" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E253" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="E253" s="1"/>
       <c r="F253" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="G253" s="1"/>
     </row>
     <row r="254" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
-      <c r="D254" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F254" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="D254" s="1"/>
+      <c r="E254" s="1"/>
+      <c r="F254" s="1"/>
       <c r="G254" s="1"/>
     </row>
     <row r="255" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B255" s="1"/>
-      <c r="C255" s="1"/>
+      <c r="C255" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="D255" s="1" t="s">
-        <v>229</v>
+        <v>2</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G255" s="1"/>
     </row>
@@ -4591,11 +4573,13 @@
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
       <c r="D256" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E256" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F256" s="1" t="s">
-        <v>159</v>
+        <v>62</v>
       </c>
       <c r="G256" s="1"/>
     </row>
@@ -4603,61 +4587,61 @@
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
       <c r="D257" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E257" s="1"/>
+        <v>222</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F257" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="G257" s="1"/>
     </row>
     <row r="258" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B258" s="1"/>
       <c r="C258" s="1"/>
-      <c r="D258" s="1"/>
+      <c r="D258" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="E258" s="1"/>
-      <c r="F258" s="1"/>
+      <c r="F258" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="G258" s="1"/>
     </row>
     <row r="259" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B259" s="1"/>
-      <c r="C259" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="C259" s="1"/>
       <c r="D259" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E259" s="1"/>
       <c r="F259" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="G259" s="1"/>
     </row>
     <row r="260" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
-      <c r="D260" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F260" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="D260" s="1"/>
+      <c r="E260" s="1"/>
+      <c r="F260" s="1"/>
       <c r="G260" s="1"/>
     </row>
     <row r="261" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
+      <c r="C261" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="D261" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E261" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F261" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G261" s="1"/>
     </row>
@@ -4665,11 +4649,13 @@
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
       <c r="D262" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E262" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F262" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G262" s="1"/>
     </row>
@@ -4677,11 +4663,11 @@
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
       <c r="D263" s="1" t="s">
-        <v>191</v>
+        <v>77</v>
       </c>
       <c r="E263" s="1"/>
       <c r="F263" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="G263" s="1"/>
     </row>
@@ -4689,11 +4675,11 @@
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
       <c r="D264" s="1" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E264" s="1"/>
       <c r="F264" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G264" s="1"/>
     </row>
@@ -4701,11 +4687,11 @@
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
       <c r="D265" s="1" t="s">
-        <v>113</v>
+        <v>184</v>
       </c>
       <c r="E265" s="1"/>
       <c r="F265" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G265" s="1"/>
     </row>
@@ -4713,11 +4699,11 @@
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
       <c r="D266" s="1" t="s">
-        <v>127</v>
+        <v>185</v>
       </c>
       <c r="E266" s="1"/>
       <c r="F266" s="1" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="G266" s="1"/>
     </row>
@@ -4725,63 +4711,59 @@
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
       <c r="D267" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="E267" s="1"/>
       <c r="F267" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="G267" s="1"/>
     </row>
     <row r="268" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
-      <c r="D268" s="1"/>
+      <c r="D268" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="E268" s="1"/>
-      <c r="F268" s="1"/>
+      <c r="F268" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G268" s="1"/>
     </row>
     <row r="269" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B269" s="1"/>
-      <c r="C269" s="1" t="s">
-        <v>194</v>
-      </c>
+      <c r="C269" s="1"/>
       <c r="D269" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E269" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="E269" s="1"/>
       <c r="F269" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="G269" s="1"/>
     </row>
     <row r="270" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
-      <c r="D270" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="E270" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F270" s="1" t="s">
-        <v>219</v>
-      </c>
+      <c r="D270" s="1"/>
+      <c r="E270" s="1"/>
+      <c r="F270" s="1"/>
       <c r="G270" s="1"/>
     </row>
     <row r="271" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B271" s="1"/>
-      <c r="C271" s="1"/>
+      <c r="C271" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="D271" s="1" t="s">
-        <v>124</v>
+        <v>2</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F271" s="1" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="G271" s="1"/>
     </row>
@@ -4789,61 +4771,63 @@
       <c r="B272" s="1"/>
       <c r="C272" s="1"/>
       <c r="D272" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E272" s="1"/>
+        <v>222</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F272" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="G272" s="1"/>
     </row>
     <row r="273" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
-      <c r="D273" s="1"/>
-      <c r="E273" s="1"/>
-      <c r="F273" s="1"/>
+      <c r="D273" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F273" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="G273" s="1"/>
     </row>
     <row r="274" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B274" s="1"/>
-      <c r="C274" s="1" t="s">
-        <v>195</v>
-      </c>
+      <c r="C274" s="1"/>
       <c r="D274" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E274" s="1"/>
       <c r="F274" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="G274" s="1"/>
     </row>
     <row r="275" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
-      <c r="D275" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E275" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F275" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="D275" s="1"/>
+      <c r="E275" s="1"/>
+      <c r="F275" s="1"/>
       <c r="G275" s="1"/>
     </row>
     <row r="276" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B276" s="1"/>
-      <c r="C276" s="1"/>
+      <c r="C276" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="D276" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E276" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F276" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G276" s="1"/>
     </row>
@@ -4851,11 +4835,13 @@
       <c r="B277" s="1"/>
       <c r="C277" s="1"/>
       <c r="D277" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E277" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F277" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G277" s="1"/>
     </row>
@@ -4863,11 +4849,11 @@
       <c r="B278" s="1"/>
       <c r="C278" s="1"/>
       <c r="D278" s="1" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="E278" s="1"/>
       <c r="F278" s="1" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="G278" s="1"/>
     </row>
@@ -4875,124 +4861,122 @@
       <c r="B279" s="1"/>
       <c r="C279" s="1"/>
       <c r="D279" s="1" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="E279" s="1"/>
       <c r="F279" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="G279" s="1"/>
     </row>
     <row r="280" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B280" s="1"/>
       <c r="C280" s="1"/>
-      <c r="D280" s="1"/>
+      <c r="D280" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="E280" s="1"/>
-      <c r="F280" s="1"/>
+      <c r="F280" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G280" s="1"/>
     </row>
     <row r="281" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B281" s="1"/>
       <c r="C281" s="1"/>
-      <c r="D281" s="1"/>
+      <c r="D281" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="E281" s="1"/>
-      <c r="F281" s="1"/>
+      <c r="F281" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="G281" s="1"/>
     </row>
     <row r="282" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B282" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C282" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D282" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E282" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F282" s="1" t="s">
-        <v>219</v>
-      </c>
+      <c r="B282" s="1"/>
+      <c r="C282" s="1"/>
+      <c r="D282" s="1"/>
+      <c r="E282" s="1"/>
+      <c r="F282" s="1"/>
       <c r="G282" s="1"/>
     </row>
     <row r="283" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B283" s="1"/>
       <c r="C283" s="1"/>
-      <c r="D283" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F283" s="1" t="s">
-        <v>242</v>
-      </c>
+      <c r="D283" s="1"/>
+      <c r="E283" s="1"/>
+      <c r="F283" s="1"/>
       <c r="G283" s="1"/>
-      <c r="H283" t="s">
-        <v>234</v>
-      </c>
     </row>
     <row r="284" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B284" s="1"/>
-      <c r="C284" s="1"/>
+      <c r="B284" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="D284" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E284" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F284" s="1" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="G284" s="1"/>
     </row>
     <row r="285" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B285" s="1"/>
       <c r="C285" s="1"/>
-      <c r="D285" s="1"/>
-      <c r="E285" s="1"/>
-      <c r="F285" s="1"/>
+      <c r="D285" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F285" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="G285" s="1"/>
+      <c r="H285" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="286" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B286" s="1"/>
-      <c r="C286" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="C286" s="1"/>
       <c r="D286" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E286" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="E286" s="1"/>
       <c r="F286" s="1" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="G286" s="1"/>
     </row>
     <row r="287" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
-      <c r="D287" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E287" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F287" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="D287" s="1"/>
+      <c r="E287" s="1"/>
+      <c r="F287" s="1"/>
       <c r="G287" s="1"/>
     </row>
     <row r="288" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B288" s="1"/>
-      <c r="C288" s="1"/>
+      <c r="C288" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D288" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="E288" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F288" s="1" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="G288" s="1"/>
     </row>
@@ -5000,11 +4984,13 @@
       <c r="B289" s="1"/>
       <c r="C289" s="1"/>
       <c r="D289" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E289" s="1"/>
+        <v>223</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F289" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G289" s="1"/>
     </row>
@@ -5012,61 +4998,59 @@
       <c r="B290" s="1"/>
       <c r="C290" s="1"/>
       <c r="D290" s="1" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="E290" s="1"/>
       <c r="F290" s="1" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="G290" s="1"/>
     </row>
     <row r="291" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
-      <c r="D291" s="1"/>
+      <c r="D291" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="E291" s="1"/>
-      <c r="F291" s="1"/>
+      <c r="F291" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="G291" s="1"/>
     </row>
     <row r="292" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B292" s="1"/>
-      <c r="C292" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="C292" s="1"/>
       <c r="D292" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="E292" s="1"/>
       <c r="F292" s="1" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="G292" s="1"/>
     </row>
     <row r="293" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B293" s="1"/>
       <c r="C293" s="1"/>
-      <c r="D293" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E293" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F293" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="D293" s="1"/>
+      <c r="E293" s="1"/>
+      <c r="F293" s="1"/>
       <c r="G293" s="1"/>
     </row>
     <row r="294" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B294" s="1"/>
-      <c r="C294" s="1"/>
+      <c r="C294" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="D294" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="E294" s="1"/>
+        <v>278</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F294" s="1" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="G294" s="1"/>
     </row>
@@ -5074,11 +5058,13 @@
       <c r="B295" s="1"/>
       <c r="C295" s="1"/>
       <c r="D295" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E295" s="1"/>
+        <v>224</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F295" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="G295" s="1"/>
     </row>
@@ -5086,61 +5072,59 @@
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
       <c r="D296" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E296" s="1"/>
       <c r="F296" s="1" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="G296" s="1"/>
     </row>
     <row r="297" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
-      <c r="D297" s="1"/>
+      <c r="D297" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E297" s="1"/>
-      <c r="F297" s="1"/>
+      <c r="F297" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="G297" s="1"/>
     </row>
     <row r="298" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B298" s="1"/>
-      <c r="C298" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="C298" s="1"/>
       <c r="D298" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="E298" s="1"/>
       <c r="F298" s="1" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="G298" s="1"/>
     </row>
     <row r="299" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B299" s="1"/>
       <c r="C299" s="1"/>
-      <c r="D299" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E299" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F299" s="1" t="s">
-        <v>219</v>
-      </c>
+      <c r="D299" s="1"/>
+      <c r="E299" s="1"/>
+      <c r="F299" s="1"/>
       <c r="G299" s="1"/>
     </row>
     <row r="300" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B300" s="1"/>
-      <c r="C300" s="1"/>
+      <c r="C300" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="D300" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E300" s="1"/>
+        <v>281</v>
+      </c>
+      <c r="E300" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F300" s="1" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="G300" s="1"/>
     </row>
@@ -5148,11 +5132,13 @@
       <c r="B301" s="1"/>
       <c r="C301" s="1"/>
       <c r="D301" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E301" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F301" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="G301" s="1"/>
     </row>
@@ -5160,11 +5146,11 @@
       <c r="B302" s="1"/>
       <c r="C302" s="1"/>
       <c r="D302" s="1" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="E302" s="1"/>
       <c r="F302" s="1" t="s">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="G302" s="1"/>
     </row>
@@ -5172,111 +5158,109 @@
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
       <c r="D303" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="E303" s="1"/>
       <c r="F303" s="1" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="G303" s="1"/>
     </row>
     <row r="304" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B304" s="1"/>
       <c r="C304" s="1"/>
-      <c r="D304" s="1"/>
+      <c r="D304" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="E304" s="1"/>
-      <c r="F304" s="1"/>
+      <c r="F304" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="G304" s="1"/>
     </row>
     <row r="305" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B305" s="1"/>
-      <c r="C305" s="1" t="s">
-        <v>294</v>
-      </c>
+      <c r="C305" s="1"/>
       <c r="D305" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E305" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="E305" s="1"/>
       <c r="F305" s="1" t="s">
-        <v>197</v>
+        <v>63</v>
       </c>
       <c r="G305" s="1"/>
     </row>
     <row r="306" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B306" s="1"/>
       <c r="C306" s="1"/>
-      <c r="D306" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E306" t="s">
-        <v>287</v>
-      </c>
-      <c r="F306" s="1" t="s">
-        <v>204</v>
-      </c>
+      <c r="D306" s="1"/>
+      <c r="E306" s="1"/>
+      <c r="F306" s="1"/>
       <c r="G306" s="1"/>
     </row>
     <row r="307" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B307" s="1"/>
-      <c r="C307" s="1"/>
+      <c r="C307" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="D307" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E307" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F307" s="1" t="s">
-        <v>242</v>
+        <v>190</v>
       </c>
       <c r="G307" s="1"/>
     </row>
     <row r="308" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B308" s="1"/>
       <c r="C308" s="1"/>
-      <c r="D308" s="1"/>
-      <c r="E308" s="1"/>
-      <c r="F308" s="1"/>
+      <c r="D308" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E308" t="s">
+        <v>280</v>
+      </c>
+      <c r="F308" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="G308" s="1"/>
     </row>
     <row r="309" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B309" s="1"/>
-      <c r="C309" s="1" t="s">
-        <v>299</v>
-      </c>
+      <c r="C309" s="1"/>
       <c r="D309" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E309" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="E309" s="1"/>
       <c r="F309" s="1" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="G309" s="1"/>
     </row>
     <row r="310" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
-      <c r="D310" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E310" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F310" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="D310" s="1"/>
+      <c r="E310" s="1"/>
+      <c r="F310" s="1"/>
       <c r="G310" s="1"/>
     </row>
     <row r="311" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B311" s="1"/>
-      <c r="C311" s="1"/>
+      <c r="C311" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="D311" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E311" s="1"/>
+        <v>293</v>
+      </c>
+      <c r="E311" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F311" s="1" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="G311" s="1"/>
     </row>
@@ -5284,11 +5268,13 @@
       <c r="B312" s="1"/>
       <c r="C312" s="1"/>
       <c r="D312" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E312" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="E312" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F312" s="1" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="G312" s="1"/>
     </row>
@@ -5296,11 +5282,11 @@
       <c r="B313" s="1"/>
       <c r="C313" s="1"/>
       <c r="D313" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E313" s="1"/>
       <c r="F313" s="1" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="G313" s="1"/>
     </row>
@@ -5308,11 +5294,11 @@
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
       <c r="D314" s="1" t="s">
-        <v>303</v>
+        <v>141</v>
       </c>
       <c r="E314" s="1"/>
       <c r="F314" s="1" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="G314" s="1"/>
     </row>
@@ -5320,61 +5306,59 @@
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
       <c r="D315" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E315" s="1"/>
       <c r="F315" s="1" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="G315" s="1"/>
     </row>
     <row r="316" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B316" s="1"/>
       <c r="C316" s="1"/>
-      <c r="D316" s="1"/>
+      <c r="D316" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="E316" s="1"/>
-      <c r="F316" s="1"/>
+      <c r="F316" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G316" s="1"/>
     </row>
     <row r="317" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B317" s="1"/>
-      <c r="C317" s="1" t="s">
-        <v>305</v>
-      </c>
+      <c r="C317" s="1"/>
       <c r="D317" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E317" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="E317" s="1"/>
       <c r="F317" s="1" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
       <c r="G317" s="1"/>
     </row>
     <row r="318" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
-      <c r="D318" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E318" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F318" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="D318" s="1"/>
+      <c r="E318" s="1"/>
+      <c r="F318" s="1"/>
       <c r="G318" s="1"/>
     </row>
     <row r="319" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B319" s="1"/>
-      <c r="C319" s="1"/>
+      <c r="C319" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="D319" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E319" s="1"/>
+        <v>293</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F319" s="1" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="G319" s="1"/>
     </row>
@@ -5382,11 +5366,13 @@
       <c r="B320" s="1"/>
       <c r="C320" s="1"/>
       <c r="D320" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E320" s="1"/>
+        <v>278</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F320" s="1" t="s">
-        <v>197</v>
+        <v>216</v>
       </c>
       <c r="G320" s="1"/>
     </row>
@@ -5394,11 +5380,11 @@
       <c r="B321" s="1"/>
       <c r="C321" s="1"/>
       <c r="D321" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E321" s="1"/>
       <c r="F321" s="1" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="G321" s="1"/>
     </row>
@@ -5406,11 +5392,11 @@
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
       <c r="D322" s="1" t="s">
-        <v>303</v>
+        <v>141</v>
       </c>
       <c r="E322" s="1"/>
       <c r="F322" s="1" t="s">
-        <v>63</v>
+        <v>190</v>
       </c>
       <c r="G322" s="1"/>
     </row>
@@ -5418,17 +5404,41 @@
       <c r="B323" s="1"/>
       <c r="C323" s="1"/>
       <c r="D323" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="E323" s="1"/>
       <c r="F323" s="1" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="G323" s="1"/>
     </row>
+    <row r="324" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B324" s="1"/>
+      <c r="C324" s="1"/>
+      <c r="D324" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E324" s="1"/>
+      <c r="F324" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G324" s="1"/>
+    </row>
     <row r="325" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B325" t="s">
-        <v>153</v>
+      <c r="B325" s="1"/>
+      <c r="C325" s="1"/>
+      <c r="D325" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E325" s="1"/>
+      <c r="F325" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G325" s="1"/>
+    </row>
+    <row r="327" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B327" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Table for Sales
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Database Design_v1.beta.xlsx
+++ b/_DOCUMENTS_/Database Design_v1.beta.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$304</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$305</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="302">
   <si>
     <t>USER LEVEL MANAGEMENT</t>
   </si>
@@ -401,9 +401,6 @@
     <t>sales_invoice</t>
   </si>
   <si>
-    <t>sales_datetime</t>
-  </si>
-  <si>
     <t>sales_total</t>
   </si>
   <si>
@@ -419,9 +416,6 @@
     <t>sales_paid</t>
   </si>
   <si>
-    <t>sales_id</t>
-  </si>
-  <si>
     <t>PRODUCTS MUTATION HEADER</t>
   </si>
   <si>
@@ -924,6 +918,12 @@
   </si>
   <si>
     <t>rp_date</t>
+  </si>
+  <si>
+    <t>sales_date</t>
+  </si>
+  <si>
+    <t>product_sales_price</t>
   </si>
 </sst>
 </file>
@@ -1303,10 +1303,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q327"/>
+  <dimension ref="B1:Q328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="F228" sqref="F228"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="D246" sqref="D246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1350,7 +1350,7 @@
         <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>54</v>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1388,13 +1388,13 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -1405,10 +1405,10 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H7" t="s">
         <v>64</v>
@@ -1444,7 +1444,7 @@
         <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1455,10 +1455,10 @@
         <v>87</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1466,11 +1466,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -1478,11 +1478,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -1490,11 +1490,11 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1514,13 +1514,13 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1528,14 +1528,14 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1559,7 +1559,7 @@
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>2</v>
@@ -1568,7 +1568,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1582,7 +1582,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1590,11 +1590,11 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1602,11 +1602,11 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1614,28 +1614,28 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>52</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>54</v>
@@ -1684,7 +1684,7 @@
         <v>61</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1692,13 +1692,13 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1760,7 +1760,7 @@
         <v>5</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -1793,7 +1793,7 @@
         <v>52</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G36" s="1"/>
       <c r="N36" t="s">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G37" s="1"/>
       <c r="N37" t="s">
@@ -1847,7 +1847,7 @@
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1871,7 +1871,7 @@
         <v>52</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>54</v>
@@ -1890,7 +1890,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -1904,11 +1904,11 @@
         <v>5</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.25">
@@ -1921,7 +1921,7 @@
         <v>57</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G44" s="1"/>
     </row>
@@ -1945,7 +1945,7 @@
         <v>52</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>54</v>
@@ -1961,7 +1961,7 @@
         <v>5</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G47" s="1"/>
     </row>
@@ -1975,7 +1975,7 @@
         <v>5</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G48" s="1"/>
     </row>
@@ -1989,7 +1989,7 @@
         <v>5</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -1997,11 +1997,11 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -2021,11 +2021,11 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G52" s="1"/>
     </row>
@@ -2033,13 +2033,13 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G53" s="1"/>
     </row>
@@ -2054,7 +2054,7 @@
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>2</v>
@@ -2063,22 +2063,22 @@
         <v>52</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G56" s="1"/>
     </row>
@@ -2093,7 +2093,7 @@
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>2</v>
@@ -2102,7 +2102,7 @@
         <v>52</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G58" s="1"/>
     </row>
@@ -2116,7 +2116,7 @@
         <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -2124,11 +2124,11 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G60" s="1"/>
     </row>
@@ -2142,25 +2142,25 @@
         <v>5</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K61" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G62" s="1"/>
     </row>
@@ -2194,7 +2194,7 @@
         <v>52</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G65" s="1"/>
     </row>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -2214,11 +2214,11 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G67" s="1"/>
     </row>
@@ -2226,11 +2226,11 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G68" s="1"/>
     </row>
@@ -2238,11 +2238,11 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G69" s="1"/>
     </row>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G70" s="1"/>
     </row>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G71" s="1"/>
     </row>
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G72" s="1"/>
     </row>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G73" s="1"/>
     </row>
@@ -2298,11 +2298,11 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G74" s="1"/>
     </row>
@@ -2310,35 +2310,35 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -2355,7 +2355,7 @@
         <v>52</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G78" s="1"/>
     </row>
@@ -2369,7 +2369,7 @@
         <v>5</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G79" s="1"/>
     </row>
@@ -2377,11 +2377,11 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G80" s="1"/>
     </row>
@@ -2389,11 +2389,11 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G81" s="1"/>
     </row>
@@ -2401,11 +2401,11 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G82" s="1"/>
     </row>
@@ -2413,11 +2413,11 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G83" s="1"/>
     </row>
@@ -2425,11 +2425,11 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G84" s="1"/>
     </row>
@@ -2463,7 +2463,7 @@
         <v>52</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>54</v>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G88" s="1"/>
     </row>
@@ -2485,11 +2485,11 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G89" s="1"/>
     </row>
@@ -2497,11 +2497,11 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G90" s="1"/>
     </row>
@@ -2509,11 +2509,11 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G91" s="1"/>
     </row>
@@ -2525,7 +2525,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G92" s="1"/>
     </row>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G93" s="1"/>
     </row>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G94" s="1"/>
     </row>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G95" s="1"/>
     </row>
@@ -2586,7 +2586,7 @@
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>2</v>
@@ -2595,7 +2595,7 @@
         <v>52</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>54</v>
@@ -2611,7 +2611,7 @@
         <v>61</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G99" s="1"/>
     </row>
@@ -2619,13 +2619,13 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>61</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G100" s="1"/>
     </row>
@@ -2633,11 +2633,11 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G101" s="1"/>
     </row>
@@ -2645,7 +2645,7 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1" t="s">
@@ -2657,11 +2657,11 @@
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>76</v>
@@ -2671,69 +2671,69 @@
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G108" s="1"/>
     </row>
@@ -2741,11 +2741,11 @@
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E109" s="5"/>
       <c r="F109" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G109" s="1"/>
     </row>
@@ -2753,11 +2753,11 @@
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E110" s="5"/>
       <c r="F110" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G110" s="1"/>
     </row>
@@ -2765,11 +2765,11 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E111" s="5"/>
       <c r="F111" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G111" s="1"/>
     </row>
@@ -2783,7 +2783,7 @@
         <v>5</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G112" s="1"/>
     </row>
@@ -2797,7 +2797,7 @@
         <v>5</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G113" s="1"/>
     </row>
@@ -2805,13 +2805,13 @@
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G114" s="1"/>
     </row>
@@ -2819,11 +2819,11 @@
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G115" s="1"/>
     </row>
@@ -2831,11 +2831,11 @@
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G116" s="1"/>
     </row>
@@ -2843,25 +2843,25 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G118" s="1"/>
     </row>
@@ -2869,16 +2869,16 @@
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
@@ -2892,7 +2892,7 @@
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>78</v>
@@ -2901,7 +2901,7 @@
         <v>52</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G121" s="1"/>
     </row>
@@ -2909,13 +2909,13 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G122" s="1"/>
     </row>
@@ -2939,7 +2939,7 @@
         <v>52</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G124" s="1"/>
     </row>
@@ -2953,7 +2953,7 @@
         <v>5</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G125" s="1"/>
     </row>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G126" s="1"/>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G127" s="1"/>
       <c r="H127" t="s">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G128" s="1"/>
     </row>
@@ -3007,7 +3007,7 @@
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>2</v>
@@ -3016,7 +3016,7 @@
         <v>52</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G130" s="1"/>
     </row>
@@ -3024,11 +3024,11 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G131" s="1"/>
     </row>
@@ -3042,7 +3042,7 @@
         <v>5</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G132" s="1"/>
     </row>
@@ -3050,11 +3050,11 @@
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G133" s="1"/>
     </row>
@@ -3062,13 +3062,13 @@
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G134" s="1"/>
     </row>
@@ -3076,11 +3076,11 @@
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G135" s="1"/>
     </row>
@@ -3088,11 +3088,11 @@
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G136" s="1"/>
     </row>
@@ -3116,7 +3116,7 @@
         <v>52</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G138" s="1"/>
     </row>
@@ -3128,7 +3128,7 @@
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G139" s="1"/>
     </row>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G141" s="1"/>
     </row>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G143" s="1"/>
     </row>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G144" s="1"/>
     </row>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G145" s="1"/>
     </row>
@@ -3213,16 +3213,16 @@
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
       <c r="C147" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G147" s="1"/>
     </row>
@@ -3230,11 +3230,11 @@
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G148" s="1"/>
     </row>
@@ -3242,7 +3242,7 @@
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1" t="s">
@@ -3254,11 +3254,11 @@
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G150" s="1"/>
     </row>
@@ -3282,7 +3282,7 @@
         <v>52</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G152" s="1"/>
     </row>
@@ -3310,7 +3310,7 @@
         <v>5</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G154" s="1"/>
     </row>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G155" s="1"/>
     </row>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G156" s="1"/>
     </row>
@@ -3342,11 +3342,11 @@
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E157" s="1"/>
       <c r="F157" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G157" s="1"/>
     </row>
@@ -3354,11 +3354,11 @@
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G158" s="1"/>
     </row>
@@ -3370,7 +3370,7 @@
       </c>
       <c r="E159" s="1"/>
       <c r="F159" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G159" s="1"/>
     </row>
@@ -3378,11 +3378,11 @@
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E160" s="1"/>
       <c r="F160" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G160" s="1"/>
     </row>
@@ -3416,7 +3416,7 @@
         <v>5</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G163" s="1"/>
     </row>
@@ -3442,7 +3442,7 @@
       </c>
       <c r="E165" s="1"/>
       <c r="F165" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G165" s="1"/>
     </row>
@@ -3450,11 +3450,11 @@
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E166" s="1"/>
       <c r="F166" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G166" s="1"/>
     </row>
@@ -3462,11 +3462,11 @@
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E167" s="1"/>
       <c r="F167" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G167" s="1"/>
     </row>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="E168" s="1"/>
       <c r="F168" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G168" s="1"/>
     </row>
@@ -3502,7 +3502,7 @@
         <v>52</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G170" s="1"/>
     </row>
@@ -3524,11 +3524,11 @@
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E172" s="1"/>
       <c r="F172" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G172" s="1"/>
     </row>
@@ -3536,11 +3536,11 @@
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E173" s="1"/>
       <c r="F173" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G173" s="1"/>
     </row>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="E174" s="1"/>
       <c r="F174" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G174" s="1"/>
     </row>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G175" s="1"/>
     </row>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="E176" s="1"/>
       <c r="F176" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G176" s="1"/>
     </row>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G177" s="1"/>
     </row>
@@ -3596,11 +3596,11 @@
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E178" s="1"/>
       <c r="F178" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G178" s="1"/>
     </row>
@@ -3624,7 +3624,7 @@
         <v>52</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G180" s="1"/>
     </row>
@@ -3652,7 +3652,7 @@
         <v>5</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G182" s="1"/>
     </row>
@@ -3660,11 +3660,11 @@
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E183" s="1"/>
       <c r="F183" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G183" s="1"/>
     </row>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G184" s="1"/>
     </row>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="E185" s="1"/>
       <c r="F185" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G185" s="1"/>
     </row>
@@ -3703,7 +3703,7 @@
     <row r="187" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B187" s="1"/>
       <c r="C187" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>2</v>
@@ -3712,7 +3712,7 @@
         <v>52</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G187" s="1"/>
     </row>
@@ -3720,7 +3720,7 @@
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>61</v>
@@ -3734,13 +3734,13 @@
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G189" s="1"/>
     </row>
@@ -3748,13 +3748,13 @@
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G190" s="1"/>
     </row>
@@ -3762,11 +3762,11 @@
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E191" s="1"/>
       <c r="F191" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G191" s="1"/>
     </row>
@@ -3774,11 +3774,11 @@
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E192" s="1"/>
       <c r="F192" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G192" s="1"/>
     </row>
@@ -3798,11 +3798,11 @@
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E194" s="1"/>
       <c r="F194" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G194" s="1"/>
     </row>
@@ -3817,7 +3817,7 @@
     <row r="196" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B196" s="1"/>
       <c r="C196" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D196" s="4" t="s">
         <v>2</v>
@@ -3826,7 +3826,7 @@
         <v>52</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G196" s="1"/>
     </row>
@@ -3834,7 +3834,7 @@
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>5</v>
@@ -3854,7 +3854,7 @@
         <v>5</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G198" s="1"/>
     </row>
@@ -3862,11 +3862,11 @@
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E199" s="1"/>
       <c r="F199" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G199" s="1"/>
     </row>
@@ -3874,11 +3874,11 @@
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E200" s="1"/>
       <c r="F200" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G200" s="1"/>
     </row>
@@ -3886,11 +3886,11 @@
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E201" s="1"/>
       <c r="F201" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G201" s="1"/>
     </row>
@@ -3905,7 +3905,7 @@
     <row r="203" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
       <c r="C203" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>2</v>
@@ -3914,7 +3914,7 @@
         <v>52</v>
       </c>
       <c r="F203" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G203" s="1"/>
     </row>
@@ -3922,7 +3922,7 @@
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>61</v>
@@ -3936,13 +3936,13 @@
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F205" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G205" s="1"/>
     </row>
@@ -3950,13 +3950,13 @@
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G206" s="1"/>
     </row>
@@ -3964,11 +3964,11 @@
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E207" s="1"/>
       <c r="F207" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G207" s="1"/>
     </row>
@@ -3976,11 +3976,11 @@
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E208" s="1"/>
       <c r="F208" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G208" s="1"/>
     </row>
@@ -3988,7 +3988,7 @@
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>61</v>
@@ -4023,7 +4023,7 @@
     <row r="212" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
       <c r="C212" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>2</v>
@@ -4032,7 +4032,7 @@
         <v>52</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G212" s="1"/>
     </row>
@@ -4040,7 +4040,7 @@
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E213" s="1"/>
       <c r="F213" s="1" t="s">
@@ -4058,7 +4058,7 @@
         <v>5</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G214" s="1"/>
     </row>
@@ -4066,11 +4066,11 @@
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E215" s="1"/>
       <c r="F215" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G215" s="1"/>
     </row>
@@ -4078,11 +4078,11 @@
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G216" s="1"/>
     </row>
@@ -4090,11 +4090,11 @@
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E217" s="1"/>
       <c r="F217" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G217" s="1"/>
     </row>
@@ -4102,11 +4102,11 @@
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E218" s="1"/>
       <c r="F218" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G218" s="1"/>
     </row>
@@ -4114,15 +4114,15 @@
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
       <c r="D219" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E219" s="1"/>
       <c r="F219" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G219" s="1"/>
       <c r="H219" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="220" spans="2:8" x14ac:dyDescent="0.25">
@@ -4145,7 +4145,7 @@
         <v>52</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G221" s="1"/>
     </row>
@@ -4173,7 +4173,7 @@
         <v>5</v>
       </c>
       <c r="F223" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G223" s="1"/>
     </row>
@@ -4181,11 +4181,11 @@
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G224" s="1"/>
     </row>
@@ -4197,7 +4197,7 @@
       </c>
       <c r="E225" s="1"/>
       <c r="F225" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G225" s="1"/>
     </row>
@@ -4205,11 +4205,11 @@
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E226" s="1"/>
       <c r="F226" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G226" s="1"/>
     </row>
@@ -4233,7 +4233,7 @@
         <v>52</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G228" s="1"/>
     </row>
@@ -4259,7 +4259,7 @@
         <v>5</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G230" s="1"/>
     </row>
@@ -4267,11 +4267,11 @@
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E231" s="1"/>
       <c r="F231" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G231" s="1"/>
     </row>
@@ -4279,11 +4279,11 @@
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
       <c r="D232" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E232" s="1"/>
       <c r="F232" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G232" s="1"/>
     </row>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="E234" s="1"/>
       <c r="F234" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G234" s="1"/>
     </row>
@@ -4331,7 +4331,7 @@
         <v>52</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G236" s="1"/>
     </row>
@@ -4359,7 +4359,7 @@
         <v>5</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G238" s="1"/>
     </row>
@@ -4367,11 +4367,11 @@
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1" t="s">
-        <v>127</v>
+        <v>300</v>
       </c>
       <c r="E239" s="1"/>
       <c r="F239" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G239" s="1"/>
     </row>
@@ -4379,11 +4379,11 @@
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
       <c r="D240" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G240" s="1"/>
     </row>
@@ -4391,11 +4391,11 @@
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
       <c r="D241" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E241" s="1"/>
       <c r="F241" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G241" s="1"/>
     </row>
@@ -4403,11 +4403,11 @@
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
       <c r="D242" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E242" s="1"/>
       <c r="F242" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G242" s="1"/>
     </row>
@@ -4415,11 +4415,11 @@
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
       <c r="D243" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E243" s="1"/>
       <c r="F243" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G243" s="1"/>
     </row>
@@ -4427,11 +4427,11 @@
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
       <c r="D244" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E244" s="1"/>
       <c r="F244" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G244" s="1"/>
     </row>
@@ -4449,13 +4449,13 @@
         <v>125</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>133</v>
+        <v>2</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F246" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G246" s="1"/>
     </row>
@@ -4463,13 +4463,11 @@
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E247" s="1"/>
       <c r="F247" s="1" t="s">
-        <v>216</v>
+        <v>62</v>
       </c>
       <c r="G247" s="1"/>
     </row>
@@ -4477,11 +4475,13 @@
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E248" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F248" s="1" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="G248" s="1"/>
     </row>
@@ -4489,11 +4489,11 @@
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
       <c r="D249" s="1" t="s">
-        <v>106</v>
+        <v>301</v>
       </c>
       <c r="E249" s="1"/>
       <c r="F249" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G249" s="1"/>
     </row>
@@ -4501,11 +4501,11 @@
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="E250" s="1"/>
       <c r="F250" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G250" s="1"/>
     </row>
@@ -4513,11 +4513,11 @@
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E251" s="1"/>
       <c r="F251" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G251" s="1"/>
     </row>
@@ -4525,11 +4525,11 @@
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
       <c r="D252" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E252" s="1"/>
       <c r="F252" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G252" s="1"/>
     </row>
@@ -4537,49 +4537,47 @@
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
       <c r="D253" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E253" s="1"/>
       <c r="F253" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G253" s="1"/>
     </row>
     <row r="254" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
-      <c r="D254" s="1"/>
+      <c r="D254" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="E254" s="1"/>
-      <c r="F254" s="1"/>
+      <c r="F254" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="G254" s="1"/>
     </row>
     <row r="255" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B255" s="1"/>
-      <c r="C255" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D255" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F255" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C255" s="1"/>
+      <c r="D255" s="1"/>
+      <c r="E255" s="1"/>
+      <c r="F255" s="1"/>
       <c r="G255" s="1"/>
     </row>
     <row r="256" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B256" s="1"/>
-      <c r="C256" s="1"/>
+      <c r="C256" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="D256" s="1" t="s">
-        <v>116</v>
+        <v>2</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F256" s="1" t="s">
-        <v>62</v>
+        <v>214</v>
       </c>
       <c r="G256" s="1"/>
     </row>
@@ -4587,13 +4585,13 @@
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
       <c r="D257" s="1" t="s">
-        <v>222</v>
+        <v>116</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="F257" s="1" t="s">
-        <v>212</v>
+        <v>62</v>
       </c>
       <c r="G257" s="1"/>
     </row>
@@ -4601,11 +4599,13 @@
       <c r="B258" s="1"/>
       <c r="C258" s="1"/>
       <c r="D258" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E258" s="1"/>
+        <v>220</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F258" s="1" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="G258" s="1"/>
     </row>
@@ -4613,49 +4613,47 @@
       <c r="B259" s="1"/>
       <c r="C259" s="1"/>
       <c r="D259" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E259" s="1"/>
       <c r="F259" s="1" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="G259" s="1"/>
     </row>
     <row r="260" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
-      <c r="D260" s="1"/>
+      <c r="D260" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="E260" s="1"/>
-      <c r="F260" s="1"/>
+      <c r="F260" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="G260" s="1"/>
     </row>
     <row r="261" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B261" s="1"/>
-      <c r="C261" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D261" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F261" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C261" s="1"/>
+      <c r="D261" s="1"/>
+      <c r="E261" s="1"/>
+      <c r="F261" s="1"/>
       <c r="G261" s="1"/>
     </row>
     <row r="262" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
+      <c r="C262" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="D262" s="1" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="E262" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G262" s="1"/>
     </row>
@@ -4663,9 +4661,11 @@
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
       <c r="D263" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E263" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F263" s="1" t="s">
         <v>214</v>
       </c>
@@ -4675,11 +4675,11 @@
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
       <c r="D264" s="1" t="s">
-        <v>183</v>
+        <v>77</v>
       </c>
       <c r="E264" s="1"/>
       <c r="F264" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G264" s="1"/>
     </row>
@@ -4687,11 +4687,11 @@
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
       <c r="D265" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E265" s="1"/>
       <c r="F265" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G265" s="1"/>
     </row>
@@ -4699,11 +4699,11 @@
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
       <c r="D266" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E266" s="1"/>
       <c r="F266" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G266" s="1"/>
     </row>
@@ -4711,11 +4711,11 @@
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
       <c r="D267" s="1" t="s">
-        <v>106</v>
+        <v>183</v>
       </c>
       <c r="E267" s="1"/>
       <c r="F267" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G267" s="1"/>
     </row>
@@ -4723,11 +4723,11 @@
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
       <c r="D268" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="E268" s="1"/>
       <c r="F268" s="1" t="s">
-        <v>63</v>
+        <v>211</v>
       </c>
       <c r="G268" s="1"/>
     </row>
@@ -4735,49 +4735,47 @@
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
       <c r="D269" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E269" s="1"/>
       <c r="F269" s="1" t="s">
-        <v>214</v>
+        <v>63</v>
       </c>
       <c r="G269" s="1"/>
     </row>
     <row r="270" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
-      <c r="D270" s="1"/>
+      <c r="D270" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="E270" s="1"/>
-      <c r="F270" s="1"/>
+      <c r="F270" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="G270" s="1"/>
     </row>
     <row r="271" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B271" s="1"/>
-      <c r="C271" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D271" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E271" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F271" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C271" s="1"/>
+      <c r="D271" s="1"/>
+      <c r="E271" s="1"/>
+      <c r="F271" s="1"/>
       <c r="G271" s="1"/>
     </row>
     <row r="272" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B272" s="1"/>
-      <c r="C272" s="1"/>
+      <c r="C272" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="D272" s="1" t="s">
-        <v>222</v>
+        <v>2</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F272" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G272" s="1"/>
     </row>
@@ -4785,13 +4783,13 @@
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
       <c r="D273" s="1" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="F273" s="1" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="G273" s="1"/>
     </row>
@@ -4799,49 +4797,49 @@
       <c r="B274" s="1"/>
       <c r="C274" s="1"/>
       <c r="D274" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E274" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F274" s="1" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="G274" s="1"/>
     </row>
     <row r="275" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
-      <c r="D275" s="1"/>
+      <c r="D275" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="E275" s="1"/>
-      <c r="F275" s="1"/>
+      <c r="F275" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="G275" s="1"/>
     </row>
     <row r="276" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B276" s="1"/>
-      <c r="C276" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D276" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E276" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F276" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C276" s="1"/>
+      <c r="D276" s="1"/>
+      <c r="E276" s="1"/>
+      <c r="F276" s="1"/>
       <c r="G276" s="1"/>
     </row>
     <row r="277" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B277" s="1"/>
-      <c r="C277" s="1"/>
+      <c r="C277" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="D277" s="1" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="E277" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F277" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G277" s="1"/>
     </row>
@@ -4849,9 +4847,11 @@
       <c r="B278" s="1"/>
       <c r="C278" s="1"/>
       <c r="D278" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E278" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F278" s="1" t="s">
         <v>214</v>
       </c>
@@ -4861,11 +4861,11 @@
       <c r="B279" s="1"/>
       <c r="C279" s="1"/>
       <c r="D279" s="1" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="E279" s="1"/>
       <c r="F279" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G279" s="1"/>
     </row>
@@ -4873,11 +4873,11 @@
       <c r="B280" s="1"/>
       <c r="C280" s="1"/>
       <c r="D280" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="E280" s="1"/>
       <c r="F280" s="1" t="s">
-        <v>63</v>
+        <v>211</v>
       </c>
       <c r="G280" s="1"/>
     </row>
@@ -4885,20 +4885,24 @@
       <c r="B281" s="1"/>
       <c r="C281" s="1"/>
       <c r="D281" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E281" s="1"/>
       <c r="F281" s="1" t="s">
-        <v>214</v>
+        <v>63</v>
       </c>
       <c r="G281" s="1"/>
     </row>
     <row r="282" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B282" s="1"/>
       <c r="C282" s="1"/>
-      <c r="D282" s="1"/>
+      <c r="D282" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="E282" s="1"/>
-      <c r="F282" s="1"/>
+      <c r="F282" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="G282" s="1"/>
     </row>
     <row r="283" spans="2:8" x14ac:dyDescent="0.25">
@@ -4910,87 +4914,81 @@
       <c r="G283" s="1"/>
     </row>
     <row r="284" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B284" s="1" t="s">
+      <c r="B284" s="1"/>
+      <c r="C284" s="1"/>
+      <c r="D284" s="1"/>
+      <c r="E284" s="1"/>
+      <c r="F284" s="1"/>
+      <c r="G284" s="1"/>
+    </row>
+    <row r="285" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B285" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C284" s="1" t="s">
+      <c r="C285" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D284" s="1" t="s">
+      <c r="D285" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E284" s="1" t="s">
+      <c r="E285" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F284" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G284" s="1"/>
-    </row>
-    <row r="285" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B285" s="1"/>
-      <c r="C285" s="1"/>
-      <c r="D285" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E285" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F285" s="1" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="G285" s="1"/>
-      <c r="H285" t="s">
-        <v>227</v>
-      </c>
     </row>
     <row r="286" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B286" s="1"/>
       <c r="C286" s="1"/>
       <c r="D286" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E286" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="F286" s="1" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="G286" s="1"/>
+      <c r="H286" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="287" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
-      <c r="D287" s="1"/>
+      <c r="D287" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="E287" s="1"/>
-      <c r="F287" s="1"/>
+      <c r="F287" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="G287" s="1"/>
     </row>
     <row r="288" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B288" s="1"/>
-      <c r="C288" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D288" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F288" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C288" s="1"/>
+      <c r="D288" s="1"/>
+      <c r="E288" s="1"/>
+      <c r="F288" s="1"/>
       <c r="G288" s="1"/>
     </row>
     <row r="289" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B289" s="1"/>
-      <c r="C289" s="1"/>
+      <c r="C289" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D289" s="1" t="s">
-        <v>223</v>
+        <v>275</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F289" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G289" s="1"/>
     </row>
@@ -4998,11 +4996,13 @@
       <c r="B290" s="1"/>
       <c r="C290" s="1"/>
       <c r="D290" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E290" s="1"/>
+        <v>221</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F290" s="1" t="s">
-        <v>152</v>
+        <v>214</v>
       </c>
       <c r="G290" s="1"/>
     </row>
@@ -5010,11 +5010,11 @@
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
       <c r="D291" s="1" t="s">
-        <v>144</v>
+        <v>288</v>
       </c>
       <c r="E291" s="1"/>
       <c r="F291" s="1" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="G291" s="1"/>
     </row>
@@ -5022,49 +5022,47 @@
       <c r="B292" s="1"/>
       <c r="C292" s="1"/>
       <c r="D292" s="1" t="s">
-        <v>291</v>
+        <v>142</v>
       </c>
       <c r="E292" s="1"/>
       <c r="F292" s="1" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="G292" s="1"/>
     </row>
     <row r="293" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B293" s="1"/>
       <c r="C293" s="1"/>
-      <c r="D293" s="1"/>
+      <c r="D293" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="E293" s="1"/>
-      <c r="F293" s="1"/>
+      <c r="F293" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="G293" s="1"/>
     </row>
     <row r="294" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B294" s="1"/>
-      <c r="C294" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D294" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E294" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F294" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C294" s="1"/>
+      <c r="D294" s="1"/>
+      <c r="E294" s="1"/>
+      <c r="F294" s="1"/>
       <c r="G294" s="1"/>
     </row>
     <row r="295" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B295" s="1"/>
-      <c r="C295" s="1"/>
+      <c r="C295" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="D295" s="1" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F295" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G295" s="1"/>
     </row>
@@ -5072,11 +5070,13 @@
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
       <c r="D296" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="E296" s="1"/>
+        <v>222</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F296" s="1" t="s">
-        <v>152</v>
+        <v>214</v>
       </c>
       <c r="G296" s="1"/>
     </row>
@@ -5084,11 +5084,11 @@
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
       <c r="D297" s="1" t="s">
-        <v>145</v>
+        <v>286</v>
       </c>
       <c r="E297" s="1"/>
       <c r="F297" s="1" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="G297" s="1"/>
     </row>
@@ -5096,49 +5096,47 @@
       <c r="B298" s="1"/>
       <c r="C298" s="1"/>
       <c r="D298" s="1" t="s">
-        <v>289</v>
+        <v>143</v>
       </c>
       <c r="E298" s="1"/>
       <c r="F298" s="1" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="G298" s="1"/>
     </row>
     <row r="299" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B299" s="1"/>
       <c r="C299" s="1"/>
-      <c r="D299" s="1"/>
+      <c r="D299" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="E299" s="1"/>
-      <c r="F299" s="1"/>
+      <c r="F299" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="G299" s="1"/>
     </row>
     <row r="300" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B300" s="1"/>
-      <c r="C300" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D300" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F300" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C300" s="1"/>
+      <c r="D300" s="1"/>
+      <c r="E300" s="1"/>
+      <c r="F300" s="1"/>
       <c r="G300" s="1"/>
     </row>
     <row r="301" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B301" s="1"/>
-      <c r="C301" s="1"/>
+      <c r="C301" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="D301" s="1" t="s">
-        <v>91</v>
+        <v>279</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F301" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G301" s="1"/>
     </row>
@@ -5146,11 +5144,13 @@
       <c r="B302" s="1"/>
       <c r="C302" s="1"/>
       <c r="D302" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E302" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F302" s="1" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="G302" s="1"/>
     </row>
@@ -5158,11 +5158,11 @@
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
       <c r="D303" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E303" s="1"/>
       <c r="F303" s="1" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="G303" s="1"/>
     </row>
@@ -5170,11 +5170,11 @@
       <c r="B304" s="1"/>
       <c r="C304" s="1"/>
       <c r="D304" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E304" s="1"/>
       <c r="F304" s="1" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="G304" s="1"/>
     </row>
@@ -5182,49 +5182,47 @@
       <c r="B305" s="1"/>
       <c r="C305" s="1"/>
       <c r="D305" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E305" s="1"/>
       <c r="F305" s="1" t="s">
-        <v>63</v>
+        <v>188</v>
       </c>
       <c r="G305" s="1"/>
     </row>
     <row r="306" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B306" s="1"/>
       <c r="C306" s="1"/>
-      <c r="D306" s="1"/>
+      <c r="D306" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="E306" s="1"/>
-      <c r="F306" s="1"/>
+      <c r="F306" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G306" s="1"/>
     </row>
     <row r="307" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B307" s="1"/>
-      <c r="C307" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D307" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E307" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F307" s="1" t="s">
-        <v>190</v>
-      </c>
+      <c r="C307" s="1"/>
+      <c r="D307" s="1"/>
+      <c r="E307" s="1"/>
+      <c r="F307" s="1"/>
       <c r="G307" s="1"/>
     </row>
     <row r="308" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B308" s="1"/>
-      <c r="C308" s="1"/>
+      <c r="C308" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="D308" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="E308" t="s">
-        <v>280</v>
+        <v>139</v>
+      </c>
+      <c r="E308" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="F308" s="1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="G308" s="1"/>
     </row>
@@ -5232,49 +5230,49 @@
       <c r="B309" s="1"/>
       <c r="C309" s="1"/>
       <c r="D309" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E309" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="E309" t="s">
+        <v>278</v>
+      </c>
       <c r="F309" s="1" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="G309" s="1"/>
     </row>
     <row r="310" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
-      <c r="D310" s="1"/>
+      <c r="D310" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="E310" s="1"/>
-      <c r="F310" s="1"/>
+      <c r="F310" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="G310" s="1"/>
     </row>
     <row r="311" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B311" s="1"/>
-      <c r="C311" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D311" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E311" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F311" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C311" s="1"/>
+      <c r="D311" s="1"/>
+      <c r="E311" s="1"/>
+      <c r="F311" s="1"/>
       <c r="G311" s="1"/>
     </row>
     <row r="312" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B312" s="1"/>
-      <c r="C312" s="1"/>
+      <c r="C312" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="D312" s="1" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F312" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G312" s="1"/>
     </row>
@@ -5282,11 +5280,13 @@
       <c r="B313" s="1"/>
       <c r="C313" s="1"/>
       <c r="D313" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E313" s="1"/>
+        <v>275</v>
+      </c>
+      <c r="E313" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F313" s="1" t="s">
-        <v>152</v>
+        <v>214</v>
       </c>
       <c r="G313" s="1"/>
     </row>
@@ -5294,11 +5294,11 @@
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
       <c r="D314" s="1" t="s">
-        <v>141</v>
+        <v>292</v>
       </c>
       <c r="E314" s="1"/>
       <c r="F314" s="1" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="G314" s="1"/>
     </row>
@@ -5306,11 +5306,11 @@
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
       <c r="D315" s="1" t="s">
-        <v>295</v>
+        <v>139</v>
       </c>
       <c r="E315" s="1"/>
       <c r="F315" s="1" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="G315" s="1"/>
     </row>
@@ -5318,11 +5318,11 @@
       <c r="B316" s="1"/>
       <c r="C316" s="1"/>
       <c r="D316" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E316" s="1"/>
       <c r="F316" s="1" t="s">
-        <v>63</v>
+        <v>212</v>
       </c>
       <c r="G316" s="1"/>
     </row>
@@ -5330,49 +5330,47 @@
       <c r="B317" s="1"/>
       <c r="C317" s="1"/>
       <c r="D317" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E317" s="1"/>
       <c r="F317" s="1" t="s">
-        <v>190</v>
+        <v>63</v>
       </c>
       <c r="G317" s="1"/>
     </row>
     <row r="318" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
-      <c r="D318" s="1"/>
+      <c r="D318" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="E318" s="1"/>
-      <c r="F318" s="1"/>
+      <c r="F318" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="G318" s="1"/>
     </row>
     <row r="319" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B319" s="1"/>
-      <c r="C319" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D319" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E319" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F319" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="C319" s="1"/>
+      <c r="D319" s="1"/>
+      <c r="E319" s="1"/>
+      <c r="F319" s="1"/>
       <c r="G319" s="1"/>
     </row>
     <row r="320" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B320" s="1"/>
-      <c r="C320" s="1"/>
+      <c r="C320" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="D320" s="1" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="E320" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="F320" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G320" s="1"/>
     </row>
@@ -5380,11 +5378,13 @@
       <c r="B321" s="1"/>
       <c r="C321" s="1"/>
       <c r="D321" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E321" s="1"/>
+        <v>276</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="F321" s="1" t="s">
-        <v>152</v>
+        <v>214</v>
       </c>
       <c r="G321" s="1"/>
     </row>
@@ -5392,11 +5392,11 @@
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
       <c r="D322" s="1" t="s">
-        <v>141</v>
+        <v>292</v>
       </c>
       <c r="E322" s="1"/>
       <c r="F322" s="1" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="G322" s="1"/>
     </row>
@@ -5404,11 +5404,11 @@
       <c r="B323" s="1"/>
       <c r="C323" s="1"/>
       <c r="D323" s="1" t="s">
-        <v>295</v>
+        <v>139</v>
       </c>
       <c r="E323" s="1"/>
       <c r="F323" s="1" t="s">
-        <v>214</v>
+        <v>188</v>
       </c>
       <c r="G323" s="1"/>
     </row>
@@ -5416,11 +5416,11 @@
       <c r="B324" s="1"/>
       <c r="C324" s="1"/>
       <c r="D324" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E324" s="1"/>
       <c r="F324" s="1" t="s">
-        <v>63</v>
+        <v>212</v>
       </c>
       <c r="G324" s="1"/>
     </row>
@@ -5428,17 +5428,29 @@
       <c r="B325" s="1"/>
       <c r="C325" s="1"/>
       <c r="D325" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E325" s="1"/>
       <c r="F325" s="1" t="s">
-        <v>190</v>
+        <v>63</v>
       </c>
       <c r="G325" s="1"/>
     </row>
-    <row r="327" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B327" t="s">
-        <v>146</v>
+    <row r="326" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B326" s="1"/>
+      <c r="C326" s="1"/>
+      <c r="D326" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E326" s="1"/>
+      <c r="F326" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G326" s="1"/>
+    </row>
+    <row r="328" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B328" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>